<commit_message>
Update Excel and TXT files from Streamlit app
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -516,7 +516,7 @@
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -525,7 +525,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45574</v>
+        <v>45572</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45575</v>
+        <v>45572</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -546,12 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>313</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -560,7 +560,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -569,10 +569,10 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45593</v>
+        <v>45581</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45593</v>
+        <v>45582</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -581,12 +581,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -595,7 +595,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -604,10 +604,10 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45560</v>
+        <v>45579</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45561</v>
+        <v>45579</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -616,12 +616,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>313</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45546</v>
+        <v>45576</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45547</v>
+        <v>45576</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -651,12 +651,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>field work near flagstaff</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -665,7 +665,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Olsen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45421</v>
+        <v>45401</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45421</v>
+        <v>45402</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -700,7 +700,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -709,10 +709,10 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45567</v>
+        <v>45600</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45568</v>
+        <v>45600</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -721,12 +721,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>313</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -735,7 +735,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Derek Uhey</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45539</v>
+        <v>45432</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45540</v>
+        <v>45538</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -756,12 +756,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>California all summer</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -770,7 +770,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -779,10 +779,10 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45553</v>
+        <v>45558</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45554</v>
+        <v>45558</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -791,12 +791,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>313</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -805,7 +805,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45551</v>
+        <v>45588</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>45551</v>
+        <v>45589</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -840,7 +840,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -849,10 +849,10 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>45558</v>
+        <v>45553</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>45558</v>
+        <v>45554</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -861,12 +861,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -875,7 +875,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Derek Uhey</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -884,10 +884,10 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45432</v>
+        <v>45539</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>45538</v>
+        <v>45540</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -896,12 +896,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>California all summer</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -910,7 +910,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -919,10 +919,10 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45600</v>
+        <v>45567</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>45600</v>
+        <v>45568</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -931,12 +931,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -945,7 +945,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Olsen</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -954,10 +954,10 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45401</v>
+        <v>45421</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>45402</v>
+        <v>45421</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -989,10 +989,10 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45576</v>
+        <v>45546</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>45576</v>
+        <v>45547</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1001,12 +1001,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>field work near flagstaff</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1024,10 +1024,10 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45579</v>
+        <v>45560</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>45579</v>
+        <v>45561</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1059,10 +1059,10 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45588</v>
+        <v>45593</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>45589</v>
+        <v>45593</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>313</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45581</v>
+        <v>45574</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>45582</v>
+        <v>45575</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1129,10 +1129,10 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45572</v>
+        <v>45551</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>45572</v>
+        <v>45551</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1141,12 +1141,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>315</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Darren Olney</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1164,10 +1164,10 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45581</v>
+        <v>45660</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>45585</v>
+        <v>45670</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>POC: deo73@nau.edu</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
@@ -1199,10 +1199,10 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45588</v>
+        <v>45594</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>45588</v>
+        <v>45595</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1234,10 +1234,10 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45554</v>
+        <v>45637</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>45556</v>
+        <v>45642</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t>Andrew Henning</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1269,10 +1269,10 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45600</v>
+        <v>45605</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>45600</v>
+        <v>45610</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1281,12 +1281,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>AZWI</t>
+          <t xml:space="preserve">Down to the valley for a conference </t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
@@ -1295,7 +1295,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>keven</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1304,10 +1304,10 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45627</v>
+        <v>45554</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>45635</v>
+        <v>45556</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1316,12 +1316,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t xml:space="preserve">We will be traveling to Organ Pipe, Casa Grande, and Tonto National monuments to conduct fieldwork for my PhD project. The vehicle will be used to transport people and materials for that work. We will have no more than 4 people in the vehicle. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Andrew Henning</t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1339,10 +1339,10 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45605</v>
+        <v>45600</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>45610</v>
+        <v>45600</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1351,12 +1351,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Down to the valley for a conference </t>
+          <t>AZWI</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1374,10 +1374,10 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45637</v>
+        <v>45588</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>45642</v>
+        <v>45588</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>AZWI</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t>Darren Olney</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1409,10 +1409,10 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45594</v>
+        <v>45581</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>45595</v>
+        <v>45585</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1421,12 +1421,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>AZWI</t>
+          <t>POC: deo73@nau.edu</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>keven</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1444,10 +1444,10 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45660</v>
+        <v>45627</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>45670</v>
+        <v>45635</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1456,12 +1456,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">We will be traveling to Organ Pipe, Casa Grande, and Tonto National monuments to conduct fieldwork for my PhD project. The vehicle will be used to transport people and materials for that work. We will have no more than 4 people in the vehicle. </t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1479,10 +1479,10 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45608</v>
+        <v>45568</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>45608</v>
+        <v>45568</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1491,12 +1491,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Payson for a workshop</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1514,10 +1514,10 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45611</v>
+        <v>45627</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>45611</v>
+        <v>45748</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1526,12 +1526,16 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>school to teach about fire for a day</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
+          <t xml:space="preserve">This vehicle will be used to travel to the Sierra Ancha Experimental Forest throughout the winter months to collect snow, snow melt, and stream samples for water stable isotopes and chemistry. </t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Emory Ellis</t>
+        </is>
+      </c>
       <c r="I31" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32">
@@ -1540,7 +1544,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>jaime</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1549,10 +1553,10 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45603</v>
+        <v>45581</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>45604</v>
+        <v>45587</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1561,12 +1565,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>SRP field work</t>
+          <t>SAEF</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
@@ -1575,7 +1579,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Megan Rangel-Lynch</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1584,10 +1588,10 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45597</v>
+        <v>45589</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>45598</v>
+        <v>45593</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1601,7 +1605,7 @@
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -1610,7 +1614,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1619,10 +1623,10 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45548</v>
+        <v>45562</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>45554</v>
+        <v>45564</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1636,7 +1640,7 @@
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35">
@@ -1645,7 +1649,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1654,10 +1658,10 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45562</v>
+        <v>45611</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>45564</v>
+        <v>45611</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1666,12 +1670,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>school to teach about fire for a day</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36">
@@ -1680,7 +1684,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Megan Rangel-Lynch</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1689,10 +1693,10 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45568</v>
+        <v>45597</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>45568</v>
+        <v>45598</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1706,7 +1710,7 @@
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37">
@@ -1715,7 +1719,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>jaime</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1724,10 +1728,10 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>45589</v>
+        <v>45603</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>45593</v>
+        <v>45604</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1736,12 +1740,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SRP field work</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38">
@@ -1750,7 +1754,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1759,10 +1763,10 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>45581</v>
+        <v>45548</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>45587</v>
+        <v>45554</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1771,12 +1775,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>SAEF</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39">
@@ -1785,7 +1789,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1794,10 +1798,10 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>45627</v>
+        <v>45608</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>45748</v>
+        <v>45608</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1806,16 +1810,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t xml:space="preserve">This vehicle will be used to travel to the Sierra Ancha Experimental Forest throughout the winter months to collect snow, snow melt, and stream samples for water stable isotopes and chemistry. </t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Emory Ellis</t>
-        </is>
-      </c>
+          <t>Payson for a workshop</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40">
@@ -1833,10 +1833,10 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>45552</v>
+        <v>45545</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>45554</v>
+        <v>45547</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41">
@@ -1868,10 +1868,10 @@
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>45566</v>
+        <v>45580</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>45568</v>
+        <v>45582</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42">
@@ -1899,14 +1899,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>45586</v>
+        <v>45573</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>45610</v>
+        <v>45575</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1915,12 +1915,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>FOR220 tuesday-thursday</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43">
@@ -1938,10 +1938,10 @@
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>45573</v>
+        <v>45559</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>45575</v>
+        <v>45561</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44">
@@ -1973,10 +1973,10 @@
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>45559</v>
+        <v>45566</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>45561</v>
+        <v>45568</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="n">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45">
@@ -2008,10 +2008,10 @@
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>45580</v>
+        <v>45552</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>45582</v>
+        <v>45554</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46">
@@ -2039,14 +2039,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>45545</v>
+        <v>45586</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>45547</v>
+        <v>45610</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2055,12 +2055,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>FOR220 tuesday-thursday</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2078,10 +2078,10 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>45642</v>
+        <v>45667</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>45643</v>
+        <v>45667</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2090,16 +2090,16 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Andrei will be joining us in the field (as long as he is feeling better) in Superior, AZ. The fieldwork is being conducted as part of my PhD research.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Keven Griffen</t>
+          <t>Jacob Shelly</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2117,10 +2117,10 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>45595</v>
+        <v>45667</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>45595</v>
+        <v>45667</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2132,9 +2132,13 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Jacob Shelly</t>
+        </is>
+      </c>
       <c r="I48" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49">
@@ -2143,7 +2147,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2152,10 +2156,10 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>45588</v>
+        <v>45667</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>45588</v>
+        <v>45667</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2167,7 +2171,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Jacob Shelly</t>
+        </is>
+      </c>
       <c r="I49" t="n">
         <v>57</v>
       </c>
@@ -2178,7 +2186,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2187,10 +2195,10 @@
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>45565</v>
+        <v>45667</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>45567</v>
+        <v>45667</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2202,9 +2210,13 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Jacob Shelly</t>
+        </is>
+      </c>
       <c r="I50" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51">
@@ -2213,7 +2225,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2222,10 +2234,10 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>45576</v>
+        <v>45667</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>45576</v>
+        <v>45667</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2237,9 +2249,13 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Jacob Shelly</t>
+        </is>
+      </c>
       <c r="I51" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52">
@@ -2248,7 +2264,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2257,10 +2273,10 @@
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>45581</v>
+        <v>45667</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>45583</v>
+        <v>45667</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2269,12 +2285,16 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>for keven, srp data collection</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Jacob Shelly</t>
+        </is>
+      </c>
       <c r="I52" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53">
@@ -2283,7 +2303,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2292,10 +2312,10 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>45667</v>
+        <v>45595</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>45667</v>
+        <v>45595</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2307,13 +2327,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Jacob Shelly</t>
-        </is>
-      </c>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="n">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54">
@@ -2322,7 +2338,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2331,10 +2347,10 @@
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>45667</v>
+        <v>45581</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>45667</v>
+        <v>45583</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2343,16 +2359,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Jacob Shelly</t>
-        </is>
-      </c>
+          <t>for keven, srp data collection</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
       <c r="I54" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55">
@@ -2361,7 +2373,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2370,10 +2382,10 @@
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>45667</v>
+        <v>45576</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>45667</v>
+        <v>45576</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2385,13 +2397,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Jacob Shelly</t>
-        </is>
-      </c>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="n">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56">
@@ -2400,7 +2408,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2409,10 +2417,10 @@
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>45667</v>
+        <v>45565</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>45667</v>
+        <v>45567</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2424,13 +2432,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Jacob Shelly</t>
-        </is>
-      </c>
+      <c r="H56" t="inlineStr"/>
       <c r="I56" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57">
@@ -2439,7 +2443,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2448,10 +2452,10 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>45667</v>
+        <v>45588</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>45667</v>
+        <v>45588</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2463,13 +2467,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Jacob Shelly</t>
-        </is>
-      </c>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>45667</v>
+        <v>45642</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>45667</v>
+        <v>45643</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2499,16 +2499,16 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Andrei will be joining us in the field (as long as he is feeling better) in Superior, AZ. The fieldwork is being conducted as part of my PhD research.</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Jacob Shelly</t>
+          <t>Keven Griffen</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59">
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>3</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60">
@@ -2586,7 +2586,7 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61">
@@ -2625,7 +2625,7 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62">
@@ -2664,7 +2664,7 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63">
@@ -2703,7 +2703,7 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65">
@@ -2781,7 +2781,7 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66">
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="I66" t="n">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68">
@@ -2894,7 +2894,7 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69">
@@ -2964,7 +2964,7 @@
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71">
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="n">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3056,10 +3056,10 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>45525</v>
+        <v>45555</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>45525</v>
+        <v>45555</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -3068,12 +3068,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data from some installed sensors, as part of our research project. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Carol Chambers</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3091,10 +3091,10 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>45509</v>
+        <v>45453</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>45514</v>
+        <v>45477</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -3103,16 +3103,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jumping mouse stuff. To and From the White Mountains. </t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Matthew Voorhees</t>
-        </is>
-      </c>
+          <t>Sierra Ancha and Verde Valley, dates not needed are TBD</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr"/>
       <c r="I74" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75">
@@ -3121,19 +3117,19 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>45517</v>
+        <v>45432</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>45518</v>
+        <v>45434</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -3142,16 +3138,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>We need a 4WD vehicle with room for 4 passengers, AC, and room for large equipment to drive to a remote field site for installing sensors. The field site is the SRP-funded Dude Fire project, which is located on the Tonto NF near Payson. Salli will drive and take 2-3 students. This is an overnight trip - we'll depart around 8am on 8/13 and return around 5pm on 8/14.</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Salli Dymond</t>
-        </is>
-      </c>
+          <t>southern AZ/NM</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr"/>
       <c r="I75" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76">
@@ -3169,10 +3161,10 @@
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>45439</v>
+        <v>45478</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>45445</v>
+        <v>45506</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -3186,7 +3178,7 @@
       </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77">
@@ -3195,19 +3187,19 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>45432</v>
+        <v>45517</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>45434</v>
+        <v>45518</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -3216,12 +3208,16 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr"/>
+          <t>We need a 4WD vehicle with room for 4 passengers, AC, and room for large equipment to drive to a remote field site for installing sensors. The field site is the SRP-funded Dude Fire project, which is located on the Tonto NF near Payson. Salli will drive and take 2-3 students. This is an overnight trip - we'll depart around 8am on 8/13 and return around 5pm on 8/14.</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Salli Dymond</t>
+        </is>
+      </c>
       <c r="I77" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78">
@@ -3230,7 +3226,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Carol Chambers</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3239,10 +3235,10 @@
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>45453</v>
+        <v>45509</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>45477</v>
+        <v>45514</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -3251,12 +3247,16 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Sierra Ancha and Verde Valley, dates not needed are TBD</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr"/>
+          <t xml:space="preserve">Jumping mouse stuff. To and From the White Mountains. </t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Matthew Voorhees</t>
+        </is>
+      </c>
       <c r="I78" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3274,10 +3274,10 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>45478</v>
+        <v>45525</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>45506</v>
+        <v>45525</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -3286,12 +3286,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data from some installed sensors, as part of our research project. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80">
@@ -3309,10 +3309,10 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>45555</v>
+        <v>45439</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>45555</v>
+        <v>45445</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>45421</v>
+        <v>45432</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>45421</v>
+        <v>45433</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82">
@@ -3379,10 +3379,10 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>45444</v>
+        <v>45627</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>45536</v>
+        <v>45688</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -3391,12 +3391,16 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>New Mexico, dates not needed are TBD</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Keven Griffen</t>
+        </is>
+      </c>
       <c r="I82" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83">
@@ -3405,7 +3409,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3414,10 +3418,10 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>45639</v>
+        <v>45541</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>45647</v>
+        <v>45571</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -3426,12 +3430,12 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84">
@@ -3440,7 +3444,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Olsen</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3449,10 +3453,10 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>45422</v>
+        <v>45401</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>45427</v>
+        <v>45402</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -3466,7 +3470,7 @@
       </c>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85">
@@ -3484,10 +3488,10 @@
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>45617</v>
+        <v>45602</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>45623</v>
+        <v>45608</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -3501,7 +3505,7 @@
       </c>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86">
@@ -3536,7 +3540,7 @@
       </c>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87">
@@ -3545,7 +3549,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3554,10 +3558,10 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>45602</v>
+        <v>45422</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>45608</v>
+        <v>45427</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -3571,7 +3575,7 @@
       </c>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88">
@@ -3580,7 +3584,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Olsen</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3589,10 +3593,10 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>45401</v>
+        <v>45639</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>45402</v>
+        <v>45647</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3606,7 +3610,7 @@
       </c>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89">
@@ -3615,7 +3619,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3624,10 +3628,10 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>45541</v>
+        <v>45444</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>45571</v>
+        <v>45536</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -3636,12 +3640,12 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
+          <t>New Mexico, dates not needed are TBD</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90">
@@ -3650,7 +3654,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3659,10 +3663,10 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>45627</v>
+        <v>45421</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>45688</v>
+        <v>45421</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -3674,13 +3678,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Keven Griffen</t>
-        </is>
-      </c>
+      <c r="H90" t="inlineStr"/>
       <c r="I90" t="n">
-        <v>10</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3698,10 +3698,10 @@
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>45432</v>
+        <v>45617</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>45433</v>
+        <v>45623</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3733,10 +3733,10 @@
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>45403</v>
+        <v>45401</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>45423</v>
+        <v>45402</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3768,10 +3768,10 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>45425</v>
+        <v>45594</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>45474</v>
+        <v>45594</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -3780,12 +3780,12 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Tonto/ dates not needed TBD</t>
+          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3803,10 +3803,10 @@
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>45475</v>
+        <v>45597</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>45565</v>
+        <v>45613</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -3815,12 +3815,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Tonto</t>
+          <t>Day use in town for the extent of stay</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95">
@@ -3829,19 +3829,19 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Peter Fule</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>45581</v>
+        <v>45667</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>45587</v>
+        <v>45787</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -3850,12 +3850,16 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>SAEF</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
       <c r="I95" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96">
@@ -3864,19 +3868,19 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Peter Fule</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>45667</v>
+        <v>45425</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>45787</v>
+        <v>45474</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3885,16 +3889,12 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Peter Fule</t>
-        </is>
-      </c>
+          <t>Tonto/ dates not needed TBD</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr"/>
       <c r="I96" t="n">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3912,10 +3912,10 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>45401</v>
+        <v>45475</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>45402</v>
+        <v>45565</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -3924,12 +3924,12 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Tonto</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3947,10 +3947,10 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>45597</v>
+        <v>45581</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>45613</v>
+        <v>45587</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -3959,12 +3959,12 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Day use in town for the extent of stay</t>
+          <t>SAEF</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3982,10 +3982,10 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>45594</v>
+        <v>45403</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>45594</v>
+        <v>45423</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -3994,12 +3994,12 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Derek Uhey</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4017,10 +4017,10 @@
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>45561</v>
+        <v>45629</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>45561</v>
+        <v>45647</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -4032,7 +4032,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H100" t="inlineStr"/>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Keven Griffen</t>
+        </is>
+      </c>
       <c r="I100" t="n">
         <v>107</v>
       </c>
@@ -4043,7 +4047,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4052,10 +4056,10 @@
         </is>
       </c>
       <c r="D101" s="2" t="n">
-        <v>45425</v>
+        <v>45610</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>45534</v>
+        <v>45614</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -4064,7 +4068,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -4078,7 +4082,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>keven</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4087,10 +4091,10 @@
         </is>
       </c>
       <c r="D102" s="2" t="n">
-        <v>45421</v>
+        <v>45629</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>45421</v>
+        <v>45648</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -4099,10 +4103,14 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr"/>
+          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Keven Griffen</t>
+        </is>
+      </c>
       <c r="I102" t="n">
         <v>105</v>
       </c>
@@ -4113,7 +4121,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4122,10 +4130,10 @@
         </is>
       </c>
       <c r="D103" s="2" t="n">
-        <v>45605</v>
+        <v>45595</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>45605</v>
+        <v>45599</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -4134,7 +4142,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pick up materials from home depot </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -4148,7 +4156,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lauren Orme</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4157,10 +4165,10 @@
         </is>
       </c>
       <c r="D104" s="2" t="n">
-        <v>45592</v>
+        <v>45401</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>45594</v>
+        <v>45410</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -4183,7 +4191,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4192,10 +4200,10 @@
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>45401</v>
+        <v>45568</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>45410</v>
+        <v>45572</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -4204,7 +4212,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>sierra ancha</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -4218,7 +4226,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4227,10 +4235,10 @@
         </is>
       </c>
       <c r="D106" s="2" t="n">
-        <v>45595</v>
+        <v>45605</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>45599</v>
+        <v>45605</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -4239,7 +4247,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">Pick up materials from home depot </t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
@@ -4253,7 +4261,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>keven</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4262,10 +4270,10 @@
         </is>
       </c>
       <c r="D107" s="2" t="n">
-        <v>45629</v>
+        <v>45421</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>45648</v>
+        <v>45421</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -4274,14 +4282,10 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>Keven Griffen</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr"/>
       <c r="I107" t="n">
         <v>100</v>
       </c>
@@ -4292,7 +4296,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4301,10 +4305,10 @@
         </is>
       </c>
       <c r="D108" s="2" t="n">
-        <v>45610</v>
+        <v>45425</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>45614</v>
+        <v>45534</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -4313,7 +4317,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -4327,7 +4331,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Derek Uhey</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4336,10 +4340,10 @@
         </is>
       </c>
       <c r="D109" s="2" t="n">
-        <v>45629</v>
+        <v>45561</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>45647</v>
+        <v>45561</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -4351,13 +4355,9 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>Keven Griffen</t>
-        </is>
-      </c>
+      <c r="H109" t="inlineStr"/>
       <c r="I109" t="n">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Lauren Orme</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4375,10 +4375,10 @@
         </is>
       </c>
       <c r="D110" s="2" t="n">
-        <v>45568</v>
+        <v>45592</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>45572</v>
+        <v>45594</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>sierra ancha</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -4410,10 +4410,10 @@
         </is>
       </c>
       <c r="D111" s="2" t="n">
-        <v>45523</v>
+        <v>45478</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>45524</v>
+        <v>45487</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Kimberly Walker</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4445,10 +4445,10 @@
         </is>
       </c>
       <c r="D112" s="2" t="n">
-        <v>45527</v>
+        <v>45440</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>45527</v>
+        <v>45440</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4480,10 +4480,10 @@
         </is>
       </c>
       <c r="D113" s="2" t="n">
-        <v>45441</v>
+        <v>45488</v>
       </c>
       <c r="E113" s="2" t="n">
-        <v>45442</v>
+        <v>45491</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -4495,7 +4495,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="H113" t="inlineStr"/>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Shay Levine</t>
+        </is>
+      </c>
       <c r="I113" t="n">
         <v>117</v>
       </c>
@@ -4506,7 +4510,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4515,10 +4519,10 @@
         </is>
       </c>
       <c r="D114" s="2" t="n">
-        <v>45516</v>
+        <v>45408</v>
       </c>
       <c r="E114" s="2" t="n">
-        <v>45521</v>
+        <v>45412</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -4541,7 +4545,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4550,10 +4554,10 @@
         </is>
       </c>
       <c r="D115" s="2" t="n">
-        <v>45533</v>
+        <v>45401</v>
       </c>
       <c r="E115" s="2" t="n">
-        <v>45534</v>
+        <v>45402</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -4562,14 +4566,10 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>I have a site visit coming up August 29th-30th and I was wondering if I could use a truck for this? It is to a location near Tsegi, AZ on Navajo Nation and it would be ideal to have a truck as there is a short section of dirt road needed to be crossed. This is for a restoration project in conjunction with Navajo Nation culturally important riparian areas work, an ongoing project to restore plants in traditionally significant areas. It would be a one night camp out trip.</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>Adair Patterson</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr"/>
       <c r="I115" t="n">
         <v>115</v>
       </c>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4589,10 +4589,10 @@
         </is>
       </c>
       <c r="D116" s="2" t="n">
-        <v>45496</v>
+        <v>45516</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>45506</v>
+        <v>45521</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -4615,7 +4615,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4624,10 +4624,10 @@
         </is>
       </c>
       <c r="D117" s="2" t="n">
-        <v>45401</v>
+        <v>45533</v>
       </c>
       <c r="E117" s="2" t="n">
-        <v>45402</v>
+        <v>45534</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -4636,10 +4636,14 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr"/>
+          <t>I have a site visit coming up August 29th-30th and I was wondering if I could use a truck for this? It is to a location near Tsegi, AZ on Navajo Nation and it would be ideal to have a truck as there is a short section of dirt road needed to be crossed. This is for a restoration project in conjunction with Navajo Nation culturally important riparian areas work, an ongoing project to restore plants in traditionally significant areas. It would be a one night camp out trip.</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Adair Patterson</t>
+        </is>
+      </c>
       <c r="I117" t="n">
         <v>113</v>
       </c>
@@ -4650,7 +4654,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4659,10 +4663,10 @@
         </is>
       </c>
       <c r="D118" s="2" t="n">
-        <v>45408</v>
+        <v>45441</v>
       </c>
       <c r="E118" s="2" t="n">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -4685,7 +4689,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4694,10 +4698,10 @@
         </is>
       </c>
       <c r="D119" s="2" t="n">
-        <v>45488</v>
+        <v>45527</v>
       </c>
       <c r="E119" s="2" t="n">
-        <v>45491</v>
+        <v>45527</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -4706,14 +4710,10 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>Shay Levine</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr"/>
       <c r="I119" t="n">
         <v>110</v>
       </c>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Kimberly Walker</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4733,10 +4733,10 @@
         </is>
       </c>
       <c r="D120" s="2" t="n">
-        <v>45440</v>
+        <v>45523</v>
       </c>
       <c r="E120" s="2" t="n">
-        <v>45440</v>
+        <v>45524</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -4745,7 +4745,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4768,10 +4768,10 @@
         </is>
       </c>
       <c r="D121" s="2" t="n">
-        <v>45478</v>
+        <v>45509</v>
       </c>
       <c r="E121" s="2" t="n">
-        <v>45487</v>
+        <v>45513</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -4794,7 +4794,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4803,10 +4803,10 @@
         </is>
       </c>
       <c r="D122" s="2" t="n">
-        <v>45509</v>
+        <v>45496</v>
       </c>
       <c r="E122" s="2" t="n">
-        <v>45513</v>
+        <v>45506</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-08-12 18:37:45
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J207"/>
+  <dimension ref="A1:J206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9505,42 +9505,6 @@
         </is>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>331</v>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="D207" s="2" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E207" s="2" t="n">
-        <v>45882</v>
-      </c>
-      <c r="F207" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="G207" t="inlineStr">
-        <is>
-          <t>testtt</t>
-        </is>
-      </c>
-      <c r="H207" t="inlineStr"/>
-      <c r="I207" t="n">
-        <v>205</v>
-      </c>
-      <c r="J207" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-12 18:38:23
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J206"/>
+  <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9505,6 +9505,42 @@
         </is>
       </c>
     </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>331</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="D207" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="E207" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>Test v4</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr"/>
+      <c r="I207" t="n">
+        <v>205</v>
+      </c>
+      <c r="J207" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-12 19:26:27
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J207"/>
+  <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9545,6 +9545,46 @@
         </is>
       </c>
     </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>331</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="D208" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="E208" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>testv5</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>['Jacob Shelly']</t>
+        </is>
+      </c>
+      <c r="I208" t="n">
+        <v>206</v>
+      </c>
+      <c r="J208" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-12-2025 -> 08-15-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5506,23 +5506,23 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E116" s="2" t="n">
-        <v>45881</v>
+        <v>45568</v>
       </c>
       <c r="F116" s="2" t="n">
-        <v>45884</v>
+        <v>45568</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Test v4</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -5539,18 +5539,22 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="J116" t="inlineStr"/>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>329 - David Auty</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -5559,10 +5563,10 @@
         </is>
       </c>
       <c r="E117" s="2" t="n">
-        <v>45568</v>
+        <v>45481</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>45568</v>
+        <v>45490</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -5576,12 +5580,12 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Jasmine Anenberg</t>
         </is>
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>329 - David Auty</t>
+          <t>331 - Michael Sloan</t>
         </is>
       </c>
     </row>
@@ -5594,7 +5598,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -5603,10 +5607,10 @@
         </is>
       </c>
       <c r="E118" s="2" t="n">
-        <v>45481</v>
+        <v>45761</v>
       </c>
       <c r="F118" s="2" t="n">
-        <v>45490</v>
+        <v>45765</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -5615,17 +5619,17 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">Our lab is traveling to Sante Fe, NM to attend the annual Western Forest Insect Work Conference. There will be will be 6 of us in total. </t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>Jasmine Anenberg</t>
+          <t>Tyler Gardner</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>331 - Michael Sloan</t>
+          <t>331 - Kristen Waring</t>
         </is>
       </c>
     </row>
@@ -5638,7 +5642,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -5647,10 +5651,10 @@
         </is>
       </c>
       <c r="E119" s="2" t="n">
-        <v>45761</v>
+        <v>45770</v>
       </c>
       <c r="F119" s="2" t="n">
-        <v>45765</v>
+        <v>45789</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -5659,17 +5663,17 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Our lab is traveling to Sante Fe, NM to attend the annual Western Forest Insect Work Conference. There will be will be 6 of us in total. </t>
+          <t xml:space="preserve">For NAU business in Mountain Campus and environs </t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>Tyler Gardner</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>331 - Kristen Waring</t>
+          <t>331 - Seafha Ramos</t>
         </is>
       </c>
     </row>
@@ -5682,7 +5686,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Jill Beckmann</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -5691,10 +5695,10 @@
         </is>
       </c>
       <c r="E120" s="2" t="n">
-        <v>45770</v>
+        <v>45747</v>
       </c>
       <c r="F120" s="2" t="n">
-        <v>45789</v>
+        <v>45752</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -5703,17 +5707,17 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t xml:space="preserve">For NAU business in Mountain Campus and environs </t>
+          <t xml:space="preserve">Logging sports Travel Use Travel to Fort Collins, CO 13 Poeple </t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Delana James, Shay Levine</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>331 - Seafha Ramos</t>
+          <t>331 - Jill Beckmann</t>
         </is>
       </c>
     </row>
@@ -5726,7 +5730,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Jill Beckmann</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -5735,10 +5739,10 @@
         </is>
       </c>
       <c r="E121" s="2" t="n">
-        <v>45747</v>
+        <v>45824</v>
       </c>
       <c r="F121" s="2" t="n">
-        <v>45752</v>
+        <v>45829</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -5747,17 +5751,17 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Logging sports Travel Use Travel to Fort Collins, CO 13 Poeple </t>
+          <t>trip to payson for writign workshop</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>Delana James, Shay Levine</t>
+          <t>Anita Antoninka, Matthew Bowker</t>
         </is>
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>331 - Jill Beckmann</t>
+          <t>331 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -5770,7 +5774,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -5779,10 +5783,10 @@
         </is>
       </c>
       <c r="E122" s="2" t="n">
-        <v>45824</v>
+        <v>45613</v>
       </c>
       <c r="F122" s="2" t="n">
-        <v>45829</v>
+        <v>45619</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -5791,17 +5795,17 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>trip to payson for writign workshop</t>
+          <t>This minivan is being requested to support staff/faculty travel to the Southwest Fire Ecology Conference, which is hosted and planned by the AZWI and SWFSC.</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>Anita Antoninka, Matthew Bowker</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>331 - Anita Joy Antoninka</t>
+          <t>331 - Wade Axup</t>
         </is>
       </c>
     </row>
@@ -5814,7 +5818,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -5823,10 +5827,10 @@
         </is>
       </c>
       <c r="E123" s="2" t="n">
-        <v>45613</v>
+        <v>45503</v>
       </c>
       <c r="F123" s="2" t="n">
-        <v>45619</v>
+        <v>45503</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -5835,17 +5839,17 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>This minivan is being requested to support staff/faculty travel to the Southwest Fire Ecology Conference, which is hosted and planned by the AZWI and SWFSC.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>Shay Levine</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>331 - Wade Axup</t>
+          <t>331 - CF</t>
         </is>
       </c>
     </row>
@@ -5858,7 +5862,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Molly McCormick</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -5867,10 +5871,10 @@
         </is>
       </c>
       <c r="E124" s="2" t="n">
-        <v>45503</v>
+        <v>45957</v>
       </c>
       <c r="F124" s="2" t="n">
-        <v>45503</v>
+        <v>45960</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -5879,17 +5883,17 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">	Take to the AZ WUI Summit in Prescott. Need the van to haul supplies.</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>Shay Levine</t>
+          <t>Molly McCormick, Andi Thode</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>331 - CF</t>
+          <t>331 - Molly McCormick</t>
         </is>
       </c>
     </row>
@@ -5902,7 +5906,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Molly McCormick</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -5911,10 +5915,10 @@
         </is>
       </c>
       <c r="E125" s="2" t="n">
-        <v>45957</v>
+        <v>45629</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>45960</v>
+        <v>45633</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -5923,17 +5927,17 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t xml:space="preserve">	Take to the AZ WUI Summit in Prescott. Need the van to haul supplies.</t>
+          <t xml:space="preserve">	This minivan is being requested to support staff/faculty travel to the AZ Wildland Urban Interface Summit, which is being planned and hosted by the AZWI &amp; SWFSC.</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>Molly McCormick, Andi Thode</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>331 - Molly McCormick</t>
+          <t>331 - Wade Axup</t>
         </is>
       </c>
     </row>
@@ -5946,7 +5950,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -5955,10 +5959,10 @@
         </is>
       </c>
       <c r="E126" s="2" t="n">
-        <v>45629</v>
+        <v>45534</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>45633</v>
+        <v>45553</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -5967,17 +5971,17 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t xml:space="preserve">	This minivan is being requested to support staff/faculty travel to the AZ Wildland Urban Interface Summit, which is being planned and hosted by the AZWI &amp; SWFSC.</t>
+          <t xml:space="preserve">transporting Dirt lab grad students and technicians to Jerome, AZ for a lab training event. </t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>331 - Wade Axup</t>
+          <t>331 - Michael Sloan</t>
         </is>
       </c>
     </row>
@@ -5990,7 +5994,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -5999,10 +6003,10 @@
         </is>
       </c>
       <c r="E127" s="2" t="n">
-        <v>45534</v>
+        <v>45737</v>
       </c>
       <c r="F127" s="2" t="n">
-        <v>45553</v>
+        <v>45741</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -6011,17 +6015,17 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t xml:space="preserve">transporting Dirt lab grad students and technicians to Jerome, AZ for a lab training event. </t>
+          <t xml:space="preserve">Field work to get out to the field using a different vehicle to get to campsite </t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Kara Gibson</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>331 - Michael Sloan</t>
+          <t>331 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -6034,7 +6038,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -6043,10 +6047,10 @@
         </is>
       </c>
       <c r="E128" s="2" t="n">
-        <v>45737</v>
+        <v>45929</v>
       </c>
       <c r="F128" s="2" t="n">
-        <v>45741</v>
+        <v>45935</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -6055,19 +6059,15 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t xml:space="preserve">Field work to get out to the field using a different vehicle to get to campsite </t>
+          <t>Taking lab group to conference in Denver.</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>Kara Gibson</t>
-        </is>
-      </c>
-      <c r="J128" t="inlineStr">
-        <is>
-          <t>331 - Matthew Bowker</t>
-        </is>
-      </c>
+          <t>['Anita Antoninka', 'Matthew Bowker', 'Keven Griffen', 'Benjamin Covington']</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Richard Hofstetter</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -6087,10 +6087,10 @@
         </is>
       </c>
       <c r="E129" s="2" t="n">
-        <v>45929</v>
+        <v>45605</v>
       </c>
       <c r="F129" s="2" t="n">
-        <v>45935</v>
+        <v>45609</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -6099,15 +6099,19 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Taking lab group to conference in Denver.</t>
+          <t xml:space="preserve">drive to Phoenix for a conference </t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>['Anita Antoninka', 'Matthew Bowker', 'Keven Griffen', 'Benjamin Covington']</t>
-        </is>
-      </c>
-      <c r="J129" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>331 - Richard Hofstetter</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -6118,7 +6122,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Richard Hofstetter</t>
+          <t>Catrin Edgeley</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -6127,10 +6131,10 @@
         </is>
       </c>
       <c r="E130" s="2" t="n">
-        <v>45605</v>
+        <v>45716</v>
       </c>
       <c r="F130" s="2" t="n">
-        <v>45609</v>
+        <v>45718</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -6139,17 +6143,17 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t xml:space="preserve">drive to Phoenix for a conference </t>
+          <t>Travel to and from Prescott for a writing retreat. Six travelers</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Catrin Edgeley, Cole Brant</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>331 - Richard Hofstetter</t>
+          <t>331 - Catrin Edgeley</t>
         </is>
       </c>
     </row>
@@ -6162,7 +6166,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Catrin Edgeley</t>
+          <t>Kimberly Walker</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -6171,10 +6175,10 @@
         </is>
       </c>
       <c r="E131" s="2" t="n">
-        <v>45716</v>
+        <v>45611</v>
       </c>
       <c r="F131" s="2" t="n">
-        <v>45718</v>
+        <v>45611</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -6183,17 +6187,17 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Travel to and from Prescott for a writing retreat. Six travelers</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>Catrin Edgeley, Cole Brant</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>331 - Catrin Edgeley</t>
+          <t>331 - Kimberly Walker</t>
         </is>
       </c>
     </row>
@@ -6202,11 +6206,11 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Kimberly Walker</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -6215,14 +6219,14 @@
         </is>
       </c>
       <c r="E132" s="2" t="n">
-        <v>45611</v>
+        <v>45555</v>
       </c>
       <c r="F132" s="2" t="n">
-        <v>45611</v>
+        <v>45555</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -6237,7 +6241,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>331 - Kimberly Walker</t>
+          <t xml:space="preserve">332 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -6250,7 +6254,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Carol Chambers</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -6259,10 +6263,10 @@
         </is>
       </c>
       <c r="E133" s="2" t="n">
-        <v>45555</v>
+        <v>45509</v>
       </c>
       <c r="F133" s="2" t="n">
-        <v>45555</v>
+        <v>45514</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -6271,17 +6275,17 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">Jumping mouse stuff. To and From the White Mountains. </t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Matthew Voorhees</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t xml:space="preserve">332 - Pete Fule </t>
+          <t>332 - Carol Chambers</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6298,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Carol Chambers</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -6303,10 +6307,10 @@
         </is>
       </c>
       <c r="E134" s="2" t="n">
-        <v>45509</v>
+        <v>45810</v>
       </c>
       <c r="F134" s="2" t="n">
-        <v>45514</v>
+        <v>45891</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -6315,17 +6319,17 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jumping mouse stuff. To and From the White Mountains. </t>
+          <t>Arizona Aspens</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>Matthew Voorhees</t>
+          <t>Jackson Bledsoe, Kristen Waring, Abiral Acharya, Julia Totty</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>332 - Carol Chambers</t>
+          <t>332 - Kristen Waring</t>
         </is>
       </c>
     </row>
@@ -6338,7 +6342,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -6347,10 +6351,10 @@
         </is>
       </c>
       <c r="E135" s="2" t="n">
-        <v>45810</v>
+        <v>45525</v>
       </c>
       <c r="F135" s="2" t="n">
-        <v>45891</v>
+        <v>45525</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -6359,17 +6363,17 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Arizona Aspens</t>
+          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data from some installed sensors, as part of our research project. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>Jackson Bledsoe, Kristen Waring, Abiral Acharya, Julia Totty</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>332 - Kristen Waring</t>
+          <t>332 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -6387,14 +6391,14 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E136" s="2" t="n">
-        <v>45525</v>
+        <v>45517</v>
       </c>
       <c r="F136" s="2" t="n">
-        <v>45525</v>
+        <v>45518</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -6403,12 +6407,12 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data from some installed sensors, as part of our research project. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
+          <t>We need a 4WD vehicle with room for 4 passengers, AC, and room for large equipment to drive to a remote field site for installing sensors. The field site is the SRP-funded Dude Fire project, which is located on the Tonto NF near Payson. Salli will drive and take 2-3 students. This is an overnight trip - we'll depart around 8am on 8/13 and return around 5pm on 8/14.</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
@@ -6431,14 +6435,14 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E137" s="2" t="n">
-        <v>45517</v>
+        <v>45764</v>
       </c>
       <c r="F137" s="2" t="n">
-        <v>45518</v>
+        <v>45775</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -6447,12 +6451,12 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>We need a 4WD vehicle with room for 4 passengers, AC, and room for large equipment to drive to a remote field site for installing sensors. The field site is the SRP-funded Dude Fire project, which is located on the Tonto NF near Payson. Salli will drive and take 2-3 students. This is an overnight trip - we'll depart around 8am on 8/13 and return around 5pm on 8/14.</t>
+          <t xml:space="preserve">This vehicle will be used to travel to Workman Creek in the Sierra Ancha Experimental Forest west of Globe, AZ to download monthly data and manage sensors. There will be a maximum of three passengers in the vehicle during this trip. </t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
@@ -6479,10 +6483,10 @@
         </is>
       </c>
       <c r="E138" s="2" t="n">
-        <v>45764</v>
+        <v>45453</v>
       </c>
       <c r="F138" s="2" t="n">
-        <v>45775</v>
+        <v>45477</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -6491,12 +6495,12 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t xml:space="preserve">This vehicle will be used to travel to Workman Creek in the Sierra Ancha Experimental Forest west of Globe, AZ to download monthly data and manage sensors. There will be a maximum of three passengers in the vehicle during this trip. </t>
+          <t>Sierra Ancha and Verde Valley, dates not needed are TBD</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
@@ -6514,7 +6518,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -6523,10 +6527,10 @@
         </is>
       </c>
       <c r="E139" s="2" t="n">
-        <v>45453</v>
+        <v>45478</v>
       </c>
       <c r="F139" s="2" t="n">
-        <v>45477</v>
+        <v>45506</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -6535,7 +6539,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Sierra Ancha and Verde Valley, dates not needed are TBD</t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -6545,7 +6549,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>332 - Salli Dymond</t>
+          <t xml:space="preserve">332 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -6567,10 +6571,10 @@
         </is>
       </c>
       <c r="E140" s="2" t="n">
-        <v>45478</v>
+        <v>45432</v>
       </c>
       <c r="F140" s="2" t="n">
-        <v>45506</v>
+        <v>45434</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -6602,7 +6606,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -6611,10 +6615,10 @@
         </is>
       </c>
       <c r="E141" s="2" t="n">
-        <v>45432</v>
+        <v>45756</v>
       </c>
       <c r="F141" s="2" t="n">
-        <v>45434</v>
+        <v>45761</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -6623,17 +6627,17 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve">Field work at diamond peak near payson, Arizona. 2-4 occupants. </t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Benjamin Covington</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t xml:space="preserve">332 - Pete Fule </t>
+          <t>332 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6650,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -6655,10 +6659,10 @@
         </is>
       </c>
       <c r="E142" s="2" t="n">
-        <v>45756</v>
+        <v>45804</v>
       </c>
       <c r="F142" s="2" t="n">
-        <v>45761</v>
+        <v>45805</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -6667,17 +6671,17 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Field work at diamond peak near payson, Arizona. 2-4 occupants. </t>
+          <t>Hi, I am hoping to borrow a 4x4 truck for the day to go to Tsegi AZ and participate in site evaluation for an upcoming restoration project this fall. I would leave early in the morning and return by mid afternoon. Only a day trip, no overnight.</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Benjamin Covington</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>332 - Matthew Bowker</t>
+          <t>332 - Adair Patterson</t>
         </is>
       </c>
     </row>
@@ -6690,7 +6694,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -6699,10 +6703,10 @@
         </is>
       </c>
       <c r="E143" s="2" t="n">
-        <v>45804</v>
+        <v>45439</v>
       </c>
       <c r="F143" s="2" t="n">
-        <v>45805</v>
+        <v>45445</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -6711,17 +6715,17 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Hi, I am hoping to borrow a 4x4 truck for the day to go to Tsegi AZ and participate in site evaluation for an upcoming restoration project this fall. I would leave early in the morning and return by mid afternoon. Only a day trip, no overnight.</t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>332 - Adair Patterson</t>
+          <t xml:space="preserve">332 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -6734,7 +6738,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -6743,10 +6747,10 @@
         </is>
       </c>
       <c r="E144" s="2" t="n">
-        <v>45439</v>
+        <v>45740</v>
       </c>
       <c r="F144" s="2" t="n">
-        <v>45445</v>
+        <v>45747</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -6755,17 +6759,17 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve">field work/trip to UTAH (please see other requests - looking for 3 trucks. </t>
         </is>
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Amy Whipple, Anita Antoninka, Audrey Harvey, Terry Hernandez</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t xml:space="preserve">332 - Pete Fule </t>
+          <t>332 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -6778,7 +6782,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -6787,10 +6791,10 @@
         </is>
       </c>
       <c r="E145" s="2" t="n">
-        <v>45740</v>
+        <v>45785</v>
       </c>
       <c r="F145" s="2" t="n">
-        <v>45747</v>
+        <v>45786</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -6799,17 +6803,17 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t xml:space="preserve">field work/trip to UTAH (please see other requests - looking for 3 trucks. </t>
+          <t xml:space="preserve">I need to drive to the Sierra Ancha Experimental Forest for a field visit. I'll need a 4WD vehicle with AC. I'm leaving midday on 5/8 and returning late evening on 5/9. </t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>Amy Whipple, Anita Antoninka, Audrey Harvey, Terry Hernandez</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>332 - Anita Joy Antoninka</t>
+          <t>332 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -6818,11 +6822,11 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -6831,29 +6835,29 @@
         </is>
       </c>
       <c r="E146" s="2" t="n">
-        <v>45785</v>
+        <v>45602</v>
       </c>
       <c r="F146" s="2" t="n">
-        <v>45786</v>
+        <v>45608</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t xml:space="preserve">I need to drive to the Sierra Ancha Experimental Forest for a field visit. I'll need a 4WD vehicle with AC. I'm leaving midday on 5/8 and returning late evening on 5/9. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>332 - Salli Dymond</t>
+          <t>333 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -6875,10 +6879,10 @@
         </is>
       </c>
       <c r="E147" s="2" t="n">
-        <v>45602</v>
+        <v>45627</v>
       </c>
       <c r="F147" s="2" t="n">
-        <v>45608</v>
+        <v>45636</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -6919,10 +6923,10 @@
         </is>
       </c>
       <c r="E148" s="2" t="n">
-        <v>45627</v>
+        <v>45617</v>
       </c>
       <c r="F148" s="2" t="n">
-        <v>45636</v>
+        <v>45623</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -6963,10 +6967,10 @@
         </is>
       </c>
       <c r="E149" s="2" t="n">
-        <v>45617</v>
+        <v>45627</v>
       </c>
       <c r="F149" s="2" t="n">
-        <v>45623</v>
+        <v>45688</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -6980,7 +6984,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Keven Griffen</t>
         </is>
       </c>
       <c r="J149" t="inlineStr">
@@ -6998,7 +7002,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -7007,10 +7011,10 @@
         </is>
       </c>
       <c r="E150" s="2" t="n">
-        <v>45627</v>
+        <v>45735</v>
       </c>
       <c r="F150" s="2" t="n">
-        <v>45688</v>
+        <v>45742</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -7019,17 +7023,17 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">We will be using the vehicle to travel to research sites &amp; collect data for Keven Griffen's PhD research. </t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>Keven Griffen</t>
+          <t>Keven Griffen, Kara Gibson</t>
         </is>
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>333 - Anita Joy Antoninka</t>
+          <t>333 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -7051,10 +7055,10 @@
         </is>
       </c>
       <c r="E151" s="2" t="n">
-        <v>45735</v>
+        <v>45716</v>
       </c>
       <c r="F151" s="2" t="n">
-        <v>45742</v>
+        <v>45725</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -7068,7 +7072,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>Keven Griffen, Kara Gibson</t>
+          <t>Keven Griffen</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
@@ -7086,7 +7090,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -7095,10 +7099,10 @@
         </is>
       </c>
       <c r="E152" s="2" t="n">
-        <v>45716</v>
+        <v>45541</v>
       </c>
       <c r="F152" s="2" t="n">
-        <v>45725</v>
+        <v>45571</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -7107,17 +7111,17 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t xml:space="preserve">We will be using the vehicle to travel to research sites &amp; collect data for Keven Griffen's PhD research. </t>
+          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>Keven Griffen</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>333 - Matthew Bowker</t>
+          <t>333 - Michael Sloan</t>
         </is>
       </c>
     </row>
@@ -7130,7 +7134,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -7139,10 +7143,10 @@
         </is>
       </c>
       <c r="E153" s="2" t="n">
-        <v>45541</v>
+        <v>45639</v>
       </c>
       <c r="F153" s="2" t="n">
-        <v>45571</v>
+        <v>45647</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -7151,7 +7155,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -7161,7 +7165,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>333 - Michael Sloan</t>
+          <t>333 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -7183,10 +7187,10 @@
         </is>
       </c>
       <c r="E154" s="2" t="n">
-        <v>45639</v>
+        <v>45748</v>
       </c>
       <c r="F154" s="2" t="n">
-        <v>45647</v>
+        <v>45752</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -7195,12 +7199,12 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Field work</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Anita Antoninka, Helen Rowe, Matthew Bowker</t>
         </is>
       </c>
       <c r="J154" t="inlineStr">
@@ -7218,7 +7222,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -7227,10 +7231,10 @@
         </is>
       </c>
       <c r="E155" s="2" t="n">
-        <v>45748</v>
+        <v>45432</v>
       </c>
       <c r="F155" s="2" t="n">
-        <v>45752</v>
+        <v>45433</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -7239,17 +7243,17 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Field work</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>Anita Antoninka, Helen Rowe, Matthew Bowker</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>333 - Anita Joy Antoninka</t>
+          <t>333 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -7262,7 +7266,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -7271,10 +7275,10 @@
         </is>
       </c>
       <c r="E156" s="2" t="n">
-        <v>45432</v>
+        <v>45421</v>
       </c>
       <c r="F156" s="2" t="n">
-        <v>45433</v>
+        <v>45421</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -7293,7 +7297,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>333 - Salli Dymond</t>
+          <t>333 - CF</t>
         </is>
       </c>
     </row>
@@ -7306,7 +7310,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Eric Olsen</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -7315,10 +7319,10 @@
         </is>
       </c>
       <c r="E157" s="2" t="n">
-        <v>45421</v>
+        <v>45401</v>
       </c>
       <c r="F157" s="2" t="n">
-        <v>45421</v>
+        <v>45402</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -7337,7 +7341,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>333 - CF</t>
+          <t>333 - Eric Olsen</t>
         </is>
       </c>
     </row>
@@ -7350,7 +7354,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Eric Olsen</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -7359,10 +7363,10 @@
         </is>
       </c>
       <c r="E158" s="2" t="n">
-        <v>45401</v>
+        <v>45422</v>
       </c>
       <c r="F158" s="2" t="n">
-        <v>45402</v>
+        <v>45427</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -7381,7 +7385,7 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>333 - Eric Olsen</t>
+          <t>333 - Michael Sloan</t>
         </is>
       </c>
     </row>
@@ -7394,7 +7398,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -7403,10 +7407,10 @@
         </is>
       </c>
       <c r="E159" s="2" t="n">
-        <v>45422</v>
+        <v>45444</v>
       </c>
       <c r="F159" s="2" t="n">
-        <v>45427</v>
+        <v>45536</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -7415,7 +7419,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>New Mexico, dates not needed are TBD</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -7425,7 +7429,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>333 - Michael Sloan</t>
+          <t>333 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -7438,7 +7442,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -7447,10 +7451,10 @@
         </is>
       </c>
       <c r="E160" s="2" t="n">
-        <v>45444</v>
+        <v>45713</v>
       </c>
       <c r="F160" s="2" t="n">
-        <v>45536</v>
+        <v>45714</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -7459,17 +7463,17 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>New Mexico, dates not needed are TBD</t>
+          <t xml:space="preserve">The purpose of this trip is to troubleshoot an evapotranspiration sensor and select stream sampling points in the study site. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Jamie Ortega, Logan Ozmet</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>333 - Anita Joy Antoninka</t>
+          <t>333 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -7482,19 +7486,19 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E161" s="2" t="n">
-        <v>45713</v>
+        <v>45778</v>
       </c>
       <c r="F161" s="2" t="n">
-        <v>45714</v>
+        <v>45930</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -7503,17 +7507,17 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t xml:space="preserve">The purpose of this trip is to troubleshoot an evapotranspiration sensor and select stream sampling points in the study site. Our destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Jaime Ortega and Logan Ozment). </t>
+          <t>Anticipated research locations	 Utah, NM, AZ, CA, NV</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>Jamie Ortega, Logan Ozmet</t>
+          <t>Anita Antoninka, Matthew Bowker, Jasmine Anenberg, Keven Griffen, Benjamin Covington</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>333 - Salli Dymond</t>
+          <t>333 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -7522,42 +7526,42 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E162" s="2" t="n">
-        <v>45778</v>
+        <v>45425</v>
       </c>
       <c r="F162" s="2" t="n">
-        <v>45930</v>
+        <v>45474</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Anticipated research locations	 Utah, NM, AZ, CA, NV</t>
+          <t>Tonto/ dates not needed TBD</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>Anita Antoninka, Matthew Bowker, Jasmine Anenberg, Keven Griffen, Benjamin Covington</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>333 - Anita Joy Antoninka</t>
+          <t>338 - Margaret Moore</t>
         </is>
       </c>
     </row>
@@ -7579,10 +7583,10 @@
         </is>
       </c>
       <c r="E163" s="2" t="n">
-        <v>45425</v>
+        <v>45581</v>
       </c>
       <c r="F163" s="2" t="n">
-        <v>45474</v>
+        <v>45587</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -7591,7 +7595,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Tonto/ dates not needed TBD</t>
+          <t>SAEF</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -7614,7 +7618,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -7623,10 +7627,10 @@
         </is>
       </c>
       <c r="E164" s="2" t="n">
-        <v>45581</v>
+        <v>45401</v>
       </c>
       <c r="F164" s="2" t="n">
-        <v>45587</v>
+        <v>45402</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -7635,7 +7639,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>SAEF</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -7645,7 +7649,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>338 - Margaret Moore</t>
+          <t>338 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -7658,7 +7662,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -7667,10 +7671,10 @@
         </is>
       </c>
       <c r="E165" s="2" t="n">
-        <v>45401</v>
+        <v>45475</v>
       </c>
       <c r="F165" s="2" t="n">
-        <v>45402</v>
+        <v>45565</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -7679,7 +7683,7 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Tonto</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -7689,7 +7693,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>338 - Matthew Bowker</t>
+          <t>338 - Margaret Moore</t>
         </is>
       </c>
     </row>
@@ -7702,7 +7706,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -7711,10 +7715,10 @@
         </is>
       </c>
       <c r="E166" s="2" t="n">
-        <v>45475</v>
+        <v>45597</v>
       </c>
       <c r="F166" s="2" t="n">
-        <v>45565</v>
+        <v>45613</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -7723,7 +7727,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Tonto</t>
+          <t>Day use in town for the extent of stay</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -7733,7 +7737,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>338 - Margaret Moore</t>
+          <t>338 - Seafha Ramos</t>
         </is>
       </c>
     </row>
@@ -7746,19 +7750,19 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E167" s="2" t="n">
-        <v>45597</v>
+        <v>45667</v>
       </c>
       <c r="F167" s="2" t="n">
-        <v>45613</v>
+        <v>45787</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -7767,17 +7771,17 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Day use in town for the extent of stay</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Peter Fule</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>338 - Seafha Ramos</t>
+          <t xml:space="preserve">338 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -7790,19 +7794,19 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E168" s="2" t="n">
-        <v>45667</v>
+        <v>45845</v>
       </c>
       <c r="F168" s="2" t="n">
-        <v>45787</v>
+        <v>45856</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -7811,17 +7815,17 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">	 Travel to field site near Alpine, AZ and nearby camping locations. 2 occupants and drivers - Waring and Bledsoe.</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>Peter Fule</t>
+          <t>Kristen Waring, Jackson Bledsoe</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t xml:space="preserve">338 - Pete Fule </t>
+          <t>338 - Kristen Waring</t>
         </is>
       </c>
     </row>
@@ -7834,7 +7838,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>Andi Thode</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -7843,10 +7847,10 @@
         </is>
       </c>
       <c r="E169" s="2" t="n">
-        <v>45845</v>
+        <v>45859</v>
       </c>
       <c r="F169" s="2" t="n">
-        <v>45856</v>
+        <v>45898</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -7855,17 +7859,17 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t xml:space="preserve">	 Travel to field site near Alpine, AZ and nearby camping locations. 2 occupants and drivers - Waring and Bledsoe.</t>
+          <t xml:space="preserve">	Local field work on the Mogollon and Peaks Ranger Districts</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>Kristen Waring, Jackson Bledsoe</t>
+          <t>Scott Gilb</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>338 - Kristen Waring</t>
+          <t>338 - Andi Thode</t>
         </is>
       </c>
     </row>
@@ -7878,7 +7882,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Andi Thode</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -7887,10 +7891,10 @@
         </is>
       </c>
       <c r="E170" s="2" t="n">
-        <v>45859</v>
+        <v>45798</v>
       </c>
       <c r="F170" s="2" t="n">
-        <v>45898</v>
+        <v>45834</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -7899,17 +7903,17 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t xml:space="preserve">	Local field work on the Mogollon and Peaks Ranger Districts</t>
+          <t>We will travel to study sites on Forest Service dirt roads, rough terrain conditions, so we need a 4WD truck.  We will have 3-4 people plus gear in the truck.  Need the truck bed large enough hold 1-m2 sampling frame (quadrats) plus gear.   Have used 333 Toyota Tacoma and 338 Nissan Titan for this purpose in the past.</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>Scott Gilb</t>
+          <t>Catherine Young, CJ Horn, Delana James, Margaret Moore, Mariola Barrera, Haley Rosenberg</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>338 - Andi Thode</t>
+          <t>338 - Margaret Moore</t>
         </is>
       </c>
     </row>
@@ -7922,7 +7926,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Catrin Edgeley</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -7931,10 +7935,10 @@
         </is>
       </c>
       <c r="E171" s="2" t="n">
-        <v>45798</v>
+        <v>45594</v>
       </c>
       <c r="F171" s="2" t="n">
-        <v>45834</v>
+        <v>45594</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -7943,17 +7947,17 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>We will travel to study sites on Forest Service dirt roads, rough terrain conditions, so we need a 4WD truck.  We will have 3-4 people plus gear in the truck.  Need the truck bed large enough hold 1-m2 sampling frame (quadrats) plus gear.   Have used 333 Toyota Tacoma and 338 Nissan Titan for this purpose in the past.</t>
+          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>Catherine Young, CJ Horn, Delana James, Margaret Moore, Mariola Barrera, Haley Rosenberg</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>338 - Margaret Moore</t>
+          <t>338 - Catrin Edgeley</t>
         </is>
       </c>
     </row>
@@ -7966,7 +7970,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Catrin Edgeley</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -7975,10 +7979,10 @@
         </is>
       </c>
       <c r="E172" s="2" t="n">
-        <v>45594</v>
+        <v>45403</v>
       </c>
       <c r="F172" s="2" t="n">
-        <v>45594</v>
+        <v>45423</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -7987,7 +7991,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -7997,7 +8001,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>338 - Catrin Edgeley</t>
+          <t>338 - Seafha Ramos</t>
         </is>
       </c>
     </row>
@@ -8006,11 +8010,11 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -8019,29 +8023,29 @@
         </is>
       </c>
       <c r="E173" s="2" t="n">
-        <v>45403</v>
+        <v>45744</v>
       </c>
       <c r="F173" s="2" t="n">
-        <v>45423</v>
+        <v>45762</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">Vehicle will be used to transport field crew and gear to and from research sites in the Mojave Desert near Primm, NV and Pahrump, NV. There will be 2-5 occupants. </t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Sienna Chapman</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>338 - Seafha Ramos</t>
+          <t>331 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -8050,11 +8054,11 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -8063,10 +8067,10 @@
         </is>
       </c>
       <c r="E174" s="2" t="n">
-        <v>45744</v>
+        <v>45425</v>
       </c>
       <c r="F174" s="2" t="n">
-        <v>45762</v>
+        <v>45534</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -8075,17 +8079,17 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vehicle will be used to transport field crew and gear to and from research sites in the Mojave Desert near Primm, NV and Pahrump, NV. There will be 2-5 occupants. </t>
+          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>Sienna Chapman</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>331 - Anita Joy Antoninka</t>
+          <t>466 - Kristen Waring</t>
         </is>
       </c>
     </row>
@@ -8098,7 +8102,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -8107,10 +8111,10 @@
         </is>
       </c>
       <c r="E175" s="2" t="n">
-        <v>45425</v>
+        <v>45568</v>
       </c>
       <c r="F175" s="2" t="n">
-        <v>45534</v>
+        <v>45572</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -8119,7 +8123,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
+          <t>sierra ancha</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -8129,7 +8133,7 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>466 - Kristen Waring</t>
+          <t>466 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -8142,7 +8146,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -8151,10 +8155,10 @@
         </is>
       </c>
       <c r="E176" s="2" t="n">
-        <v>45568</v>
+        <v>45595</v>
       </c>
       <c r="F176" s="2" t="n">
-        <v>45572</v>
+        <v>45599</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -8163,7 +8167,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>sierra ancha</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -8173,7 +8177,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>466 - Salli Dymond</t>
+          <t>466 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -8186,7 +8190,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -8195,10 +8199,10 @@
         </is>
       </c>
       <c r="E177" s="2" t="n">
-        <v>45595</v>
+        <v>45629</v>
       </c>
       <c r="F177" s="2" t="n">
-        <v>45599</v>
+        <v>45647</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -8212,12 +8216,12 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Keven Griffen</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>466 - Anita Joy Antoninka</t>
+          <t>466 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -8230,7 +8234,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -8242,7 +8246,7 @@
         <v>45629</v>
       </c>
       <c r="F178" s="2" t="n">
-        <v>45647</v>
+        <v>45648</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -8251,7 +8255,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -8261,7 +8265,7 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>466 - Matthew Bowker</t>
+          <t>466 - TBD</t>
         </is>
       </c>
     </row>
@@ -8274,7 +8278,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Helen Rowe</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -8283,10 +8287,10 @@
         </is>
       </c>
       <c r="E179" s="2" t="n">
-        <v>45629</v>
+        <v>45688</v>
       </c>
       <c r="F179" s="2" t="n">
-        <v>45648</v>
+        <v>45690</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -8295,17 +8299,17 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
+          <t>Biocrust Research</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>Keven Griffen</t>
+          <t>Darren Olney</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>466 - TBD</t>
+          <t>466 - Helen Rowe</t>
         </is>
       </c>
     </row>
@@ -8318,7 +8322,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Helen Rowe</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -8327,10 +8331,10 @@
         </is>
       </c>
       <c r="E180" s="2" t="n">
-        <v>45688</v>
+        <v>45401</v>
       </c>
       <c r="F180" s="2" t="n">
-        <v>45690</v>
+        <v>45410</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -8339,17 +8343,17 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Biocrust Research</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>Darren Olney</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>466 - Helen Rowe</t>
+          <t>466 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -8362,7 +8366,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -8371,10 +8375,10 @@
         </is>
       </c>
       <c r="E181" s="2" t="n">
-        <v>45401</v>
+        <v>45709</v>
       </c>
       <c r="F181" s="2" t="n">
-        <v>45410</v>
+        <v>45711</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -8383,17 +8387,17 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve"> We will be traveling to our field sites near Superior, AZ, for data collection &amp; site maintenance. </t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Keven Griffen</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>466 - Anita Joy Antoninka</t>
+          <t>466 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -8406,7 +8410,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -8415,10 +8419,10 @@
         </is>
       </c>
       <c r="E182" s="2" t="n">
-        <v>45709</v>
+        <v>45610</v>
       </c>
       <c r="F182" s="2" t="n">
-        <v>45711</v>
+        <v>45614</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -8427,17 +8431,17 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We will be traveling to our field sites near Superior, AZ, for data collection &amp; site maintenance. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>Keven Griffen</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>466 - Matthew Bowker</t>
+          <t>466 - TBD</t>
         </is>
       </c>
     </row>
@@ -8450,7 +8454,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -8459,10 +8463,10 @@
         </is>
       </c>
       <c r="E183" s="2" t="n">
-        <v>45610</v>
+        <v>45729</v>
       </c>
       <c r="F183" s="2" t="n">
-        <v>45614</v>
+        <v>45730</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -8471,17 +8475,17 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data and collect stream water samples. Our destination trip is Tonto NF near Payson, AZ. One occupant will be in the vehicle (Jaime Ortega). </t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>Jamie Ortega</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>466 - TBD</t>
+          <t>466 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -8494,7 +8498,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Derek Uhey</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -8503,10 +8507,10 @@
         </is>
       </c>
       <c r="E184" s="2" t="n">
-        <v>45729</v>
+        <v>45561</v>
       </c>
       <c r="F184" s="2" t="n">
-        <v>45730</v>
+        <v>45561</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -8515,17 +8519,17 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t xml:space="preserve">The purpose of this trip is to download evapotranspiration data and collect stream water samples. Our destination trip is Tonto NF near Payson, AZ. One occupant will be in the vehicle (Jaime Ortega). </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>Jamie Ortega</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>466 - Salli Dymond</t>
+          <t>466 - Derek Uhey</t>
         </is>
       </c>
     </row>
@@ -8538,7 +8542,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Derek Uhey</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -8547,10 +8551,10 @@
         </is>
       </c>
       <c r="E185" s="2" t="n">
-        <v>45561</v>
+        <v>45778</v>
       </c>
       <c r="F185" s="2" t="n">
-        <v>45561</v>
+        <v>45796</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -8559,17 +8563,17 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Pheonix</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Anita Antoninka</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>466 - Derek Uhey</t>
+          <t>466 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -8582,7 +8586,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -8591,10 +8595,10 @@
         </is>
       </c>
       <c r="E186" s="2" t="n">
-        <v>45778</v>
+        <v>45605</v>
       </c>
       <c r="F186" s="2" t="n">
-        <v>45796</v>
+        <v>45605</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -8603,17 +8607,17 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Pheonix</t>
+          <t xml:space="preserve">Pick up materials from home depot </t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>Anita Antoninka</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>466 - Anita Joy Antoninka</t>
+          <t>466 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -8626,7 +8630,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -8635,10 +8639,10 @@
         </is>
       </c>
       <c r="E187" s="2" t="n">
-        <v>45605</v>
+        <v>45820</v>
       </c>
       <c r="F187" s="2" t="n">
-        <v>45605</v>
+        <v>45900</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -8647,17 +8651,17 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pick up materials from home depot </t>
+          <t>Flagstaff area</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Peter Fule, Sophia Czosek, Elena Powell</t>
         </is>
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>466 - Matthew Bowker</t>
+          <t xml:space="preserve">466 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -8670,7 +8674,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Lauren Orme</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -8679,10 +8683,10 @@
         </is>
       </c>
       <c r="E188" s="2" t="n">
-        <v>45820</v>
+        <v>45592</v>
       </c>
       <c r="F188" s="2" t="n">
-        <v>45900</v>
+        <v>45594</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -8691,17 +8695,17 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Flagstaff area</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>Peter Fule, Sophia Czosek, Elena Powell</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t xml:space="preserve">466 - Pete Fule </t>
+          <t>466 - Lauren Orme</t>
         </is>
       </c>
     </row>
@@ -8714,7 +8718,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Lauren Orme</t>
+          <t>Gabrielle Ayres</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -8723,10 +8727,10 @@
         </is>
       </c>
       <c r="E189" s="2" t="n">
-        <v>45592</v>
+        <v>45677</v>
       </c>
       <c r="F189" s="2" t="n">
-        <v>45594</v>
+        <v>45678</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -8735,17 +8739,17 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Traveling to Phoenix to meet with Tonto National Forest staff and attend a 1 day field trip across the Tonto National Forest - driving dirt roads to visit fire scars. Total number of occupants - full vehicle.</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Andi Thode, Gabrielle Ayres</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>466 - Lauren Orme</t>
+          <t>466 - Gabrielle Ayres</t>
         </is>
       </c>
     </row>
@@ -8758,7 +8762,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Gabrielle Ayres</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -8767,10 +8771,10 @@
         </is>
       </c>
       <c r="E190" s="2" t="n">
-        <v>45677</v>
+        <v>45421</v>
       </c>
       <c r="F190" s="2" t="n">
-        <v>45678</v>
+        <v>45421</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -8779,17 +8783,17 @@
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Traveling to Phoenix to meet with Tonto National Forest staff and attend a 1 day field trip across the Tonto National Forest - driving dirt roads to visit fire scars. Total number of occupants - full vehicle.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>Andi Thode, Gabrielle Ayres</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>466 - Gabrielle Ayres</t>
+          <t>466 - CF</t>
         </is>
       </c>
     </row>
@@ -8798,11 +8802,11 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Kimberly Walker</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -8811,14 +8815,14 @@
         </is>
       </c>
       <c r="E191" s="2" t="n">
-        <v>45421</v>
+        <v>45440</v>
       </c>
       <c r="F191" s="2" t="n">
-        <v>45421</v>
+        <v>45440</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -8833,7 +8837,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>466 - CF</t>
+          <t>467 - Kimberly Walker</t>
         </is>
       </c>
     </row>
@@ -8846,7 +8850,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Kimberly Walker</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -8855,10 +8859,10 @@
         </is>
       </c>
       <c r="E192" s="2" t="n">
-        <v>45440</v>
+        <v>45740</v>
       </c>
       <c r="F192" s="2" t="n">
-        <v>45440</v>
+        <v>45747</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -8867,17 +8871,17 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve">field work/trip to UTAH (please see other requests - looking for 3 trucks. </t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Amy Whipple, Anita Antoninka, Audrey Harvey, Terry Hernandez</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>467 - Kimberly Walker</t>
+          <t>467 - Anita Joy Antoninka</t>
         </is>
       </c>
     </row>
@@ -8890,7 +8894,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -8899,10 +8903,10 @@
         </is>
       </c>
       <c r="E193" s="2" t="n">
-        <v>45740</v>
+        <v>45478</v>
       </c>
       <c r="F193" s="2" t="n">
-        <v>45747</v>
+        <v>45487</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -8911,17 +8915,17 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t xml:space="preserve">field work/trip to UTAH (please see other requests - looking for 3 trucks. </t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>Amy Whipple, Anita Antoninka, Audrey Harvey, Terry Hernandez</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>467 - Anita Joy Antoninka</t>
+          <t xml:space="preserve">467 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -8934,7 +8938,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -8943,10 +8947,10 @@
         </is>
       </c>
       <c r="E194" s="2" t="n">
-        <v>45478</v>
+        <v>45722</v>
       </c>
       <c r="F194" s="2" t="n">
-        <v>45487</v>
+        <v>45730</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -8955,17 +8959,17 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve">Field work at Diamond Peak, Arizona (North East of Payson, Arizona). There will be 4 occupants, 2 per vehicle. Vehicles will have to drive on moderate dirt roads. </t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Benjamin Covington, Mikaya Wason</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t xml:space="preserve">467 - Pete Fule </t>
+          <t>467 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -8978,19 +8982,19 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Carol Chambers</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E195" s="2" t="n">
-        <v>45722</v>
+        <v>45768</v>
       </c>
       <c r="F195" s="2" t="n">
-        <v>45730</v>
+        <v>45928</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -8999,17 +9003,17 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t xml:space="preserve">Field work at Diamond Peak, Arizona (North East of Payson, Arizona). There will be 4 occupants, 2 per vehicle. Vehicles will have to drive on moderate dirt roads. </t>
+          <t>Anticipated research locations	Bandelier National Monument (NM) Valles Caldera National Monument (NM)</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>Benjamin Covington, Mikaya Wason</t>
+          <t>José G. Martínez-Fonseca, Carol Chambers</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>467 - Matthew Bowker</t>
+          <t>467 - Carol Chambers</t>
         </is>
       </c>
     </row>
@@ -9022,19 +9026,19 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Carol Chambers</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E196" s="2" t="n">
-        <v>45768</v>
+        <v>45757</v>
       </c>
       <c r="F196" s="2" t="n">
-        <v>45928</v>
+        <v>45761</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -9043,17 +9047,17 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Anticipated research locations	Bandelier National Monument (NM) Valles Caldera National Monument (NM)</t>
+          <t xml:space="preserve">We will be traveling to Superior, AZ in order to conduct field research in support of Keven Griffen's PhD research </t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>José G. Martínez-Fonseca, Carol Chambers</t>
+          <t>Megan Dreher, Keven Griffen, Mairead Brogan</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>467 - Carol Chambers</t>
+          <t>467 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -9066,7 +9070,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -9075,10 +9079,10 @@
         </is>
       </c>
       <c r="E197" s="2" t="n">
-        <v>45757</v>
+        <v>45533</v>
       </c>
       <c r="F197" s="2" t="n">
-        <v>45761</v>
+        <v>45534</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -9087,17 +9091,17 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t xml:space="preserve">We will be traveling to Superior, AZ in order to conduct field research in support of Keven Griffen's PhD research </t>
+          <t>I have a site visit coming up August 29th-30th and I was wondering if I could use a truck for this? It is to a location near Tsegi, AZ on Navajo Nation and it would be ideal to have a truck as there is a short section of dirt road needed to be crossed. This is for a restoration project in conjunction with Navajo Nation culturally important riparian areas work, an ongoing project to restore plants in traditionally significant areas. It would be a one night camp out trip.</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>Megan Dreher, Keven Griffen, Mairead Brogan</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>467 - Matthew Bowker</t>
+          <t>467 - Adair Patterson</t>
         </is>
       </c>
     </row>
@@ -9110,7 +9114,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -9119,10 +9123,10 @@
         </is>
       </c>
       <c r="E198" s="2" t="n">
-        <v>45533</v>
+        <v>45441</v>
       </c>
       <c r="F198" s="2" t="n">
-        <v>45534</v>
+        <v>45442</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -9131,17 +9135,17 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>I have a site visit coming up August 29th-30th and I was wondering if I could use a truck for this? It is to a location near Tsegi, AZ on Navajo Nation and it would be ideal to have a truck as there is a short section of dirt road needed to be crossed. This is for a restoration project in conjunction with Navajo Nation culturally important riparian areas work, an ongoing project to restore plants in traditionally significant areas. It would be a one night camp out trip.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>467 - Adair Patterson</t>
+          <t>467 - Kristen Waring</t>
         </is>
       </c>
     </row>
@@ -9154,7 +9158,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -9163,10 +9167,10 @@
         </is>
       </c>
       <c r="E199" s="2" t="n">
-        <v>45441</v>
+        <v>45488</v>
       </c>
       <c r="F199" s="2" t="n">
-        <v>45442</v>
+        <v>45491</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -9180,12 +9184,12 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Shay Levine</t>
         </is>
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>467 - Kristen Waring</t>
+          <t>467 - CF</t>
         </is>
       </c>
     </row>
@@ -9207,10 +9211,10 @@
         </is>
       </c>
       <c r="E200" s="2" t="n">
-        <v>45488</v>
+        <v>45509</v>
       </c>
       <c r="F200" s="2" t="n">
-        <v>45491</v>
+        <v>45513</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -9224,7 +9228,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>Shay Levine</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
@@ -9251,10 +9255,10 @@
         </is>
       </c>
       <c r="E201" s="2" t="n">
-        <v>45509</v>
+        <v>45516</v>
       </c>
       <c r="F201" s="2" t="n">
-        <v>45513</v>
+        <v>45521</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -9286,7 +9290,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -9295,10 +9299,10 @@
         </is>
       </c>
       <c r="E202" s="2" t="n">
-        <v>45516</v>
+        <v>45527</v>
       </c>
       <c r="F202" s="2" t="n">
-        <v>45521</v>
+        <v>45527</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -9307,7 +9311,7 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
@@ -9317,7 +9321,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>467 - CF</t>
+          <t>467 - David Auty</t>
         </is>
       </c>
     </row>
@@ -9330,7 +9334,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -9339,10 +9343,10 @@
         </is>
       </c>
       <c r="E203" s="2" t="n">
-        <v>45527</v>
+        <v>45401</v>
       </c>
       <c r="F203" s="2" t="n">
-        <v>45527</v>
+        <v>45402</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -9351,7 +9355,7 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I203" t="inlineStr">
@@ -9361,7 +9365,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>467 - David Auty</t>
+          <t>467 - Matthew Bowker</t>
         </is>
       </c>
     </row>
@@ -9374,7 +9378,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -9383,10 +9387,10 @@
         </is>
       </c>
       <c r="E204" s="2" t="n">
-        <v>45401</v>
+        <v>45496</v>
       </c>
       <c r="F204" s="2" t="n">
-        <v>45402</v>
+        <v>45506</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -9395,7 +9399,7 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
@@ -9405,7 +9409,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>467 - Matthew Bowker</t>
+          <t xml:space="preserve">467 - Pete Fule </t>
         </is>
       </c>
     </row>
@@ -9427,10 +9431,10 @@
         </is>
       </c>
       <c r="E205" s="2" t="n">
-        <v>45496</v>
+        <v>45523</v>
       </c>
       <c r="F205" s="2" t="n">
-        <v>45506</v>
+        <v>45524</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -9439,7 +9443,7 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -9462,7 +9466,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -9471,10 +9475,10 @@
         </is>
       </c>
       <c r="E206" s="2" t="n">
-        <v>45523</v>
+        <v>45431</v>
       </c>
       <c r="F206" s="2" t="n">
-        <v>45524</v>
+        <v>45436</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -9483,7 +9487,7 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
+          <t xml:space="preserve">Sierra Ancha, </t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
@@ -9493,7 +9497,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t xml:space="preserve">467 - Pete Fule </t>
+          <t>467 - Salli Dymond</t>
         </is>
       </c>
     </row>
@@ -9506,7 +9510,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -9515,10 +9519,10 @@
         </is>
       </c>
       <c r="E207" s="2" t="n">
-        <v>45431</v>
+        <v>45408</v>
       </c>
       <c r="F207" s="2" t="n">
-        <v>45436</v>
+        <v>45412</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -9527,7 +9531,7 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sierra Ancha, </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
@@ -9536,50 +9540,6 @@
         </is>
       </c>
       <c r="J207" t="inlineStr">
-        <is>
-          <t>467 - Salli Dymond</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>467</v>
-      </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>Michael Sloan</t>
-        </is>
-      </c>
-      <c r="D208" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E208" s="2" t="n">
-        <v>45408</v>
-      </c>
-      <c r="F208" s="2" t="n">
-        <v>45412</v>
-      </c>
-      <c r="G208" t="inlineStr">
-        <is>
-          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
-        </is>
-      </c>
-      <c r="H208" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I208" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J208" t="inlineStr">
         <is>
           <t>467 - Michael Sloan</t>
         </is>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 19:02:22
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10015,14 +10015,14 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E209" s="2" t="n">
-        <v>45882</v>
+        <v>45877</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45887</v>
+        <v>45889</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>test uid</t>
+          <t>test uid 209</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 19:17:54
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0001</t>
+          <t>0209</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0025</t>
+          <t>0210</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0024</t>
+          <t>0211</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -630,7 +630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0023</t>
+          <t>0212</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0021</t>
+          <t>0213</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0020</t>
+          <t>0214</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0019</t>
+          <t>0215</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -814,7 +814,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0018</t>
+          <t>0216</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -860,7 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0017</t>
+          <t>0217</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -906,7 +906,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0016</t>
+          <t>0218</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0015</t>
+          <t>0219</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -998,7 +998,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0014</t>
+          <t>0220</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1044,7 +1044,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0022</t>
+          <t>0221</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1090,7 +1090,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0012</t>
+          <t>0222</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1136,7 +1136,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0011</t>
+          <t>0223</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1182,7 +1182,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0010</t>
+          <t>0224</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1228,7 +1228,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0009</t>
+          <t>0225</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1274,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0008</t>
+          <t>0226</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1320,7 +1320,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0007</t>
+          <t>0227</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0006</t>
+          <t>0228</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1412,7 +1412,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0005</t>
+          <t>0229</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1458,7 +1458,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0013</t>
+          <t>0230</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1504,7 +1504,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0004</t>
+          <t>0231</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1550,7 +1550,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0003</t>
+          <t>0232</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1596,7 +1596,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0002</t>
+          <t>0233</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1642,7 +1642,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0035</t>
+          <t>0234</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1688,7 +1688,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0038</t>
+          <t>0235</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1734,7 +1734,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0037</t>
+          <t>0236</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1780,7 +1780,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0034</t>
+          <t>0237</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1826,7 +1826,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0036</t>
+          <t>0238</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1872,7 +1872,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0033</t>
+          <t>0239</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1918,7 +1918,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0029</t>
+          <t>0240</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1964,7 +1964,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0031</t>
+          <t>0241</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2010,7 +2010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0030</t>
+          <t>0242</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2056,7 +2056,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>0028</t>
+          <t>0243</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2102,7 +2102,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0027</t>
+          <t>0244</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2148,7 +2148,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0026</t>
+          <t>0245</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2194,7 +2194,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0032</t>
+          <t>0246</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2240,7 +2240,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>0046</t>
+          <t>0247</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2286,7 +2286,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0050</t>
+          <t>0248</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2332,7 +2332,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0049</t>
+          <t>0249</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2378,7 +2378,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0048</t>
+          <t>0250</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2424,7 +2424,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0047</t>
+          <t>0251</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2470,7 +2470,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0045</t>
+          <t>0252</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2516,7 +2516,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0042</t>
+          <t>0253</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2562,7 +2562,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>0043</t>
+          <t>0254</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2608,7 +2608,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0041</t>
+          <t>0255</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2654,7 +2654,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0040</t>
+          <t>0256</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2700,7 +2700,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0039</t>
+          <t>0257</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2746,7 +2746,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0044</t>
+          <t>0258</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2792,7 +2792,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0071</t>
+          <t>0259</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2838,7 +2838,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0070</t>
+          <t>0260</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2884,7 +2884,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0069</t>
+          <t>0261</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2930,7 +2930,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0068</t>
+          <t>0262</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2976,7 +2976,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0067</t>
+          <t>0263</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -3022,7 +3022,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0066</t>
+          <t>0264</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -3068,7 +3068,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0064</t>
+          <t>0265</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3114,7 +3114,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0063</t>
+          <t>0266</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -3160,7 +3160,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0062</t>
+          <t>0267</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3206,7 +3206,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0061</t>
+          <t>0268</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3252,7 +3252,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>0065</t>
+          <t>0269</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3298,7 +3298,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0059</t>
+          <t>0270</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3344,7 +3344,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0058</t>
+          <t>0271</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3390,7 +3390,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0057</t>
+          <t>0272</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3436,7 +3436,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0056</t>
+          <t>0273</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3482,7 +3482,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0055</t>
+          <t>0274</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3528,7 +3528,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0054</t>
+          <t>0275</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3574,7 +3574,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0053</t>
+          <t>0276</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -3620,7 +3620,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0052</t>
+          <t>0277</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -3666,7 +3666,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>0051</t>
+          <t>0278</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3712,7 +3712,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0060</t>
+          <t>0279</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -3758,7 +3758,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0087</t>
+          <t>0280</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3804,7 +3804,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0088</t>
+          <t>0281</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3850,7 +3850,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0089</t>
+          <t>0282</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3896,7 +3896,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>0090</t>
+          <t>0283</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3942,7 +3942,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0091</t>
+          <t>0284</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3988,7 +3988,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>0096</t>
+          <t>0285</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -4034,7 +4034,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0093</t>
+          <t>0286</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -4080,7 +4080,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0094</t>
+          <t>0287</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -4126,7 +4126,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0095</t>
+          <t>0288</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -4168,7 +4168,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>0097</t>
+          <t>0289</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -4214,7 +4214,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>0086</t>
+          <t>0290</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -4260,7 +4260,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0092</t>
+          <t>0291</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -4306,7 +4306,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0085</t>
+          <t>0292</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -4352,7 +4352,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0207</t>
+          <t>0293</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -4394,7 +4394,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0083</t>
+          <t>0294</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -4440,7 +4440,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0084</t>
+          <t>0295</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -4486,7 +4486,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>0072</t>
+          <t>0296</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -4532,7 +4532,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>0073</t>
+          <t>0297</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -4578,7 +4578,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0075</t>
+          <t>0298</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -4624,7 +4624,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>0076</t>
+          <t>0299</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -4670,7 +4670,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>0074</t>
+          <t>0300</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -4716,7 +4716,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>0078</t>
+          <t>0301</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -4762,7 +4762,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0079</t>
+          <t>0302</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -4808,7 +4808,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0080</t>
+          <t>0303</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -4854,7 +4854,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>0081</t>
+          <t>0304</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -4900,7 +4900,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0082</t>
+          <t>0305</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -4946,7 +4946,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0077</t>
+          <t>0306</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -4992,7 +4992,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0107</t>
+          <t>0307</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -5038,7 +5038,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>0112</t>
+          <t>0308</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -5084,7 +5084,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>0111</t>
+          <t>0309</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -5130,7 +5130,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>0110</t>
+          <t>0310</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -5176,7 +5176,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>0109</t>
+          <t>0311</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -5222,7 +5222,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>0108</t>
+          <t>0312</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -5268,7 +5268,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>0106</t>
+          <t>0313</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -5314,7 +5314,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>0104</t>
+          <t>0314</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -5360,7 +5360,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>0103</t>
+          <t>0315</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -5406,7 +5406,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>0102</t>
+          <t>0316</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -5452,7 +5452,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>0101</t>
+          <t>0317</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -5498,7 +5498,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>0100</t>
+          <t>0318</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -5544,7 +5544,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>0099</t>
+          <t>0319</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -5590,7 +5590,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>0105</t>
+          <t>0320</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -5636,7 +5636,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>0098</t>
+          <t>0321</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -5682,7 +5682,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>0129</t>
+          <t>0322</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -5728,7 +5728,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>0130</t>
+          <t>0323</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -5774,7 +5774,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>0128</t>
+          <t>0324</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -5820,7 +5820,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>0126</t>
+          <t>0325</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -5866,7 +5866,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>0125</t>
+          <t>0326</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -5912,7 +5912,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>0124</t>
+          <t>0327</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -5958,7 +5958,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>0123</t>
+          <t>0328</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -6004,7 +6004,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>0122</t>
+          <t>0329</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -6050,7 +6050,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>0127</t>
+          <t>0330</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -6096,7 +6096,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>0120</t>
+          <t>0331</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -6142,7 +6142,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>0119</t>
+          <t>0332</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -6188,7 +6188,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>0118</t>
+          <t>0333</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -6234,7 +6234,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>0117</t>
+          <t>0334</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -6280,7 +6280,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>0116</t>
+          <t>0335</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -6326,7 +6326,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>0115</t>
+          <t>0336</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -6368,7 +6368,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>0113</t>
+          <t>0337</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -6414,7 +6414,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>0114</t>
+          <t>0338</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -6460,7 +6460,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>0121</t>
+          <t>0339</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -6506,7 +6506,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>0144</t>
+          <t>0340</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -6552,7 +6552,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>0143</t>
+          <t>0341</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -6598,7 +6598,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>0142</t>
+          <t>0342</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -6644,7 +6644,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0141</t>
+          <t>0343</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -6690,7 +6690,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>0140</t>
+          <t>0344</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -6736,7 +6736,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>0139</t>
+          <t>0345</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -6782,7 +6782,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>0135</t>
+          <t>0346</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -6828,7 +6828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>0137</t>
+          <t>0347</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -6874,7 +6874,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0136</t>
+          <t>0348</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -6920,7 +6920,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>0134</t>
+          <t>0349</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -6966,7 +6966,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>0133</t>
+          <t>0350</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -7012,7 +7012,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0132</t>
+          <t>0351</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -7058,7 +7058,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>0131</t>
+          <t>0352</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -7104,7 +7104,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>0138</t>
+          <t>0353</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -7150,7 +7150,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>0156</t>
+          <t>0354</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -7196,7 +7196,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>0158</t>
+          <t>0355</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -7242,7 +7242,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>0157</t>
+          <t>0356</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -7288,7 +7288,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>0160</t>
+          <t>0357</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -7334,7 +7334,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>0155</t>
+          <t>0358</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -7380,7 +7380,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>0159</t>
+          <t>0359</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -7426,7 +7426,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>0154</t>
+          <t>0360</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -7472,7 +7472,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>0146</t>
+          <t>0361</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -7518,7 +7518,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>0152</t>
+          <t>0362</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -7564,7 +7564,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>0145</t>
+          <t>0363</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -7610,7 +7610,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>0147</t>
+          <t>0364</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -7656,7 +7656,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>0148</t>
+          <t>0365</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -7702,7 +7702,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>0153</t>
+          <t>0366</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -7748,7 +7748,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>0150</t>
+          <t>0367</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -7794,7 +7794,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>0151</t>
+          <t>0368</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -7840,7 +7840,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>0149</t>
+          <t>0369</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -7886,7 +7886,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>0171</t>
+          <t>0370</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -7932,7 +7932,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>0170</t>
+          <t>0371</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -7978,7 +7978,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>0168</t>
+          <t>0372</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -8024,7 +8024,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>0166</t>
+          <t>0373</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -8070,7 +8070,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>0169</t>
+          <t>0374</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -8116,7 +8116,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>0164</t>
+          <t>0375</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -8162,7 +8162,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>0163</t>
+          <t>0376</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -8208,7 +8208,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>0162</t>
+          <t>0377</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -8254,7 +8254,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>0161</t>
+          <t>0378</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -8300,7 +8300,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>0165</t>
+          <t>0379</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -8346,7 +8346,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>0167</t>
+          <t>0380</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -8392,7 +8392,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>0182</t>
+          <t>0381</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -8438,7 +8438,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>0189</t>
+          <t>0382</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -8484,7 +8484,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>0188</t>
+          <t>0383</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -8530,7 +8530,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>0187</t>
+          <t>0384</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -8576,7 +8576,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>0186</t>
+          <t>0385</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -8622,7 +8622,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>0185</t>
+          <t>0386</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -8668,7 +8668,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>0184</t>
+          <t>0387</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -8714,7 +8714,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>0183</t>
+          <t>0388</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -8760,7 +8760,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>0389</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -8806,7 +8806,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>0179</t>
+          <t>0390</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -8852,7 +8852,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>0178</t>
+          <t>0391</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -8898,7 +8898,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>0177</t>
+          <t>0392</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -8944,7 +8944,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>0176</t>
+          <t>0393</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -8990,7 +8990,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>0175</t>
+          <t>0394</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -9036,7 +9036,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>0174</t>
+          <t>0395</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -9082,7 +9082,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>0173</t>
+          <t>0396</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -9128,7 +9128,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>0172</t>
+          <t>0397</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -9174,7 +9174,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>0181</t>
+          <t>0398</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -9220,7 +9220,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>0205</t>
+          <t>0399</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -9266,7 +9266,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>0204</t>
+          <t>0400</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -9312,7 +9312,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>0203</t>
+          <t>0401</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -9358,7 +9358,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>0202</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -9404,7 +9404,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>0403</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -9450,7 +9450,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>0200</t>
+          <t>0404</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -9496,7 +9496,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>0199</t>
+          <t>0405</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -9542,7 +9542,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>0194</t>
+          <t>0406</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -9588,7 +9588,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>0197</t>
+          <t>0407</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -9634,7 +9634,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>0196</t>
+          <t>0408</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -9680,7 +9680,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>0195</t>
+          <t>0409</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -9726,7 +9726,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>0193</t>
+          <t>0410</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -9772,7 +9772,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>0192</t>
+          <t>0411</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -9818,7 +9818,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>0191</t>
+          <t>0412</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -9864,7 +9864,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>0190</t>
+          <t>0413</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -9910,7 +9910,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>0198</t>
+          <t>0414</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -9956,7 +9956,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>0206</t>
+          <t>0415</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -10002,7 +10002,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>0208</t>
+          <t>0416</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -10015,14 +10015,14 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E209" s="2" t="n">
-        <v>45877</v>
+        <v>45882</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45889</v>
+        <v>45887</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>test uid 209</t>
+          <t>test uid not 208</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 19:33:47
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10015,14 +10015,14 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E209" s="2" t="n">
         <v>45882</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45889</v>
+        <v>45883</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -10031,7 +10031,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>209</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 19:50:39
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10044,7 +10044,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>0209</t>
+          <t>0210</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -10057,14 +10057,14 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E210" s="2" t="n">
-        <v>45882</v>
+        <v>45887</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45889</v>
+        <v>45888</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>210</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 19:56:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0001</t>
+          <t>0211</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0025</t>
+          <t>0212</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0024</t>
+          <t>0213</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -630,7 +630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0023</t>
+          <t>0214</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0022</t>
+          <t>0215</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0021</t>
+          <t>0216</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0020</t>
+          <t>0217</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -814,7 +814,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0019</t>
+          <t>0218</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -860,7 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0018</t>
+          <t>0219</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -906,7 +906,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0017</t>
+          <t>0220</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0015</t>
+          <t>0221</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -998,7 +998,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0014</t>
+          <t>0222</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1044,7 +1044,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0016</t>
+          <t>0223</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1090,7 +1090,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0012</t>
+          <t>0224</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1136,7 +1136,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0002</t>
+          <t>0225</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1182,7 +1182,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0003</t>
+          <t>0226</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1228,7 +1228,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0004</t>
+          <t>0227</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1274,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0013</t>
+          <t>0228</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1320,7 +1320,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0006</t>
+          <t>0229</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0005</t>
+          <t>0230</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1412,7 +1412,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0008</t>
+          <t>0231</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1458,7 +1458,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0009</t>
+          <t>0232</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1504,7 +1504,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0010</t>
+          <t>0233</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1550,7 +1550,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0011</t>
+          <t>0234</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1596,7 +1596,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0007</t>
+          <t>0235</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1642,7 +1642,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0034</t>
+          <t>0236</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1688,7 +1688,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0038</t>
+          <t>0237</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1734,7 +1734,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0037</t>
+          <t>0238</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1780,7 +1780,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0036</t>
+          <t>0239</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1826,7 +1826,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0035</t>
+          <t>0240</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1872,7 +1872,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0033</t>
+          <t>0241</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1918,7 +1918,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0030</t>
+          <t>0242</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1964,7 +1964,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0031</t>
+          <t>0243</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2010,7 +2010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0029</t>
+          <t>0244</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2056,7 +2056,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>0028</t>
+          <t>0245</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2102,7 +2102,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0027</t>
+          <t>0246</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2148,7 +2148,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0026</t>
+          <t>0247</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2194,7 +2194,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0032</t>
+          <t>0248</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2240,7 +2240,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>0050</t>
+          <t>0249</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2286,7 +2286,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0049</t>
+          <t>0250</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2332,7 +2332,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0048</t>
+          <t>0251</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2378,7 +2378,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0047</t>
+          <t>0252</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2424,7 +2424,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0045</t>
+          <t>0253</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2470,7 +2470,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0046</t>
+          <t>0254</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2516,7 +2516,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0043</t>
+          <t>0255</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2562,7 +2562,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>0042</t>
+          <t>0256</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2608,7 +2608,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0041</t>
+          <t>0257</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2654,7 +2654,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0040</t>
+          <t>0258</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2700,7 +2700,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0039</t>
+          <t>0259</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2746,7 +2746,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0044</t>
+          <t>0260</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2792,7 +2792,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0063</t>
+          <t>0261</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2838,7 +2838,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0071</t>
+          <t>0262</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2884,7 +2884,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0070</t>
+          <t>0263</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2930,7 +2930,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0069</t>
+          <t>0264</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2976,7 +2976,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0068</t>
+          <t>0265</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -3022,7 +3022,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0067</t>
+          <t>0266</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -3068,7 +3068,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0066</t>
+          <t>0267</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3114,7 +3114,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0065</t>
+          <t>0268</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -3160,7 +3160,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0064</t>
+          <t>0269</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3206,7 +3206,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0062</t>
+          <t>0270</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3252,7 +3252,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>0053</t>
+          <t>0271</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3298,7 +3298,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0060</t>
+          <t>0272</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3344,7 +3344,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0059</t>
+          <t>0273</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3390,7 +3390,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0058</t>
+          <t>0274</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3436,7 +3436,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0057</t>
+          <t>0275</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3482,7 +3482,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0056</t>
+          <t>0276</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3528,7 +3528,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0055</t>
+          <t>0277</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3574,7 +3574,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0054</t>
+          <t>0278</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -3620,7 +3620,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0052</t>
+          <t>0279</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -3666,7 +3666,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>0051</t>
+          <t>0280</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3712,7 +3712,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0061</t>
+          <t>0281</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -3758,7 +3758,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0087</t>
+          <t>0282</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3804,7 +3804,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0088</t>
+          <t>0283</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3850,7 +3850,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0089</t>
+          <t>0284</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3896,7 +3896,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>0090</t>
+          <t>0285</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3942,7 +3942,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0091</t>
+          <t>0286</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3988,7 +3988,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>0096</t>
+          <t>0287</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -4034,7 +4034,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0093</t>
+          <t>0288</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -4080,7 +4080,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0094</t>
+          <t>0289</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -4126,7 +4126,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0095</t>
+          <t>0290</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -4172,7 +4172,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>0097</t>
+          <t>0291</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -4218,7 +4218,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>0098</t>
+          <t>0292</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -4264,7 +4264,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0092</t>
+          <t>0293</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -4310,7 +4310,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0086</t>
+          <t>0294</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -4356,7 +4356,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0083</t>
+          <t>0295</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -4402,7 +4402,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0084</t>
+          <t>0296</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -4448,7 +4448,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0072</t>
+          <t>0297</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -4494,7 +4494,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>0073</t>
+          <t>0298</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -4540,7 +4540,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>0085</t>
+          <t>0299</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -4586,7 +4586,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0075</t>
+          <t>0300</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -4632,7 +4632,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>0076</t>
+          <t>0301</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -4678,7 +4678,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>0074</t>
+          <t>0302</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -4720,7 +4720,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>0078</t>
+          <t>0303</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -4766,7 +4766,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0079</t>
+          <t>0304</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -4812,7 +4812,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0080</t>
+          <t>0305</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -4854,7 +4854,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>0081</t>
+          <t>0306</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -4900,7 +4900,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0082</t>
+          <t>0307</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -4946,7 +4946,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0077</t>
+          <t>0308</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -4992,7 +4992,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0108</t>
+          <t>0309</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -5038,7 +5038,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>0113</t>
+          <t>0310</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -5084,7 +5084,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>0112</t>
+          <t>0311</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -5130,7 +5130,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>0111</t>
+          <t>0312</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -5176,7 +5176,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>0110</t>
+          <t>0313</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -5222,7 +5222,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>0109</t>
+          <t>0314</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -5268,7 +5268,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>0107</t>
+          <t>0315</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -5314,7 +5314,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>0104</t>
+          <t>0316</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -5360,7 +5360,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>0105</t>
+          <t>0317</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -5406,7 +5406,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>0106</t>
+          <t>0318</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -5452,7 +5452,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>0103</t>
+          <t>0319</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -5498,7 +5498,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>0102</t>
+          <t>0320</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -5544,7 +5544,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>0101</t>
+          <t>0321</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -5590,7 +5590,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>0100</t>
+          <t>0322</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -5636,7 +5636,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>0099</t>
+          <t>0323</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -5682,7 +5682,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>0131</t>
+          <t>0324</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -5728,7 +5728,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>0130</t>
+          <t>0325</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -5774,7 +5774,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>0129</t>
+          <t>0326</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -5820,7 +5820,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>0128</t>
+          <t>0327</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -5866,7 +5866,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>0127</t>
+          <t>0328</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -5908,7 +5908,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>0126</t>
+          <t>0329</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -5954,7 +5954,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>0125</t>
+          <t>0330</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -6000,7 +6000,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>0124</t>
+          <t>0331</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -6046,7 +6046,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>0123</t>
+          <t>0332</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -6092,7 +6092,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>0208</t>
+          <t>0333</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -6134,7 +6134,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>0121</t>
+          <t>0334</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -6180,7 +6180,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>0120</t>
+          <t>0335</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -6226,7 +6226,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>0119</t>
+          <t>0336</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -6272,7 +6272,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>0118</t>
+          <t>0337</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -6318,7 +6318,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>0117</t>
+          <t>0338</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -6364,7 +6364,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>0116</t>
+          <t>0339</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -6410,7 +6410,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>0115</t>
+          <t>0340</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -6456,7 +6456,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>0114</t>
+          <t>0341</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -6502,7 +6502,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>0122</t>
+          <t>0342</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -6548,7 +6548,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>0145</t>
+          <t>0343</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -6594,7 +6594,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>0144</t>
+          <t>0344</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -6640,7 +6640,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0143</t>
+          <t>0345</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -6686,7 +6686,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>0142</t>
+          <t>0346</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -6732,7 +6732,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>0141</t>
+          <t>0347</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -6778,7 +6778,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>0140</t>
+          <t>0348</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -6824,7 +6824,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>0138</t>
+          <t>0349</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -6870,7 +6870,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0137</t>
+          <t>0350</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -6916,7 +6916,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>0136</t>
+          <t>0351</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -6962,7 +6962,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>0135</t>
+          <t>0352</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -7008,7 +7008,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0134</t>
+          <t>0353</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -7054,7 +7054,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>0133</t>
+          <t>0354</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -7100,7 +7100,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>0132</t>
+          <t>0355</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -7146,7 +7146,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>0139</t>
+          <t>0356</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -7192,7 +7192,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>0155</t>
+          <t>0357</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -7238,7 +7238,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>0161</t>
+          <t>0358</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -7284,7 +7284,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>0160</t>
+          <t>0359</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -7330,7 +7330,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>0159</t>
+          <t>0360</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -7376,7 +7376,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>0158</t>
+          <t>0361</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -7422,7 +7422,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>0156</t>
+          <t>0362</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -7468,7 +7468,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>0154</t>
+          <t>0363</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -7514,7 +7514,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>0157</t>
+          <t>0364</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -7560,7 +7560,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>0152</t>
+          <t>0365</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -7606,7 +7606,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>0151</t>
+          <t>0366</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -7652,7 +7652,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>0153</t>
+          <t>0367</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -7698,7 +7698,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>0150</t>
+          <t>0368</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -7744,7 +7744,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>0149</t>
+          <t>0369</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -7790,7 +7790,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>0148</t>
+          <t>0370</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -7836,7 +7836,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>0147</t>
+          <t>0371</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -7882,7 +7882,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>0146</t>
+          <t>0372</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -7928,7 +7928,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>0172</t>
+          <t>0373</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -7974,7 +7974,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>0171</t>
+          <t>0374</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -8020,7 +8020,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>0170</t>
+          <t>0375</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -8066,7 +8066,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>0169</t>
+          <t>0376</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -8112,7 +8112,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>0168</t>
+          <t>0377</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -8158,7 +8158,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>0166</t>
+          <t>0378</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -8204,7 +8204,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>0165</t>
+          <t>0379</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -8250,7 +8250,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>0164</t>
+          <t>0380</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -8296,7 +8296,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>0163</t>
+          <t>0381</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -8342,7 +8342,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>0162</t>
+          <t>0382</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -8388,7 +8388,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>0167</t>
+          <t>0383</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -8434,7 +8434,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>0190</t>
+          <t>0384</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -8480,7 +8480,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>0189</t>
+          <t>0385</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -8526,7 +8526,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>0187</t>
+          <t>0386</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -8572,7 +8572,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>0186</t>
+          <t>0387</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -8618,7 +8618,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>0185</t>
+          <t>0388</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -8664,7 +8664,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>0184</t>
+          <t>0389</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -8710,7 +8710,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>0183</t>
+          <t>0390</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -8756,7 +8756,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>0182</t>
+          <t>0391</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -8802,7 +8802,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>0188</t>
+          <t>0392</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -8848,7 +8848,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>0180</t>
+          <t>0393</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -8894,7 +8894,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>0173</t>
+          <t>0394</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -8940,7 +8940,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>0174</t>
+          <t>0395</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -8986,7 +8986,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>0175</t>
+          <t>0396</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -9032,7 +9032,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>0181</t>
+          <t>0397</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -9078,7 +9078,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>0177</t>
+          <t>0398</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -9124,7 +9124,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>0178</t>
+          <t>0399</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -9170,7 +9170,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>0179</t>
+          <t>0400</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -9216,7 +9216,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>0176</t>
+          <t>0401</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -9262,7 +9262,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>0206</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -9308,7 +9308,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>0205</t>
+          <t>0403</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -9354,7 +9354,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>0204</t>
+          <t>0404</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -9400,7 +9400,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>0203</t>
+          <t>0405</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -9446,7 +9446,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>0202</t>
+          <t>0406</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -9492,7 +9492,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>0201</t>
+          <t>0407</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -9538,7 +9538,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>0200</t>
+          <t>0408</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -9584,7 +9584,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>0198</t>
+          <t>0409</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -9630,7 +9630,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>0197</t>
+          <t>0410</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -9676,7 +9676,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>0196</t>
+          <t>0411</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -9722,7 +9722,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>0207</t>
+          <t>0412</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -9768,7 +9768,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>0194</t>
+          <t>0413</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -9814,7 +9814,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>0193</t>
+          <t>0414</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -9860,7 +9860,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>0192</t>
+          <t>0415</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -9906,7 +9906,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>0191</t>
+          <t>0416</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -9952,7 +9952,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>0199</t>
+          <t>0417</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -9998,7 +9998,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>0195</t>
+          <t>0418</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -10044,7 +10044,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>0210</t>
+          <t>0419</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -10057,14 +10057,14 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E210" s="2" t="n">
-        <v>45887</v>
+        <v>45882</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45888</v>
+        <v>45889</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 20:07:56
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0211</t>
+          <t>0210</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0212</t>
+          <t>0211</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -584,7 +584,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0213</t>
+          <t>0212</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -630,7 +630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0214</t>
+          <t>0213</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0215</t>
+          <t>0214</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -722,7 +722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0216</t>
+          <t>0215</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -768,7 +768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0217</t>
+          <t>0216</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -814,7 +814,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0218</t>
+          <t>0217</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -860,7 +860,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0219</t>
+          <t>0218</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -906,7 +906,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0220</t>
+          <t>0219</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0221</t>
+          <t>0220</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -998,7 +998,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0222</t>
+          <t>0221</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1044,7 +1044,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0223</t>
+          <t>0222</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1090,7 +1090,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0224</t>
+          <t>0223</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1136,7 +1136,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0225</t>
+          <t>0224</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1182,7 +1182,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0226</t>
+          <t>0225</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1228,7 +1228,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0227</t>
+          <t>0226</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1274,7 +1274,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0228</t>
+          <t>0227</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1320,7 +1320,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0229</t>
+          <t>0228</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1366,7 +1366,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0230</t>
+          <t>0229</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1412,7 +1412,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0231</t>
+          <t>0230</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1458,7 +1458,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0232</t>
+          <t>0231</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1504,7 +1504,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0233</t>
+          <t>0232</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1550,7 +1550,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0234</t>
+          <t>0233</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1596,7 +1596,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0235</t>
+          <t>0234</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1642,7 +1642,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0236</t>
+          <t>0235</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1688,7 +1688,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0237</t>
+          <t>0236</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1734,7 +1734,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0238</t>
+          <t>0237</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1780,7 +1780,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0239</t>
+          <t>0238</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1826,7 +1826,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0240</t>
+          <t>0239</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1872,7 +1872,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0241</t>
+          <t>0240</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1918,7 +1918,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0242</t>
+          <t>0241</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1964,7 +1964,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0243</t>
+          <t>0242</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2010,7 +2010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0244</t>
+          <t>0243</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2056,7 +2056,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>0245</t>
+          <t>0244</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2102,7 +2102,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0246</t>
+          <t>0245</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2148,7 +2148,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0247</t>
+          <t>0246</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2194,7 +2194,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0248</t>
+          <t>0247</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2240,7 +2240,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>0249</t>
+          <t>0248</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2286,7 +2286,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0250</t>
+          <t>0249</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2332,7 +2332,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0251</t>
+          <t>0250</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2378,7 +2378,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0252</t>
+          <t>0251</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2424,7 +2424,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0253</t>
+          <t>0252</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2470,7 +2470,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0254</t>
+          <t>0253</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2516,7 +2516,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0255</t>
+          <t>0254</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2562,7 +2562,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>0256</t>
+          <t>0255</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2608,7 +2608,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0257</t>
+          <t>0256</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2654,7 +2654,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0258</t>
+          <t>0257</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2700,7 +2700,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0259</t>
+          <t>0258</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2746,7 +2746,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0260</t>
+          <t>0259</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2792,7 +2792,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0261</t>
+          <t>0260</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2838,7 +2838,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0262</t>
+          <t>0261</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2884,7 +2884,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0263</t>
+          <t>0262</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2930,7 +2930,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0264</t>
+          <t>0263</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2976,7 +2976,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0265</t>
+          <t>0264</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -3022,7 +3022,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0266</t>
+          <t>0265</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -3068,7 +3068,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0267</t>
+          <t>0266</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3114,7 +3114,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0268</t>
+          <t>0267</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -3160,7 +3160,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0269</t>
+          <t>0268</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3206,7 +3206,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0270</t>
+          <t>0269</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3252,7 +3252,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>0271</t>
+          <t>0270</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3298,7 +3298,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0272</t>
+          <t>0271</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3344,7 +3344,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0273</t>
+          <t>0272</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3390,7 +3390,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0274</t>
+          <t>0273</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3436,7 +3436,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0275</t>
+          <t>0274</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3482,7 +3482,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0276</t>
+          <t>0275</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3528,7 +3528,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0277</t>
+          <t>0276</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3574,7 +3574,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0278</t>
+          <t>0277</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -3620,7 +3620,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0279</t>
+          <t>0278</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -3666,7 +3666,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>0280</t>
+          <t>0279</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3712,7 +3712,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0281</t>
+          <t>0280</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -3758,7 +3758,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0282</t>
+          <t>0281</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3804,7 +3804,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0283</t>
+          <t>0282</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3850,7 +3850,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0284</t>
+          <t>0283</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3896,7 +3896,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>0285</t>
+          <t>0284</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3942,7 +3942,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0286</t>
+          <t>0285</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3988,7 +3988,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>0287</t>
+          <t>0286</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -4034,7 +4034,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0288</t>
+          <t>0287</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -4080,7 +4080,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0289</t>
+          <t>0288</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -4126,7 +4126,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0290</t>
+          <t>0289</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -4172,7 +4172,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>0291</t>
+          <t>0290</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -4218,7 +4218,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>0292</t>
+          <t>0291</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -4264,7 +4264,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0293</t>
+          <t>0292</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -4310,7 +4310,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0294</t>
+          <t>0293</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -4356,7 +4356,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0295</t>
+          <t>0294</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -4402,7 +4402,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0296</t>
+          <t>0295</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -4448,7 +4448,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0297</t>
+          <t>0296</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -4494,7 +4494,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>0298</t>
+          <t>0297</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -4540,7 +4540,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>0299</t>
+          <t>0298</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -4586,7 +4586,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0300</t>
+          <t>0299</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -4632,7 +4632,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>0301</t>
+          <t>0300</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -4678,7 +4678,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>0302</t>
+          <t>0301</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -4720,7 +4720,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>0303</t>
+          <t>0302</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -4766,7 +4766,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0304</t>
+          <t>0303</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -4812,7 +4812,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0305</t>
+          <t>0304</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -4854,7 +4854,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>0306</t>
+          <t>0305</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -4900,7 +4900,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0307</t>
+          <t>0306</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -4946,7 +4946,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0308</t>
+          <t>0307</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -4992,7 +4992,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0309</t>
+          <t>0308</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -5038,7 +5038,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>0310</t>
+          <t>0309</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -5084,7 +5084,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>0311</t>
+          <t>0310</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -5130,7 +5130,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>0312</t>
+          <t>0311</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -5176,7 +5176,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>0313</t>
+          <t>0312</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -5222,7 +5222,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>0314</t>
+          <t>0313</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -5268,7 +5268,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>0315</t>
+          <t>0314</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -5314,7 +5314,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>0316</t>
+          <t>0315</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -5360,7 +5360,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>0317</t>
+          <t>0316</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -5406,7 +5406,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>0318</t>
+          <t>0317</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -5452,7 +5452,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>0319</t>
+          <t>0318</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -5498,7 +5498,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>0320</t>
+          <t>0319</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -5544,7 +5544,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>0321</t>
+          <t>0320</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -5590,7 +5590,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>0322</t>
+          <t>0321</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -5636,7 +5636,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>0323</t>
+          <t>0322</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -5682,7 +5682,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>0324</t>
+          <t>0323</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -5728,7 +5728,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>0325</t>
+          <t>0324</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -5774,7 +5774,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>0326</t>
+          <t>0325</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -5820,7 +5820,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>0327</t>
+          <t>0326</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -5866,7 +5866,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>0328</t>
+          <t>0327</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -5908,7 +5908,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>0329</t>
+          <t>0328</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -5954,7 +5954,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>0330</t>
+          <t>0329</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -6000,7 +6000,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>0331</t>
+          <t>0330</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -6046,7 +6046,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>0332</t>
+          <t>0331</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -6092,7 +6092,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>0333</t>
+          <t>0332</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -6134,7 +6134,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>0334</t>
+          <t>0333</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -6180,7 +6180,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>0335</t>
+          <t>0334</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -6226,7 +6226,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>0336</t>
+          <t>0335</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -6272,7 +6272,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>0337</t>
+          <t>0336</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -6318,7 +6318,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>0338</t>
+          <t>0337</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -6364,7 +6364,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>0339</t>
+          <t>0338</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -6410,7 +6410,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>0340</t>
+          <t>0339</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -6456,7 +6456,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>0341</t>
+          <t>0340</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -6502,7 +6502,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>0342</t>
+          <t>0341</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -6548,7 +6548,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>0343</t>
+          <t>0342</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -6594,7 +6594,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>0344</t>
+          <t>0343</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -6640,7 +6640,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0345</t>
+          <t>0344</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -6686,7 +6686,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>0346</t>
+          <t>0345</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -6732,7 +6732,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>0347</t>
+          <t>0346</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -6778,7 +6778,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>0348</t>
+          <t>0347</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -6824,7 +6824,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>0349</t>
+          <t>0348</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -6870,7 +6870,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0350</t>
+          <t>0349</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -6916,7 +6916,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>0351</t>
+          <t>0350</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -6962,7 +6962,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>0352</t>
+          <t>0351</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -7008,7 +7008,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>0353</t>
+          <t>0352</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -7054,7 +7054,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>0354</t>
+          <t>0353</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -7100,7 +7100,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>0355</t>
+          <t>0354</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -7146,7 +7146,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>0356</t>
+          <t>0355</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -7192,7 +7192,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>0357</t>
+          <t>0356</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -7238,7 +7238,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>0358</t>
+          <t>0357</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -7284,7 +7284,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>0359</t>
+          <t>0358</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -7330,7 +7330,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>0360</t>
+          <t>0359</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -7376,7 +7376,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>0361</t>
+          <t>0360</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -7422,7 +7422,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>0362</t>
+          <t>0361</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -7468,7 +7468,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>0363</t>
+          <t>0362</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -7514,7 +7514,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>0364</t>
+          <t>0363</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -7560,7 +7560,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>0365</t>
+          <t>0364</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -7606,7 +7606,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>0366</t>
+          <t>0365</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -7652,7 +7652,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>0367</t>
+          <t>0366</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -7698,7 +7698,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>0368</t>
+          <t>0367</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -7744,7 +7744,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>0369</t>
+          <t>0368</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -7790,7 +7790,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>0370</t>
+          <t>0369</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -7836,7 +7836,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>0371</t>
+          <t>0370</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -7882,7 +7882,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>0372</t>
+          <t>0371</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -7928,7 +7928,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>0373</t>
+          <t>0372</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -7974,7 +7974,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>0374</t>
+          <t>0373</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -8020,7 +8020,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>0375</t>
+          <t>0374</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -8066,7 +8066,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>0376</t>
+          <t>0375</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -8112,7 +8112,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>0377</t>
+          <t>0376</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -8158,7 +8158,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>0378</t>
+          <t>0377</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -8204,7 +8204,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>0379</t>
+          <t>0378</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -8250,7 +8250,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>0380</t>
+          <t>0379</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -8296,7 +8296,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>0381</t>
+          <t>0380</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -8342,7 +8342,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>0382</t>
+          <t>0381</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -8388,7 +8388,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>0383</t>
+          <t>0382</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -8434,7 +8434,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>0384</t>
+          <t>0383</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -8480,7 +8480,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>0385</t>
+          <t>0384</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -8526,7 +8526,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>0386</t>
+          <t>0385</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -8572,7 +8572,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>0387</t>
+          <t>0386</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -8618,7 +8618,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>0388</t>
+          <t>0387</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -8664,7 +8664,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>0389</t>
+          <t>0388</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -8710,7 +8710,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>0390</t>
+          <t>0389</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -8756,7 +8756,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>0391</t>
+          <t>0390</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -8802,7 +8802,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>0392</t>
+          <t>0391</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -8848,7 +8848,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>0393</t>
+          <t>0392</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -8894,7 +8894,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>0394</t>
+          <t>0393</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -8940,7 +8940,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>0395</t>
+          <t>0394</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -8986,7 +8986,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>0396</t>
+          <t>0395</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -9032,7 +9032,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>0397</t>
+          <t>0396</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -9078,7 +9078,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>0398</t>
+          <t>0397</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -9124,7 +9124,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>0399</t>
+          <t>0398</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -9170,7 +9170,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>0400</t>
+          <t>0399</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -9216,7 +9216,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>0401</t>
+          <t>0400</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -9262,7 +9262,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>0402</t>
+          <t>0401</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -9308,7 +9308,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>0403</t>
+          <t>0402</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -9354,7 +9354,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>0404</t>
+          <t>0403</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -9400,7 +9400,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>0405</t>
+          <t>0404</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -9446,7 +9446,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>0406</t>
+          <t>0405</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -9492,7 +9492,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>0407</t>
+          <t>0406</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -9538,7 +9538,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>0408</t>
+          <t>0407</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -9584,7 +9584,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>0409</t>
+          <t>0408</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -9630,7 +9630,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>0410</t>
+          <t>0409</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -9676,7 +9676,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>0411</t>
+          <t>0410</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -9722,7 +9722,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>0412</t>
+          <t>0411</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -9768,7 +9768,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>0413</t>
+          <t>0412</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -9814,7 +9814,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>0414</t>
+          <t>0413</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -9860,7 +9860,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>0415</t>
+          <t>0414</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -9906,7 +9906,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>0416</t>
+          <t>0415</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -9952,7 +9952,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>0417</t>
+          <t>0416</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -9998,7 +9998,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>0418</t>
+          <t>0417</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -10044,7 +10044,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>0419</t>
+          <t>0418</t>
         </is>
       </c>
       <c r="B210" t="n">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:07:14
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J207"/>
+  <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9545,6 +9545,46 @@
         </is>
       </c>
     </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>331</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E208" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="F208" s="2" t="n">
+        <v>45883</v>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:08:01
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9559,14 +9559,14 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E208" s="2" t="n">
         <v>45882</v>
       </c>
       <c r="F208" s="2" t="n">
-        <v>45883</v>
+        <v>45887</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -9575,7 +9575,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>207</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:09:12
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9585,6 +9585,46 @@
       </c>
       <c r="J208" t="inlineStr"/>
     </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>331</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E209" s="2" t="n">
+        <v>45882</v>
+      </c>
+      <c r="F209" s="2" t="n">
+        <v>45883</v>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:14:10
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9625,6 +9625,46 @@
       </c>
       <c r="J209" t="inlineStr"/>
     </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>331</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E210" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="F210" s="2" t="n">
+        <v>45885</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:17:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9643,10 +9643,10 @@
         </is>
       </c>
       <c r="E210" s="2" t="n">
-        <v>45884</v>
+        <v>45887</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45885</v>
+        <v>45887</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>209</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:18:41
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J210"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9665,6 +9665,42 @@
       </c>
       <c r="J210" t="inlineStr"/>
     </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>331</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E211" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="F211" s="2" t="n">
+        <v>45886</v>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr"/>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:19:20
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9693,13 +9693,57 @@
           <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="H211" t="inlineStr"/>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I211" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>331</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E212" s="2" t="n">
+        <v>45890</v>
+      </c>
+      <c r="F212" s="2" t="n">
+        <v>45891</v>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-13-2025 -> 08-14-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J212"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9603,10 +9603,10 @@
         </is>
       </c>
       <c r="E209" s="2" t="n">
-        <v>45882</v>
+        <v>45887</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45883</v>
+        <v>45887</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>209</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
@@ -9643,10 +9643,10 @@
         </is>
       </c>
       <c r="E210" s="2" t="n">
-        <v>45887</v>
+        <v>45884</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45887</v>
+        <v>45886</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -9683,10 +9683,10 @@
         </is>
       </c>
       <c r="E211" s="2" t="n">
-        <v>45884</v>
+        <v>45890</v>
       </c>
       <c r="F211" s="2" t="n">
-        <v>45886</v>
+        <v>45891</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -9695,7 +9695,7 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>210</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
@@ -9704,46 +9704,6 @@
         </is>
       </c>
       <c r="J211" t="inlineStr"/>
-    </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>331</v>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E212" s="2" t="n">
-        <v>45890</v>
-      </c>
-      <c r="F212" s="2" t="n">
-        <v>45891</v>
-      </c>
-      <c r="G212" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="H212" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="I212" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J212" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-18-2025 -> 08-18-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9603,10 +9603,10 @@
         </is>
       </c>
       <c r="E209" s="2" t="n">
-        <v>45887</v>
+        <v>45884</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45887</v>
+        <v>45886</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
@@ -9643,10 +9643,10 @@
         </is>
       </c>
       <c r="E210" s="2" t="n">
-        <v>45884</v>
+        <v>45890</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45886</v>
+        <v>45891</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>210</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -9664,46 +9664,6 @@
         </is>
       </c>
       <c r="J210" t="inlineStr"/>
-    </row>
-    <row r="211">
-      <c r="A211" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="n">
-        <v>331</v>
-      </c>
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="D211" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E211" s="2" t="n">
-        <v>45890</v>
-      </c>
-      <c r="F211" s="2" t="n">
-        <v>45891</v>
-      </c>
-      <c r="G211" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="H211" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="I211" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J211" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-15-2025 -> 08-17-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J210"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9603,10 +9603,10 @@
         </is>
       </c>
       <c r="E209" s="2" t="n">
-        <v>45884</v>
+        <v>45890</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45886</v>
+        <v>45891</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>210</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
@@ -9624,46 +9624,6 @@
         </is>
       </c>
       <c r="J209" t="inlineStr"/>
-    </row>
-    <row r="210">
-      <c r="A210" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="n">
-        <v>331</v>
-      </c>
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="D210" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E210" s="2" t="n">
-        <v>45890</v>
-      </c>
-      <c r="F210" s="2" t="n">
-        <v>45891</v>
-      </c>
-      <c r="G210" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="H210" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="I210" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J210" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-13-2025 -> 08-18-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9559,14 +9559,14 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Reserved</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="E208" s="2" t="n">
-        <v>45882</v>
+        <v>45890</v>
       </c>
       <c r="F208" s="2" t="n">
-        <v>45887</v>
+        <v>45891</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -9575,7 +9575,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>210</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">
@@ -9584,46 +9584,6 @@
         </is>
       </c>
       <c r="J208" t="inlineStr"/>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="n">
-        <v>331</v>
-      </c>
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="D209" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E209" s="2" t="n">
-        <v>45890</v>
-      </c>
-      <c r="F209" s="2" t="n">
-        <v>45891</v>
-      </c>
-      <c r="G209" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="H209" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="I209" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J209" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted single entry: 331 - CF (08-21-2025 -> 08-22-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9545,46 +9545,6 @@
         </is>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>331</v>
-      </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>CF</t>
-        </is>
-      </c>
-      <c r="D208" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E208" s="2" t="n">
-        <v>45890</v>
-      </c>
-      <c r="F208" s="2" t="n">
-        <v>45891</v>
-      </c>
-      <c r="G208" t="inlineStr">
-        <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
-        </is>
-      </c>
-      <c r="H208" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
-      <c r="I208" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J208" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:44:44
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J207"/>
+  <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9545,6 +9545,46 @@
         </is>
       </c>
     </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>329</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Han sup Han</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E208" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="F208" s="2" t="n">
+        <v>45885</v>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>Class field trip (FOR 419) to view active logging operations and forest roads near Flagstaff, up to 4 people</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>['Han sup Han']</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:46:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9585,6 +9585,46 @@
       </c>
       <c r="J208" t="inlineStr"/>
     </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>329</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Han sup Han</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E209" s="2" t="n">
+        <v>45936</v>
+      </c>
+      <c r="F209" s="2" t="n">
+        <v>45937</v>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>Class field trip (FOR 419) to view active logging operations and forest roads near Flagstaff, up to 4 people</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>['Han sup Han']</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:48:19
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9625,6 +9625,46 @@
       </c>
       <c r="J209" t="inlineStr"/>
     </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>329</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Han sup Han</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E210" s="2" t="n">
+        <v>45950</v>
+      </c>
+      <c r="F210" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>Class field trip to view logging operations near Flagstaff, up to 4 people</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>['Han sup Han']</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:52:54
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J210"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9665,6 +9665,46 @@
       </c>
       <c r="J210" t="inlineStr"/>
     </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>329</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Han sup Han</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E211" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="F211" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>Field trip to view active logging operations near Flagstaff, up to 4 people</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>['Han sup Han']</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-13 21:54:21
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9705,6 +9705,46 @@
       </c>
       <c r="J211" t="inlineStr"/>
     </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>329</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Han sup Han</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E212" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="F212" s="2" t="n">
+        <v>45993</v>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>Class field trip to view biomass operations near Flagstaff, up to 4 people</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>['Han sup Han']</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-14 17:53:54
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J212"/>
+  <dimension ref="A1:J213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9745,6 +9745,46 @@
       </c>
       <c r="J212" t="inlineStr"/>
     </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>330</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Seafha Ramos</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E213" s="2" t="n">
+        <v>45884</v>
+      </c>
+      <c r="F213" s="2" t="n">
+        <v>45885</v>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>330 - 2024 Toyota Camry Hybrid, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>Using to attend meeting in Kykotsmovi Village, Hopi to discuss project directions.</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>['Destiny Sanderson', 'Seafha Ramos']</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-08-14 17:55:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9750,7 +9750,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -9770,7 +9770,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>330 - 2024 Toyota Camry Hybrid, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-19 00:51:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J213"/>
+  <dimension ref="A1:J214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9785,6 +9785,46 @@
       </c>
       <c r="J213" t="inlineStr"/>
     </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>329</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Azade Deljouei</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E214" s="2" t="n">
+        <v>45889</v>
+      </c>
+      <c r="F214" s="2" t="n">
+        <v>45890</v>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>I am going to visit the forest for the FOR-211 field lab visit with the previous instructor, Eric Olsen. The total number of occupants is three.</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>['Seyed Mohammad Moein Sadeghi']</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-20 20:43:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:J215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9825,6 +9825,46 @@
       </c>
       <c r="J214" t="inlineStr"/>
     </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>329</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E215" s="2" t="n">
+        <v>45897</v>
+      </c>
+      <c r="F215" s="2" t="n">
+        <v>45900</v>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>Payson, AZ, to install field equipment for research. The PI (Bryant) and one student will go down for 2 days. The field site is in a remote location and requires robust four wheel drive that can handle rocky terrain.</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>['Kelsey Bryant']</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-08-20 20:44:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -1698,7 +1698,7 @@
         <v>45855</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>45894</v>
+        <v>45900</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -3458,7 +3458,7 @@
         <v>45855</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>45894</v>
+        <v>45900</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-22 16:36:14
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J215"/>
+  <dimension ref="A1:J216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9865,6 +9865,46 @@
       </c>
       <c r="J215" t="inlineStr"/>
     </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>332</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Salli Dymond</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E216" s="2" t="n">
+        <v>45897</v>
+      </c>
+      <c r="F216" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Data collection and sensor maintenance. My destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Logan Ozmet and Jaime Ortega).</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>['Jamie Ortega', 'Logan Ozmet']</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-08-23 23:27:44
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J216"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9905,6 +9905,48 @@
       </c>
       <c r="J216" t="inlineStr"/>
     </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>332</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Reserved</t>
+        </is>
+      </c>
+      <c r="E217" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="F217" s="2" t="n">
+        <v>45940</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>Intended use: Aspen field works around Arizona
+Destination: Flagstaff RD and Kaibab RD
+No. of occupants: 2 to 3</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>['Kristen Waring', 'Jackson Bledsoe', 'Julia Totty', 'Elsa Kauffman', 'Abiral Acharya']</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted single entry: 332 - Salli Dymond (08-28-2025 -> 08-30-2025)
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:J216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9874,19 +9874,19 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="E216" s="2" t="n">
-        <v>45897</v>
+        <v>45903</v>
       </c>
       <c r="F216" s="2" t="n">
-        <v>45899</v>
+        <v>45940</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -9894,58 +9894,18 @@
         </is>
       </c>
       <c r="H216" t="inlineStr">
-        <is>
-          <t>Data collection and sensor maintenance. My destination trip is Tonto NF near Payson, AZ. Two occupants will be in the vehicle (Logan Ozmet and Jaime Ortega).</t>
-        </is>
-      </c>
-      <c r="I216" t="inlineStr">
-        <is>
-          <t>['Jamie Ortega', 'Logan Ozmet']</t>
-        </is>
-      </c>
-      <c r="J216" t="inlineStr"/>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="n">
-        <v>332</v>
-      </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>Kristen Waring</t>
-        </is>
-      </c>
-      <c r="D217" t="inlineStr">
-        <is>
-          <t>Reserved</t>
-        </is>
-      </c>
-      <c r="E217" s="2" t="n">
-        <v>45903</v>
-      </c>
-      <c r="F217" s="2" t="n">
-        <v>45940</v>
-      </c>
-      <c r="G217" t="inlineStr">
-        <is>
-          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
-        </is>
-      </c>
-      <c r="H217" t="inlineStr">
         <is>
           <t>Intended use: Aspen field works around Arizona
 Destination: Flagstaff RD and Kaibab RD
 No. of occupants: 2 to 3</t>
         </is>
       </c>
-      <c r="I217" t="inlineStr">
+      <c r="I216" t="inlineStr">
         <is>
           <t>['Kristen Waring', 'Jackson Bledsoe', 'Julia Totty', 'Elsa Kauffman', 'Abiral Acharya']</t>
         </is>
       </c>
-      <c r="J217" t="inlineStr"/>
+      <c r="J216" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-02 22:28:19
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J216"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9907,6 +9907,42 @@
       </c>
       <c r="J216" t="inlineStr"/>
     </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>331</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E217" s="2" t="n">
+        <v>45902</v>
+      </c>
+      <c r="F217" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr"/>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-03 22:47:11
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9935,13 +9935,57 @@
           <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="H217" t="inlineStr"/>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I217" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>330</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Seafha Ramos</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E218" s="2" t="n">
+        <v>45906</v>
+      </c>
+      <c r="F218" s="2" t="n">
+        <v>45924</v>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>330 - 2024 Toyota Camry Hybrid, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Speedchart 1680013C16 </t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 14:53:40
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J218"/>
+  <dimension ref="A1:J219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9987,6 +9987,42 @@
       </c>
       <c r="J218" t="inlineStr"/>
     </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>325</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E219" s="2" t="n">
+        <v>45905</v>
+      </c>
+      <c r="F219" s="2" t="n">
+        <v>46006</v>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr"/>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 18:53:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9570,7 +9570,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -9610,7 +9610,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -9690,7 +9690,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -9730,7 +9730,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -10015,7 +10015,11 @@
           <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
-      <c r="H219" t="inlineStr"/>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I219" t="inlineStr">
         <is>
           <t>[]</t>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 18:57:01
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9550,7 +9550,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C208" t="inlineStr">
         <is>
@@ -9590,7 +9590,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C209" t="inlineStr">
         <is>
@@ -9630,7 +9630,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C210" t="inlineStr">
         <is>
@@ -9670,7 +9670,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C211" t="inlineStr">
         <is>
@@ -9710,7 +9710,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C212" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 19:00:38
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J219"/>
+  <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10027,6 +10027,42 @@
       </c>
       <c r="J219" t="inlineStr"/>
     </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>321</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>OUT OF COMMISION</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E220" s="2" t="n">
+        <v>45904</v>
+      </c>
+      <c r="F220" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr"/>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 19:19:07
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10022,7 +10022,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>Alyssa Sanderson, Sophia Czosek</t>
         </is>
       </c>
       <c r="J219" t="inlineStr"/>
@@ -10055,7 +10055,11 @@
           <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
-      <c r="H220" t="inlineStr"/>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I220" t="inlineStr">
         <is>
           <t>[]</t>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 19:24:35
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9590,7 +9590,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="C209" t="inlineStr">
         <is>
@@ -9610,7 +9610,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:25:08
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J220"/>
+  <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10067,6 +10067,42 @@
       </c>
       <c r="J220" t="inlineStr"/>
     </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>466</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E221" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="F221" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr"/>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:25:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J221"/>
+  <dimension ref="A1:J222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10095,13 +10095,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H221" t="inlineStr"/>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I221" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>466</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E222" s="2" t="n">
+        <v>45916</v>
+      </c>
+      <c r="F222" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr"/>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:27:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J222"/>
+  <dimension ref="A1:J223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10135,13 +10135,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H222" t="inlineStr"/>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I222" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>466</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E223" s="2" t="n">
+        <v>45923</v>
+      </c>
+      <c r="F223" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr"/>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:28:33
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J223"/>
+  <dimension ref="A1:J224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10175,13 +10175,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H223" t="inlineStr"/>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I223" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>466</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E224" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="F224" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr"/>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 20:29:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -3370,7 +3370,7 @@
         <v>45545</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>45547</v>
+        <v>45548</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -10088,7 +10088,7 @@
         <v>45909</v>
       </c>
       <c r="F221" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="G221" t="inlineStr">
         <is>
@@ -10128,7 +10128,7 @@
         <v>45916</v>
       </c>
       <c r="F222" s="2" t="n">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="G222" t="inlineStr">
         <is>
@@ -10168,7 +10168,7 @@
         <v>45923</v>
       </c>
       <c r="F223" s="2" t="n">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="G223" t="inlineStr">
         <is>
@@ -10208,14 +10208,18 @@
         <v>45930</v>
       </c>
       <c r="F224" s="2" t="n">
-        <v>45932</v>
+        <v>45933</v>
       </c>
       <c r="G224" t="inlineStr">
         <is>
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H224" t="inlineStr"/>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I224" t="inlineStr">
         <is>
           <t>[]</t>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:30:59
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J224"/>
+  <dimension ref="A1:J225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10227,6 +10227,42 @@
       </c>
       <c r="J224" t="inlineStr"/>
     </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>466</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E225" s="2" t="n">
+        <v>45937</v>
+      </c>
+      <c r="F225" s="2" t="n">
+        <v>45940</v>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr"/>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:31:31
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J225"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10255,13 +10255,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H225" t="inlineStr"/>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I225" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>466</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E226" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="F226" s="2" t="n">
+        <v>45947</v>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr"/>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:32:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J226"/>
+  <dimension ref="A1:J227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10295,13 +10295,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H226" t="inlineStr"/>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I226" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>466</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E227" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="F227" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr"/>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J227" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:32:28
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J227"/>
+  <dimension ref="A1:J228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10335,13 +10335,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H227" t="inlineStr"/>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I227" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>466</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E228" s="2" t="n">
+        <v>45958</v>
+      </c>
+      <c r="F228" s="2" t="n">
+        <v>45961</v>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr"/>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J228" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:33:34
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J228"/>
+  <dimension ref="A1:J229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10375,13 +10375,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H228" t="inlineStr"/>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I228" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>466</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Derek Uhey</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E229" s="2" t="n">
+        <v>45965</v>
+      </c>
+      <c r="F229" s="2" t="n">
+        <v>45968</v>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr"/>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J229" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:50:49
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J229"/>
+  <dimension ref="A1:J230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10415,13 +10415,53 @@
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="H229" t="inlineStr"/>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I229" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>329</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E230" s="2" t="n">
+        <v>45915</v>
+      </c>
+      <c r="F230" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr"/>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>['Elsa Kauffman', 'Bear Murillo', 'Jackson Bledsoe']</t>
+        </is>
+      </c>
+      <c r="J230" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-04 20:52:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10448,14 +10448,18 @@
         <v>45915</v>
       </c>
       <c r="F230" s="2" t="n">
-        <v>45917</v>
+        <v>45918</v>
       </c>
       <c r="G230" t="inlineStr">
         <is>
           <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
-      <c r="H230" t="inlineStr"/>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I230" t="inlineStr">
         <is>
           <t>['Elsa Kauffman', 'Bear Murillo', 'Jackson Bledsoe']</t>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:53:01
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J230"/>
+  <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10467,6 +10467,46 @@
       </c>
       <c r="J230" t="inlineStr"/>
     </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>329</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E231" s="2" t="n">
+        <v>45922</v>
+      </c>
+      <c r="F231" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Bear Murillo', 'Elsa Kauffman']</t>
+        </is>
+      </c>
+      <c r="J231" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:53:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J231"/>
+  <dimension ref="A1:J232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10507,6 +10507,46 @@
       </c>
       <c r="J231" t="inlineStr"/>
     </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>329</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E232" s="2" t="n">
+        <v>45936</v>
+      </c>
+      <c r="F232" s="2" t="n">
+        <v>45939</v>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Bear Murillo', 'Elsa Kauffman']</t>
+        </is>
+      </c>
+      <c r="J232" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:54:46
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J232"/>
+  <dimension ref="A1:J233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10547,6 +10547,46 @@
       </c>
       <c r="J232" t="inlineStr"/>
     </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>329</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E233" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F233" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Bear Murillo', 'Elsa Kauffman']</t>
+        </is>
+      </c>
+      <c r="J233" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:55:28
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J233"/>
+  <dimension ref="A1:J234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10587,6 +10587,46 @@
       </c>
       <c r="J233" t="inlineStr"/>
     </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>329</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E234" s="2" t="n">
+        <v>45957</v>
+      </c>
+      <c r="F234" s="2" t="n">
+        <v>45960</v>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Bear Murillo', 'Elsa Kauffman']</t>
+        </is>
+      </c>
+      <c r="J234" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:56:10
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J234"/>
+  <dimension ref="A1:J235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10627,6 +10627,46 @@
       </c>
       <c r="J234" t="inlineStr"/>
     </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>329</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E235" s="2" t="n">
+        <v>45964</v>
+      </c>
+      <c r="F235" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Bear Murillo', 'Elsa Kauffman']</t>
+        </is>
+      </c>
+      <c r="J235" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:57:09
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J235"/>
+  <dimension ref="A1:J236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10667,6 +10667,46 @@
       </c>
       <c r="J235" t="inlineStr"/>
     </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>329</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E236" s="2" t="n">
+        <v>45971</v>
+      </c>
+      <c r="F236" s="2" t="n">
+        <v>45974</v>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Elsa Kauffman', 'Bear Murillo']</t>
+        </is>
+      </c>
+      <c r="J236" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-04 20:57:33
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J236"/>
+  <dimension ref="A1:J237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10707,6 +10707,46 @@
       </c>
       <c r="J236" t="inlineStr"/>
     </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>329</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E237" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="F237" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>FOR 315</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe']</t>
+        </is>
+      </c>
+      <c r="J237" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:08:11
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J237"/>
+  <dimension ref="A1:J238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10747,6 +10747,46 @@
       </c>
       <c r="J237" t="inlineStr"/>
     </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>338</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Reserved</t>
+        </is>
+      </c>
+      <c r="E238" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="F238" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>Vehicle to be used to travel to sample TLS plot locations for a Wildfire Crisis Strategy POD boundary fuels characterization project we are doing on the Coconino National Forest. Sites are primarily along road networks. Vehicle will primarily be used on weekends (Friday through Sundays) - with potential/occasional day trips in the week.</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>['Gabrielle Ayres', 'Scott Gilb', 'Kevin Espinoza']</t>
+        </is>
+      </c>
+      <c r="J238" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:18:35
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J238"/>
+  <dimension ref="A1:J239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10787,6 +10787,42 @@
       </c>
       <c r="J238" t="inlineStr"/>
     </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>338</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E239" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="F239" s="2" t="n">
+        <v>45914</v>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr"/>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J239" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:18:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J239"/>
+  <dimension ref="A1:J240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10815,13 +10815,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H239" t="inlineStr"/>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I239" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>338</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E240" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="F240" s="2" t="n">
+        <v>45921</v>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr"/>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J240" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:19:11
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J240"/>
+  <dimension ref="A1:J241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10855,13 +10855,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H240" t="inlineStr"/>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I240" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>338</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E241" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="F241" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr"/>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J241" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:19:35
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J241"/>
+  <dimension ref="A1:J242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10895,13 +10895,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H241" t="inlineStr"/>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I241" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>338</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E242" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="F242" s="2" t="n">
+        <v>45935</v>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr"/>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J242" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:19:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J242"/>
+  <dimension ref="A1:J243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10935,13 +10935,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H242" t="inlineStr"/>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I242" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>338</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E243" s="2" t="n">
+        <v>45940</v>
+      </c>
+      <c r="F243" s="2" t="n">
+        <v>45942</v>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr"/>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J243" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:20:30
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J243"/>
+  <dimension ref="A1:J244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10975,13 +10975,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H243" t="inlineStr"/>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I243" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>338</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E244" s="2" t="n">
+        <v>45947</v>
+      </c>
+      <c r="F244" s="2" t="n">
+        <v>45949</v>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr"/>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J244" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:21:56
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J244"/>
+  <dimension ref="A1:J245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11015,13 +11015,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H244" t="inlineStr"/>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I244" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>338</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E245" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="F245" s="2" t="n">
+        <v>45956</v>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr"/>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J245" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:22:31
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J245"/>
+  <dimension ref="A1:J246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11055,13 +11055,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H245" t="inlineStr"/>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I245" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>338</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E246" s="2" t="n">
+        <v>45961</v>
+      </c>
+      <c r="F246" s="2" t="n">
+        <v>45963</v>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr"/>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J246" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:22:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J246"/>
+  <dimension ref="A1:J247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11095,13 +11095,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H246" t="inlineStr"/>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I246" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>338</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E247" s="2" t="n">
+        <v>45968</v>
+      </c>
+      <c r="F247" s="2" t="n">
+        <v>45970</v>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr"/>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J247" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:23:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J247"/>
+  <dimension ref="A1:J248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11135,13 +11135,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H247" t="inlineStr"/>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I247" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>338</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E248" s="2" t="n">
+        <v>45975</v>
+      </c>
+      <c r="F248" s="2" t="n">
+        <v>45977</v>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr"/>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J248" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:23:23
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J248"/>
+  <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11175,13 +11175,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H248" t="inlineStr"/>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I248" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>338</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E249" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="F249" s="2" t="n">
+        <v>45984</v>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr"/>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J249" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:23:52
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J249"/>
+  <dimension ref="A1:J250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11215,13 +11215,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H249" t="inlineStr"/>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I249" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>338</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E250" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="F250" s="2" t="n">
+        <v>45991</v>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr"/>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J250" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:24:25
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J250"/>
+  <dimension ref="A1:J251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11255,13 +11255,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H250" t="inlineStr"/>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I250" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>338</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E251" s="2" t="n">
+        <v>45996</v>
+      </c>
+      <c r="F251" s="2" t="n">
+        <v>45998</v>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr"/>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J251" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-09 21:24:50
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J251"/>
+  <dimension ref="A1:J252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11295,13 +11295,53 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H251" t="inlineStr"/>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I251" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>338</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Gabrielle Ayres</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E252" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="F252" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr"/>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J252" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-10 18:43:46
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J252"/>
+  <dimension ref="A1:J253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11335,13 +11335,57 @@
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="H252" t="inlineStr"/>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I252" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>310</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>OUT OF COMMISION</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E253" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="F253" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>At Fleet for repairs</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>['Jacob Shelly']</t>
+        </is>
+      </c>
+      <c r="J253" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-15 21:47:41
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J253"/>
+  <dimension ref="A1:J254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11387,6 +11387,42 @@
       </c>
       <c r="J253" t="inlineStr"/>
     </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>321</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Adair Patterson</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E254" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F254" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr"/>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>['Adair Patterson']</t>
+        </is>
+      </c>
+      <c r="J254" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-15 21:48:15
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J254"/>
+  <dimension ref="A1:J255"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11415,13 +11415,53 @@
           <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
-      <c r="H254" t="inlineStr"/>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I254" t="inlineStr">
         <is>
           <t>['Adair Patterson']</t>
         </is>
       </c>
       <c r="J254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>321</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Adair Patterson</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E255" s="2" t="n">
+        <v>45957</v>
+      </c>
+      <c r="F255" s="2" t="n">
+        <v>45958</v>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr"/>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>['Adair Patterson']</t>
+        </is>
+      </c>
+      <c r="J255" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-15 22:17:00
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J255"/>
+  <dimension ref="A1:J256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11455,13 +11455,57 @@
           <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
-      <c r="H255" t="inlineStr"/>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I255" t="inlineStr">
         <is>
           <t>['Adair Patterson']</t>
         </is>
       </c>
       <c r="J255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>321</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Salli Dymond</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E256" s="2" t="n">
+        <v>45918</v>
+      </c>
+      <c r="F256" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>Students will drive to sites on Ellison and Bonita Creeks on the Tonto NF outside of Payson, AZ to collect water for stable isotope and nutrient analysis as part of the Dude Fire project funded by SRP Dude. This will be a 1-day trip with 3 NAU student/tech occupants.</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>['Paige Whitton', 'Logan Ozmet']</t>
+        </is>
+      </c>
+      <c r="J256" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-15 22:27:40
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J256"/>
+  <dimension ref="A1:J257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11507,6 +11507,46 @@
       </c>
       <c r="J256" t="inlineStr"/>
     </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>268</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E257" s="2" t="n">
+        <v>45917</v>
+      </c>
+      <c r="F257" s="2" t="n">
+        <v>45920</v>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>Fieldwork at Diné College campus, Tsaile, AZ</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>['Arantxa Curley', 'Mariola Barrera']</t>
+        </is>
+      </c>
+      <c r="J257" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-23 15:36:17
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -11516,7 +11516,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Pete Fule</t>
+          <t>OUT OF COMMISION</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -11528,7 +11528,7 @@
         <v>45917</v>
       </c>
       <c r="F257" s="2" t="n">
-        <v>45920</v>
+        <v>45930</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
@@ -11537,14 +11537,10 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Fieldwork at Diné College campus, Tsaile, AZ</t>
-        </is>
-      </c>
-      <c r="I257" t="inlineStr">
-        <is>
-          <t>['Arantxa Curley', 'Mariola Barrera']</t>
-        </is>
-      </c>
+          <t>Bad Tire</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr"/>
       <c r="J257" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-23 15:37:46
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J257"/>
+  <dimension ref="A1:J258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11543,6 +11543,46 @@
       <c r="I257" t="inlineStr"/>
       <c r="J257" t="inlineStr"/>
     </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>310</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Salli Dymond</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E258" s="2" t="n">
+        <v>45923</v>
+      </c>
+      <c r="F258" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>will be driving to Workman Creek in the Sierra Ancha Experimental Forest near Globe, AZ to do field work pertaining to my PhD dissertation which focuses on vadose zone processes, critical zone hydrology, and the effects of fire on the hydrologic cycle in headwater catchments.</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>['Emory Ellis']</t>
+        </is>
+      </c>
+      <c r="J258" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-23 15:39:39
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J258"/>
+  <dimension ref="A1:J259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11540,7 +11540,11 @@
           <t>Bad Tire</t>
         </is>
       </c>
-      <c r="I257" t="inlineStr"/>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J257" t="inlineStr"/>
     </row>
     <row r="258">
@@ -11582,6 +11586,46 @@
         </is>
       </c>
       <c r="J258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>329</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E259" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="F259" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>['Jackson Bledsoe', 'Kristen Waring']</t>
+        </is>
+      </c>
+      <c r="J259" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-23 16:59:09
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J259"/>
+  <dimension ref="A1:J260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11627,6 +11627,46 @@
       </c>
       <c r="J259" t="inlineStr"/>
     </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>467</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>OUT OF COMMISION</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E260" s="2" t="n">
+        <v>45923</v>
+      </c>
+      <c r="F260" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>Plow bracket removal</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>['Jacob Shelly']</t>
+        </is>
+      </c>
+      <c r="J260" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-23 20:28:55
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J260"/>
+  <dimension ref="A1:J261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11667,6 +11667,46 @@
       </c>
       <c r="J260" t="inlineStr"/>
     </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>331</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Nathan Saurer</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E261" s="2" t="n">
+        <v>45923</v>
+      </c>
+      <c r="F261" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>Motor Pool Supplemental vehicle.</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>['Nathan Saurer']</t>
+        </is>
+      </c>
+      <c r="J261" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-23 20:47:37
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J261"/>
+  <dimension ref="A1:J262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11707,6 +11707,46 @@
       </c>
       <c r="J261" t="inlineStr"/>
     </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>268</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E262" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="F262" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>['Kristen Waring', 'Jackson Bledsoe']</t>
+        </is>
+      </c>
+      <c r="J262" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-24 17:46:02
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -9630,7 +9630,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="C210" t="inlineStr">
         <is>
@@ -9650,7 +9650,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -9670,7 +9670,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="C211" t="inlineStr">
         <is>
@@ -9690,7 +9690,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -9710,7 +9710,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>331</v>
+        <v>466</v>
       </c>
       <c r="C212" t="inlineStr">
         <is>
@@ -9730,7 +9730,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-26 15:39:21
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -510,7 +510,7 @@
         <v>45595</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45596</v>
+        <v>45596.99930555555</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -554,7 +554,7 @@
         <v>45558</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45558</v>
+        <v>45558.99930555555</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -598,7 +598,7 @@
         <v>45593</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45593</v>
+        <v>45593.99930555555</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -642,7 +642,7 @@
         <v>45574</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45575</v>
+        <v>45575.99930555555</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -686,7 +686,7 @@
         <v>45553</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45554</v>
+        <v>45554.99930555555</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         <v>45712</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45716</v>
+        <v>45716.99930555555</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         <v>45600</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45600</v>
+        <v>45600.99930555555</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
         <v>45581</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45582</v>
+        <v>45582.99930555555</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
         <v>45551</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45551</v>
+        <v>45551.99930555555</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -906,7 +906,7 @@
         <v>45560</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45561</v>
+        <v>45561.99930555555</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -950,7 +950,7 @@
         <v>45567</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45568</v>
+        <v>45568.99930555555</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         <v>45401</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45402</v>
+        <v>45402.99930555555</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1038,7 +1038,7 @@
         <v>45572</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>45572</v>
+        <v>45572.99930555555</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
         <v>45432</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>45538</v>
+        <v>45538.99930555555</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1126,7 +1126,7 @@
         <v>45539</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45540</v>
+        <v>45540.99930555555</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1170,7 +1170,7 @@
         <v>45579</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45579</v>
+        <v>45579.99930555555</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1214,7 +1214,7 @@
         <v>45546</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45547</v>
+        <v>45547.99930555555</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>45421</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45421</v>
+        <v>45421.99930555555</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>45744</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45762</v>
+        <v>45762.99930555555</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1346,7 +1346,7 @@
         <v>45674</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45694</v>
+        <v>45694.99930555555</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         <v>45789</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45898</v>
+        <v>45898.99930555555</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         <v>45576</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45576</v>
+        <v>45576.99930555555</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1478,7 +1478,7 @@
         <v>45588</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45589</v>
+        <v>45589.99930555555</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1522,7 +1522,7 @@
         <v>45719</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>45729</v>
+        <v>45729.99930555555</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1566,7 +1566,7 @@
         <v>45733</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45737</v>
+        <v>45737.99930555555</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1610,7 +1610,7 @@
         <v>45581</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45585</v>
+        <v>45585.99930555555</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>45637</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>45642</v>
+        <v>45642.99930555555</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1698,7 +1698,7 @@
         <v>45855</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>45900</v>
+        <v>45900.99930555555</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1742,7 +1742,7 @@
         <v>45660</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>45670</v>
+        <v>45670.99930555555</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1786,7 +1786,7 @@
         <v>45627</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>45635</v>
+        <v>45635.99930555555</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         <v>45588</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>45588</v>
+        <v>45588.99930555555</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1874,7 +1874,7 @@
         <v>45789</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>45851</v>
+        <v>45851.99930555555</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
         <v>45554</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>45556</v>
+        <v>45556.99930555555</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
         <v>45679</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>45788</v>
+        <v>45788.99930555555</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2006,7 +2006,7 @@
         <v>45605</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>45610</v>
+        <v>45610.99930555555</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2050,7 +2050,7 @@
         <v>45600</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>45600</v>
+        <v>45600.99930555555</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         <v>45758</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>45759</v>
+        <v>45759.99930555555</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>45594</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>45595</v>
+        <v>45595.99930555555</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
         <v>45774</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>45775</v>
+        <v>45775.99930555555</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2226,7 +2226,7 @@
         <v>45627</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>45748</v>
+        <v>45748.99930555555</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2270,7 +2270,7 @@
         <v>45608</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>45608</v>
+        <v>45608.99930555555</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2314,7 +2314,7 @@
         <v>45562</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>45564</v>
+        <v>45564.99930555555</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2358,7 +2358,7 @@
         <v>45589</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>45593</v>
+        <v>45593.99930555555</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2402,7 +2402,7 @@
         <v>45568</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>45568</v>
+        <v>45568.99930555555</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2446,7 +2446,7 @@
         <v>45548</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>45554</v>
+        <v>45554.99930555555</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2490,7 +2490,7 @@
         <v>45789</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>45891</v>
+        <v>45891.99930555555</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2534,7 +2534,7 @@
         <v>45603</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>45604</v>
+        <v>45604.99930555555</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>45597</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>45598</v>
+        <v>45598.99930555555</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2622,7 +2622,7 @@
         <v>45581</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>45587</v>
+        <v>45587.99930555555</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2666,7 +2666,7 @@
         <v>45611</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>45611</v>
+        <v>45611.99930555555</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2710,7 +2710,7 @@
         <v>45736</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>45737</v>
+        <v>45737.99930555555</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2754,7 +2754,7 @@
         <v>45790</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>45790</v>
+        <v>45790.99930555555</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2798,7 +2798,7 @@
         <v>45744</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>45745</v>
+        <v>45745.99930555555</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2842,7 +2842,7 @@
         <v>45756</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>45761</v>
+        <v>45761.99930555555</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2886,7 +2886,7 @@
         <v>45772</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>45773</v>
+        <v>45773.99930555555</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2930,7 +2930,7 @@
         <v>45740</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>45741</v>
+        <v>45741.99930555555</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2974,7 +2974,7 @@
         <v>45552</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>45554</v>
+        <v>45554.99930555555</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
         <v>45802</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>45855</v>
+        <v>45855.99930555555</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
         <v>45768</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>45769</v>
+        <v>45769.99930555555</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -3106,7 +3106,7 @@
         <v>45786</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>45790</v>
+        <v>45790.99930555555</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -3150,7 +3150,7 @@
         <v>45566</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>45568</v>
+        <v>45568.99930555555</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -3194,7 +3194,7 @@
         <v>45678</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>45679</v>
+        <v>45679.99930555555</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -3238,7 +3238,7 @@
         <v>45559</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>45561</v>
+        <v>45561.99930555555</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3282,7 +3282,7 @@
         <v>45681</v>
       </c>
       <c r="F65" s="2" t="n">
-        <v>45688</v>
+        <v>45688.99930555555</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -3326,7 +3326,7 @@
         <v>45586</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>45610</v>
+        <v>45610.99930555555</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -3370,7 +3370,7 @@
         <v>45545</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>45548</v>
+        <v>45548.99930555555</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -3414,7 +3414,7 @@
         <v>45573</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>45575</v>
+        <v>45575.99930555555</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3458,7 +3458,7 @@
         <v>45855</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>45900</v>
+        <v>45900.99930555555</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3502,7 +3502,7 @@
         <v>45754</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>45755</v>
+        <v>45755.99930555555</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         <v>45580</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>45582</v>
+        <v>45582.99930555555</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3590,7 +3590,7 @@
         <v>45722</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>45730</v>
+        <v>45730.99930555555</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3634,7 +3634,7 @@
         <v>45868</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>45870</v>
+        <v>45870.99930555555</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
         <v>45595</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>45595</v>
+        <v>45595.99930555555</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3722,7 +3722,7 @@
         <v>45581</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>45583</v>
+        <v>45583.99930555555</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3766,7 +3766,7 @@
         <v>45565</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>45567</v>
+        <v>45567.99930555555</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3810,7 +3810,7 @@
         <v>45833</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>45834</v>
+        <v>45834.99930555555</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3854,7 +3854,7 @@
         <v>45866</v>
       </c>
       <c r="F78" s="2" t="n">
-        <v>45867</v>
+        <v>45867.99930555555</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3898,7 +3898,7 @@
         <v>45667</v>
       </c>
       <c r="F79" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3942,7 +3942,7 @@
         <v>45667</v>
       </c>
       <c r="F80" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3986,7 +3986,7 @@
         <v>45881</v>
       </c>
       <c r="F81" s="2" t="n">
-        <v>45883</v>
+        <v>45883.99930555555</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -4026,7 +4026,7 @@
         <v>45852</v>
       </c>
       <c r="F82" s="2" t="n">
-        <v>45853</v>
+        <v>45853.99930555555</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -4070,7 +4070,7 @@
         <v>45667</v>
       </c>
       <c r="F83" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -4114,7 +4114,7 @@
         <v>45845</v>
       </c>
       <c r="F84" s="2" t="n">
-        <v>45848</v>
+        <v>45848.99930555555</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -4158,7 +4158,7 @@
         <v>45667</v>
       </c>
       <c r="F85" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -4202,7 +4202,7 @@
         <v>45588</v>
       </c>
       <c r="F86" s="2" t="n">
-        <v>45588</v>
+        <v>45588.99930555555</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -4246,7 +4246,7 @@
         <v>45576</v>
       </c>
       <c r="F87" s="2" t="n">
-        <v>45576</v>
+        <v>45576.99930555555</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -4290,7 +4290,7 @@
         <v>45667</v>
       </c>
       <c r="F88" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -4334,7 +4334,7 @@
         <v>45825</v>
       </c>
       <c r="F89" s="2" t="n">
-        <v>45826</v>
+        <v>45826.99930555555</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
         <v>45717</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>45813</v>
+        <v>45813.99930555555</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -4422,7 +4422,7 @@
         <v>45667</v>
       </c>
       <c r="F91" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -4466,7 +4466,7 @@
         <v>45667</v>
       </c>
       <c r="F92" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -4510,7 +4510,7 @@
         <v>45859</v>
       </c>
       <c r="F93" s="2" t="n">
-        <v>45861</v>
+        <v>45861.99930555555</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -4554,7 +4554,7 @@
         <v>45642</v>
       </c>
       <c r="F94" s="2" t="n">
-        <v>45643</v>
+        <v>45643.99930555555</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -4598,7 +4598,7 @@
         <v>45667</v>
       </c>
       <c r="F95" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -4642,7 +4642,7 @@
         <v>45667</v>
       </c>
       <c r="F96" s="2" t="n">
-        <v>45667</v>
+        <v>45667.99930555555</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -4686,7 +4686,7 @@
         <v>45831</v>
       </c>
       <c r="F97" s="2" t="n">
-        <v>45832</v>
+        <v>45832.99930555555</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -4730,7 +4730,7 @@
         <v>45840</v>
       </c>
       <c r="F98" s="2" t="n">
-        <v>45841</v>
+        <v>45841.99930555555</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -4774,7 +4774,7 @@
         <v>45839</v>
       </c>
       <c r="F99" s="2" t="n">
-        <v>45840</v>
+        <v>45840.99930555555</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -4818,7 +4818,7 @@
         <v>45709</v>
       </c>
       <c r="F100" s="2" t="n">
-        <v>45709</v>
+        <v>45709.99930555555</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -4862,7 +4862,7 @@
         <v>45709</v>
       </c>
       <c r="F101" s="2" t="n">
-        <v>45709</v>
+        <v>45709.99930555555</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -4906,7 +4906,7 @@
         <v>45776</v>
       </c>
       <c r="F102" s="2" t="n">
-        <v>45781</v>
+        <v>45781.99930555555</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4950,7 +4950,7 @@
         <v>45747</v>
       </c>
       <c r="F103" s="2" t="n">
-        <v>45752</v>
+        <v>45752.99930555555</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4994,7 +4994,7 @@
         <v>45709</v>
       </c>
       <c r="F104" s="2" t="n">
-        <v>45710</v>
+        <v>45710.99930555555</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -5038,7 +5038,7 @@
         <v>45835</v>
       </c>
       <c r="F105" s="2" t="n">
-        <v>45836</v>
+        <v>45836.99930555555</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -5082,7 +5082,7 @@
         <v>45756</v>
       </c>
       <c r="F106" s="2" t="n">
-        <v>45759</v>
+        <v>45759.99930555555</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -5126,7 +5126,7 @@
         <v>45687</v>
       </c>
       <c r="F107" s="2" t="n">
-        <v>45689</v>
+        <v>45689.99930555555</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -5170,7 +5170,7 @@
         <v>45878</v>
       </c>
       <c r="F108" s="2" t="n">
-        <v>45884</v>
+        <v>45884.99930555555</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -5214,7 +5214,7 @@
         <v>45631</v>
       </c>
       <c r="F109" s="2" t="n">
-        <v>45643</v>
+        <v>45643.99930555555</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -5258,7 +5258,7 @@
         <v>45792</v>
       </c>
       <c r="F110" s="2" t="n">
-        <v>45795</v>
+        <v>45795.99930555555</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -5302,7 +5302,7 @@
         <v>45824</v>
       </c>
       <c r="F111" s="2" t="n">
-        <v>45835</v>
+        <v>45835.99930555555</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -5346,7 +5346,7 @@
         <v>45716</v>
       </c>
       <c r="F112" s="2" t="n">
-        <v>45722</v>
+        <v>45722.99930555555</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -5390,7 +5390,7 @@
         <v>45705</v>
       </c>
       <c r="F113" s="2" t="n">
-        <v>45707</v>
+        <v>45707.99930555555</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -5434,7 +5434,7 @@
         <v>45572</v>
       </c>
       <c r="F114" s="2" t="n">
-        <v>45576</v>
+        <v>45576.99930555555</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -5478,7 +5478,7 @@
         <v>45642</v>
       </c>
       <c r="F115" s="2" t="n">
-        <v>45642</v>
+        <v>45642.99930555555</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -5522,7 +5522,7 @@
         <v>45568</v>
       </c>
       <c r="F116" s="2" t="n">
-        <v>45568</v>
+        <v>45568.99930555555</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -5566,7 +5566,7 @@
         <v>45481</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>45490</v>
+        <v>45490.99930555555</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -5610,7 +5610,7 @@
         <v>45761</v>
       </c>
       <c r="F118" s="2" t="n">
-        <v>45765</v>
+        <v>45765.99930555555</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -5654,7 +5654,7 @@
         <v>45770</v>
       </c>
       <c r="F119" s="2" t="n">
-        <v>45789</v>
+        <v>45789.99930555555</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -5698,7 +5698,7 @@
         <v>45747</v>
       </c>
       <c r="F120" s="2" t="n">
-        <v>45752</v>
+        <v>45752.99930555555</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -5742,7 +5742,7 @@
         <v>45824</v>
       </c>
       <c r="F121" s="2" t="n">
-        <v>45829</v>
+        <v>45829.99930555555</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -5786,7 +5786,7 @@
         <v>45613</v>
       </c>
       <c r="F122" s="2" t="n">
-        <v>45619</v>
+        <v>45619.99930555555</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -5830,7 +5830,7 @@
         <v>45503</v>
       </c>
       <c r="F123" s="2" t="n">
-        <v>45503</v>
+        <v>45503.99930555555</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -5874,7 +5874,7 @@
         <v>45957</v>
       </c>
       <c r="F124" s="2" t="n">
-        <v>45960</v>
+        <v>45960.99930555555</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -5918,7 +5918,7 @@
         <v>45629</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>45633</v>
+        <v>45633.99930555555</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -5962,7 +5962,7 @@
         <v>45534</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>45553</v>
+        <v>45553.99930555555</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -6006,7 +6006,7 @@
         <v>45737</v>
       </c>
       <c r="F127" s="2" t="n">
-        <v>45741</v>
+        <v>45741.99930555555</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -6050,7 +6050,7 @@
         <v>45929</v>
       </c>
       <c r="F128" s="2" t="n">
-        <v>45935</v>
+        <v>45935.99930555555</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -6090,7 +6090,7 @@
         <v>45605</v>
       </c>
       <c r="F129" s="2" t="n">
-        <v>45609</v>
+        <v>45609.99930555555</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -6134,7 +6134,7 @@
         <v>45716</v>
       </c>
       <c r="F130" s="2" t="n">
-        <v>45718</v>
+        <v>45718.99930555555</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
         <v>45611</v>
       </c>
       <c r="F131" s="2" t="n">
-        <v>45611</v>
+        <v>45611.99930555555</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -6222,7 +6222,7 @@
         <v>45555</v>
       </c>
       <c r="F132" s="2" t="n">
-        <v>45555</v>
+        <v>45555.99930555555</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -6266,7 +6266,7 @@
         <v>45509</v>
       </c>
       <c r="F133" s="2" t="n">
-        <v>45514</v>
+        <v>45514.99930555555</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -6310,7 +6310,7 @@
         <v>45810</v>
       </c>
       <c r="F134" s="2" t="n">
-        <v>45891</v>
+        <v>45891.99930555555</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -6354,7 +6354,7 @@
         <v>45525</v>
       </c>
       <c r="F135" s="2" t="n">
-        <v>45525</v>
+        <v>45525.99930555555</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -6398,7 +6398,7 @@
         <v>45517</v>
       </c>
       <c r="F136" s="2" t="n">
-        <v>45518</v>
+        <v>45518.99930555555</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -6442,7 +6442,7 @@
         <v>45764</v>
       </c>
       <c r="F137" s="2" t="n">
-        <v>45775</v>
+        <v>45775.99930555555</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -6486,7 +6486,7 @@
         <v>45453</v>
       </c>
       <c r="F138" s="2" t="n">
-        <v>45477</v>
+        <v>45477.99930555555</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -6530,7 +6530,7 @@
         <v>45478</v>
       </c>
       <c r="F139" s="2" t="n">
-        <v>45506</v>
+        <v>45506.99930555555</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -6574,7 +6574,7 @@
         <v>45432</v>
       </c>
       <c r="F140" s="2" t="n">
-        <v>45434</v>
+        <v>45434.99930555555</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -6618,7 +6618,7 @@
         <v>45756</v>
       </c>
       <c r="F141" s="2" t="n">
-        <v>45761</v>
+        <v>45761.99930555555</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -6662,7 +6662,7 @@
         <v>45804</v>
       </c>
       <c r="F142" s="2" t="n">
-        <v>45805</v>
+        <v>45805.99930555555</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -6706,7 +6706,7 @@
         <v>45439</v>
       </c>
       <c r="F143" s="2" t="n">
-        <v>45445</v>
+        <v>45445.99930555555</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -6750,7 +6750,7 @@
         <v>45740</v>
       </c>
       <c r="F144" s="2" t="n">
-        <v>45747</v>
+        <v>45747.99930555555</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -6794,7 +6794,7 @@
         <v>45785</v>
       </c>
       <c r="F145" s="2" t="n">
-        <v>45786</v>
+        <v>45786.99930555555</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -6838,7 +6838,7 @@
         <v>45602</v>
       </c>
       <c r="F146" s="2" t="n">
-        <v>45608</v>
+        <v>45608.99930555555</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
@@ -6882,7 +6882,7 @@
         <v>45627</v>
       </c>
       <c r="F147" s="2" t="n">
-        <v>45636</v>
+        <v>45636.99930555555</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -6926,7 +6926,7 @@
         <v>45617</v>
       </c>
       <c r="F148" s="2" t="n">
-        <v>45623</v>
+        <v>45623.99930555555</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -6970,7 +6970,7 @@
         <v>45627</v>
       </c>
       <c r="F149" s="2" t="n">
-        <v>45688</v>
+        <v>45688.99930555555</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -7014,7 +7014,7 @@
         <v>45735</v>
       </c>
       <c r="F150" s="2" t="n">
-        <v>45742</v>
+        <v>45742.99930555555</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -7058,7 +7058,7 @@
         <v>45716</v>
       </c>
       <c r="F151" s="2" t="n">
-        <v>45725</v>
+        <v>45725.99930555555</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -7102,7 +7102,7 @@
         <v>45541</v>
       </c>
       <c r="F152" s="2" t="n">
-        <v>45571</v>
+        <v>45571.99930555555</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -7146,7 +7146,7 @@
         <v>45639</v>
       </c>
       <c r="F153" s="2" t="n">
-        <v>45647</v>
+        <v>45647.99930555555</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -7190,7 +7190,7 @@
         <v>45748</v>
       </c>
       <c r="F154" s="2" t="n">
-        <v>45752</v>
+        <v>45752.99930555555</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -7234,7 +7234,7 @@
         <v>45432</v>
       </c>
       <c r="F155" s="2" t="n">
-        <v>45433</v>
+        <v>45433.99930555555</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -7278,7 +7278,7 @@
         <v>45421</v>
       </c>
       <c r="F156" s="2" t="n">
-        <v>45421</v>
+        <v>45421.99930555555</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -7322,7 +7322,7 @@
         <v>45401</v>
       </c>
       <c r="F157" s="2" t="n">
-        <v>45402</v>
+        <v>45402.99930555555</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -7366,7 +7366,7 @@
         <v>45422</v>
       </c>
       <c r="F158" s="2" t="n">
-        <v>45427</v>
+        <v>45427.99930555555</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -7410,7 +7410,7 @@
         <v>45444</v>
       </c>
       <c r="F159" s="2" t="n">
-        <v>45536</v>
+        <v>45536.99930555555</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -7454,7 +7454,7 @@
         <v>45713</v>
       </c>
       <c r="F160" s="2" t="n">
-        <v>45714</v>
+        <v>45714.99930555555</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -7498,7 +7498,7 @@
         <v>45778</v>
       </c>
       <c r="F161" s="2" t="n">
-        <v>45930</v>
+        <v>45930.99930555555</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -7542,7 +7542,7 @@
         <v>45425</v>
       </c>
       <c r="F162" s="2" t="n">
-        <v>45474</v>
+        <v>45474.99930555555</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -7586,7 +7586,7 @@
         <v>45581</v>
       </c>
       <c r="F163" s="2" t="n">
-        <v>45587</v>
+        <v>45587.99930555555</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -7630,7 +7630,7 @@
         <v>45401</v>
       </c>
       <c r="F164" s="2" t="n">
-        <v>45402</v>
+        <v>45402.99930555555</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -7674,7 +7674,7 @@
         <v>45475</v>
       </c>
       <c r="F165" s="2" t="n">
-        <v>45565</v>
+        <v>45565.99930555555</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -7718,7 +7718,7 @@
         <v>45597</v>
       </c>
       <c r="F166" s="2" t="n">
-        <v>45613</v>
+        <v>45613.99930555555</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -7762,7 +7762,7 @@
         <v>45667</v>
       </c>
       <c r="F167" s="2" t="n">
-        <v>45787</v>
+        <v>45787.99930555555</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -7806,7 +7806,7 @@
         <v>45845</v>
       </c>
       <c r="F168" s="2" t="n">
-        <v>45856</v>
+        <v>45856.99930555555</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -7850,7 +7850,7 @@
         <v>45859</v>
       </c>
       <c r="F169" s="2" t="n">
-        <v>45898</v>
+        <v>45898.99930555555</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -7894,7 +7894,7 @@
         <v>45798</v>
       </c>
       <c r="F170" s="2" t="n">
-        <v>45834</v>
+        <v>45834.99930555555</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -7938,7 +7938,7 @@
         <v>45594</v>
       </c>
       <c r="F171" s="2" t="n">
-        <v>45594</v>
+        <v>45594.99930555555</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -7982,7 +7982,7 @@
         <v>45403</v>
       </c>
       <c r="F172" s="2" t="n">
-        <v>45423</v>
+        <v>45423.99930555555</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -8026,7 +8026,7 @@
         <v>45744</v>
       </c>
       <c r="F173" s="2" t="n">
-        <v>45762</v>
+        <v>45762.99930555555</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -8070,7 +8070,7 @@
         <v>45425</v>
       </c>
       <c r="F174" s="2" t="n">
-        <v>45534</v>
+        <v>45534.99930555555</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -8114,7 +8114,7 @@
         <v>45568</v>
       </c>
       <c r="F175" s="2" t="n">
-        <v>45572</v>
+        <v>45572.99930555555</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -8158,7 +8158,7 @@
         <v>45595</v>
       </c>
       <c r="F176" s="2" t="n">
-        <v>45599</v>
+        <v>45599.99930555555</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -8202,7 +8202,7 @@
         <v>45629</v>
       </c>
       <c r="F177" s="2" t="n">
-        <v>45647</v>
+        <v>45647.99930555555</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -8246,7 +8246,7 @@
         <v>45629</v>
       </c>
       <c r="F178" s="2" t="n">
-        <v>45648</v>
+        <v>45648.99930555555</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -8290,7 +8290,7 @@
         <v>45688</v>
       </c>
       <c r="F179" s="2" t="n">
-        <v>45690</v>
+        <v>45690.99930555555</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -8334,7 +8334,7 @@
         <v>45401</v>
       </c>
       <c r="F180" s="2" t="n">
-        <v>45410</v>
+        <v>45410.99930555555</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -8378,7 +8378,7 @@
         <v>45709</v>
       </c>
       <c r="F181" s="2" t="n">
-        <v>45711</v>
+        <v>45711.99930555555</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -8422,7 +8422,7 @@
         <v>45610</v>
       </c>
       <c r="F182" s="2" t="n">
-        <v>45614</v>
+        <v>45614.99930555555</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -8466,7 +8466,7 @@
         <v>45729</v>
       </c>
       <c r="F183" s="2" t="n">
-        <v>45730</v>
+        <v>45730.99930555555</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -8510,7 +8510,7 @@
         <v>45561</v>
       </c>
       <c r="F184" s="2" t="n">
-        <v>45561</v>
+        <v>45561.99930555555</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -8554,7 +8554,7 @@
         <v>45778</v>
       </c>
       <c r="F185" s="2" t="n">
-        <v>45796</v>
+        <v>45796.99930555555</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -8598,7 +8598,7 @@
         <v>45605</v>
       </c>
       <c r="F186" s="2" t="n">
-        <v>45605</v>
+        <v>45605.99930555555</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -8642,7 +8642,7 @@
         <v>45820</v>
       </c>
       <c r="F187" s="2" t="n">
-        <v>45900</v>
+        <v>45900.99930555555</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -8686,7 +8686,7 @@
         <v>45592</v>
       </c>
       <c r="F188" s="2" t="n">
-        <v>45594</v>
+        <v>45594.99930555555</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -8730,7 +8730,7 @@
         <v>45677</v>
       </c>
       <c r="F189" s="2" t="n">
-        <v>45678</v>
+        <v>45678.99930555555</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -8774,7 +8774,7 @@
         <v>45421</v>
       </c>
       <c r="F190" s="2" t="n">
-        <v>45421</v>
+        <v>45421.99930555555</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -8818,7 +8818,7 @@
         <v>45440</v>
       </c>
       <c r="F191" s="2" t="n">
-        <v>45440</v>
+        <v>45440.99930555555</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -8862,7 +8862,7 @@
         <v>45740</v>
       </c>
       <c r="F192" s="2" t="n">
-        <v>45747</v>
+        <v>45747.99930555555</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -8906,7 +8906,7 @@
         <v>45478</v>
       </c>
       <c r="F193" s="2" t="n">
-        <v>45487</v>
+        <v>45487.99930555555</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -8950,7 +8950,7 @@
         <v>45722</v>
       </c>
       <c r="F194" s="2" t="n">
-        <v>45730</v>
+        <v>45730.99930555555</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -8994,7 +8994,7 @@
         <v>45768</v>
       </c>
       <c r="F195" s="2" t="n">
-        <v>45915</v>
+        <v>45915.99930555555</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -9038,7 +9038,7 @@
         <v>45757</v>
       </c>
       <c r="F196" s="2" t="n">
-        <v>45761</v>
+        <v>45761.99930555555</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -9082,7 +9082,7 @@
         <v>45533</v>
       </c>
       <c r="F197" s="2" t="n">
-        <v>45534</v>
+        <v>45534.99930555555</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -9126,7 +9126,7 @@
         <v>45441</v>
       </c>
       <c r="F198" s="2" t="n">
-        <v>45442</v>
+        <v>45442.99930555555</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -9170,7 +9170,7 @@
         <v>45488</v>
       </c>
       <c r="F199" s="2" t="n">
-        <v>45491</v>
+        <v>45491.99930555555</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -9214,7 +9214,7 @@
         <v>45509</v>
       </c>
       <c r="F200" s="2" t="n">
-        <v>45513</v>
+        <v>45513.99930555555</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -9258,7 +9258,7 @@
         <v>45516</v>
       </c>
       <c r="F201" s="2" t="n">
-        <v>45521</v>
+        <v>45521.99930555555</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -9302,7 +9302,7 @@
         <v>45527</v>
       </c>
       <c r="F202" s="2" t="n">
-        <v>45527</v>
+        <v>45527.99930555555</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -9346,7 +9346,7 @@
         <v>45401</v>
       </c>
       <c r="F203" s="2" t="n">
-        <v>45402</v>
+        <v>45402.99930555555</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -9390,7 +9390,7 @@
         <v>45496</v>
       </c>
       <c r="F204" s="2" t="n">
-        <v>45506</v>
+        <v>45506.99930555555</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -9434,7 +9434,7 @@
         <v>45523</v>
       </c>
       <c r="F205" s="2" t="n">
-        <v>45524</v>
+        <v>45524.99930555555</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
         <v>45431</v>
       </c>
       <c r="F206" s="2" t="n">
-        <v>45436</v>
+        <v>45436.99930555555</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -9522,7 +9522,7 @@
         <v>45408</v>
       </c>
       <c r="F207" s="2" t="n">
-        <v>45412</v>
+        <v>45412.99930555555</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -9566,7 +9566,7 @@
         <v>45915</v>
       </c>
       <c r="F208" s="2" t="n">
-        <v>45916</v>
+        <v>45915.99930555555</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -9606,7 +9606,7 @@
         <v>45936</v>
       </c>
       <c r="F209" s="2" t="n">
-        <v>45937</v>
+        <v>45936.99930555555</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -9646,7 +9646,7 @@
         <v>45950</v>
       </c>
       <c r="F210" s="2" t="n">
-        <v>45951</v>
+        <v>45950.99930555555</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -9686,7 +9686,7 @@
         <v>45978</v>
       </c>
       <c r="F211" s="2" t="n">
-        <v>45979</v>
+        <v>45978.99930555555</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -9726,7 +9726,7 @@
         <v>45992</v>
       </c>
       <c r="F212" s="2" t="n">
-        <v>45993</v>
+        <v>45992.99930555555</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
@@ -9766,7 +9766,7 @@
         <v>45884</v>
       </c>
       <c r="F213" s="2" t="n">
-        <v>45885</v>
+        <v>45885.99930555555</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
@@ -9806,7 +9806,7 @@
         <v>45888</v>
       </c>
       <c r="F214" s="2" t="n">
-        <v>45890</v>
+        <v>45890.99930555555</v>
       </c>
       <c r="G214" t="inlineStr">
         <is>
@@ -9846,7 +9846,7 @@
         <v>45897</v>
       </c>
       <c r="F215" s="2" t="n">
-        <v>45900</v>
+        <v>45900.99930555555</v>
       </c>
       <c r="G215" t="inlineStr">
         <is>
@@ -9886,7 +9886,7 @@
         <v>45898</v>
       </c>
       <c r="F216" s="2" t="n">
-        <v>45940</v>
+        <v>45940.99930555555</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -9928,7 +9928,7 @@
         <v>45902</v>
       </c>
       <c r="F217" s="2" t="n">
-        <v>45905</v>
+        <v>45905.99930555555</v>
       </c>
       <c r="G217" t="inlineStr">
         <is>
@@ -9968,7 +9968,7 @@
         <v>45906</v>
       </c>
       <c r="F218" s="2" t="n">
-        <v>45924</v>
+        <v>45924.99930555555</v>
       </c>
       <c r="G218" t="inlineStr">
         <is>
@@ -10008,7 +10008,7 @@
         <v>45905</v>
       </c>
       <c r="F219" s="2" t="n">
-        <v>46006</v>
+        <v>46006.99930555555</v>
       </c>
       <c r="G219" t="inlineStr">
         <is>
@@ -10048,7 +10048,7 @@
         <v>45904</v>
       </c>
       <c r="F220" s="2" t="n">
-        <v>45910</v>
+        <v>45910.99930555555</v>
       </c>
       <c r="G220" t="inlineStr">
         <is>
@@ -10088,7 +10088,7 @@
         <v>45909</v>
       </c>
       <c r="F221" s="2" t="n">
-        <v>45912</v>
+        <v>45912.99930555555</v>
       </c>
       <c r="G221" t="inlineStr">
         <is>
@@ -10128,7 +10128,7 @@
         <v>45916</v>
       </c>
       <c r="F222" s="2" t="n">
-        <v>45919</v>
+        <v>45919.99930555555</v>
       </c>
       <c r="G222" t="inlineStr">
         <is>
@@ -10168,7 +10168,7 @@
         <v>45923</v>
       </c>
       <c r="F223" s="2" t="n">
-        <v>45926</v>
+        <v>45926.99930555555</v>
       </c>
       <c r="G223" t="inlineStr">
         <is>
@@ -10208,7 +10208,7 @@
         <v>45930</v>
       </c>
       <c r="F224" s="2" t="n">
-        <v>45933</v>
+        <v>45933.99930555555</v>
       </c>
       <c r="G224" t="inlineStr">
         <is>
@@ -10248,7 +10248,7 @@
         <v>45937</v>
       </c>
       <c r="F225" s="2" t="n">
-        <v>45940</v>
+        <v>45940.99930555555</v>
       </c>
       <c r="G225" t="inlineStr">
         <is>
@@ -10288,7 +10288,7 @@
         <v>45944</v>
       </c>
       <c r="F226" s="2" t="n">
-        <v>45947</v>
+        <v>45947.99930555555</v>
       </c>
       <c r="G226" t="inlineStr">
         <is>
@@ -10328,7 +10328,7 @@
         <v>45951</v>
       </c>
       <c r="F227" s="2" t="n">
-        <v>45954</v>
+        <v>45954.99930555555</v>
       </c>
       <c r="G227" t="inlineStr">
         <is>
@@ -10368,7 +10368,7 @@
         <v>45958</v>
       </c>
       <c r="F228" s="2" t="n">
-        <v>45961</v>
+        <v>45961.99930555555</v>
       </c>
       <c r="G228" t="inlineStr">
         <is>
@@ -10408,7 +10408,7 @@
         <v>45965</v>
       </c>
       <c r="F229" s="2" t="n">
-        <v>45968</v>
+        <v>45968.99930555555</v>
       </c>
       <c r="G229" t="inlineStr">
         <is>
@@ -10448,7 +10448,7 @@
         <v>45915</v>
       </c>
       <c r="F230" s="2" t="n">
-        <v>45918</v>
+        <v>45918.99930555555</v>
       </c>
       <c r="G230" t="inlineStr">
         <is>
@@ -10488,7 +10488,7 @@
         <v>45922</v>
       </c>
       <c r="F231" s="2" t="n">
-        <v>45925</v>
+        <v>45925.99930555555</v>
       </c>
       <c r="G231" t="inlineStr">
         <is>
@@ -10528,7 +10528,7 @@
         <v>45936</v>
       </c>
       <c r="F232" s="2" t="n">
-        <v>45939</v>
+        <v>45939.99930555555</v>
       </c>
       <c r="G232" t="inlineStr">
         <is>
@@ -10568,7 +10568,7 @@
         <v>45943</v>
       </c>
       <c r="F233" s="2" t="n">
-        <v>45946</v>
+        <v>45946.99930555555</v>
       </c>
       <c r="G233" t="inlineStr">
         <is>
@@ -10608,7 +10608,7 @@
         <v>45957</v>
       </c>
       <c r="F234" s="2" t="n">
-        <v>45960</v>
+        <v>45960.99930555555</v>
       </c>
       <c r="G234" t="inlineStr">
         <is>
@@ -10648,7 +10648,7 @@
         <v>45964</v>
       </c>
       <c r="F235" s="2" t="n">
-        <v>45967</v>
+        <v>45967.99930555555</v>
       </c>
       <c r="G235" t="inlineStr">
         <is>
@@ -10688,7 +10688,7 @@
         <v>45971</v>
       </c>
       <c r="F236" s="2" t="n">
-        <v>45974</v>
+        <v>45974.99930555555</v>
       </c>
       <c r="G236" t="inlineStr">
         <is>
@@ -10728,7 +10728,7 @@
         <v>45911</v>
       </c>
       <c r="F237" s="2" t="n">
-        <v>45912</v>
+        <v>45912.99930555555</v>
       </c>
       <c r="G237" t="inlineStr">
         <is>
@@ -10768,7 +10768,7 @@
         <v>45912</v>
       </c>
       <c r="F238" s="2" t="n">
-        <v>46003</v>
+        <v>46003.99930555555</v>
       </c>
       <c r="G238" t="inlineStr">
         <is>
@@ -10808,7 +10808,7 @@
         <v>45912</v>
       </c>
       <c r="F239" s="2" t="n">
-        <v>45914</v>
+        <v>45914.99930555555</v>
       </c>
       <c r="G239" t="inlineStr">
         <is>
@@ -10848,7 +10848,7 @@
         <v>45919</v>
       </c>
       <c r="F240" s="2" t="n">
-        <v>45921</v>
+        <v>45921.99930555555</v>
       </c>
       <c r="G240" t="inlineStr">
         <is>
@@ -10888,7 +10888,7 @@
         <v>45926</v>
       </c>
       <c r="F241" s="2" t="n">
-        <v>45928</v>
+        <v>45928.99930555555</v>
       </c>
       <c r="G241" t="inlineStr">
         <is>
@@ -10928,7 +10928,7 @@
         <v>45933</v>
       </c>
       <c r="F242" s="2" t="n">
-        <v>45935</v>
+        <v>45935.99930555555</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -10968,7 +10968,7 @@
         <v>45940</v>
       </c>
       <c r="F243" s="2" t="n">
-        <v>45942</v>
+        <v>45942.99930555555</v>
       </c>
       <c r="G243" t="inlineStr">
         <is>
@@ -11008,7 +11008,7 @@
         <v>45947</v>
       </c>
       <c r="F244" s="2" t="n">
-        <v>45949</v>
+        <v>45949.99930555555</v>
       </c>
       <c r="G244" t="inlineStr">
         <is>
@@ -11048,7 +11048,7 @@
         <v>45954</v>
       </c>
       <c r="F245" s="2" t="n">
-        <v>45956</v>
+        <v>45956.99930555555</v>
       </c>
       <c r="G245" t="inlineStr">
         <is>
@@ -11088,7 +11088,7 @@
         <v>45961</v>
       </c>
       <c r="F246" s="2" t="n">
-        <v>45963</v>
+        <v>45963.99930555555</v>
       </c>
       <c r="G246" t="inlineStr">
         <is>
@@ -11128,7 +11128,7 @@
         <v>45968</v>
       </c>
       <c r="F247" s="2" t="n">
-        <v>45970</v>
+        <v>45970.99930555555</v>
       </c>
       <c r="G247" t="inlineStr">
         <is>
@@ -11168,7 +11168,7 @@
         <v>45975</v>
       </c>
       <c r="F248" s="2" t="n">
-        <v>45977</v>
+        <v>45977.99930555555</v>
       </c>
       <c r="G248" t="inlineStr">
         <is>
@@ -11208,7 +11208,7 @@
         <v>45982</v>
       </c>
       <c r="F249" s="2" t="n">
-        <v>45984</v>
+        <v>45984.99930555555</v>
       </c>
       <c r="G249" t="inlineStr">
         <is>
@@ -11248,7 +11248,7 @@
         <v>45989</v>
       </c>
       <c r="F250" s="2" t="n">
-        <v>45991</v>
+        <v>45991.99930555555</v>
       </c>
       <c r="G250" t="inlineStr">
         <is>
@@ -11288,7 +11288,7 @@
         <v>45996</v>
       </c>
       <c r="F251" s="2" t="n">
-        <v>45998</v>
+        <v>45998.99930555555</v>
       </c>
       <c r="G251" t="inlineStr">
         <is>
@@ -11328,7 +11328,7 @@
         <v>46003</v>
       </c>
       <c r="F252" s="2" t="n">
-        <v>46003</v>
+        <v>46003.99930555555</v>
       </c>
       <c r="G252" t="inlineStr">
         <is>
@@ -11368,7 +11368,7 @@
         <v>45910</v>
       </c>
       <c r="F253" s="2" t="n">
-        <v>45919</v>
+        <v>45919.99930555555</v>
       </c>
       <c r="G253" t="inlineStr">
         <is>
@@ -11408,7 +11408,7 @@
         <v>45943</v>
       </c>
       <c r="F254" s="2" t="n">
-        <v>45944</v>
+        <v>45944.99930555555</v>
       </c>
       <c r="G254" t="inlineStr">
         <is>
@@ -11448,7 +11448,7 @@
         <v>45957</v>
       </c>
       <c r="F255" s="2" t="n">
-        <v>45958</v>
+        <v>45958.99930555555</v>
       </c>
       <c r="G255" t="inlineStr">
         <is>
@@ -11488,7 +11488,7 @@
         <v>45918</v>
       </c>
       <c r="F256" s="2" t="n">
-        <v>45919</v>
+        <v>45919.99930555555</v>
       </c>
       <c r="G256" t="inlineStr">
         <is>
@@ -11528,7 +11528,7 @@
         <v>45917</v>
       </c>
       <c r="F257" s="2" t="n">
-        <v>45923</v>
+        <v>45923.99930555555</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
@@ -11568,7 +11568,7 @@
         <v>45923</v>
       </c>
       <c r="F258" s="2" t="n">
-        <v>45931</v>
+        <v>45931.99930555555</v>
       </c>
       <c r="G258" t="inlineStr">
         <is>
@@ -11608,7 +11608,7 @@
         <v>45926</v>
       </c>
       <c r="F259" s="2" t="n">
-        <v>45928</v>
+        <v>45928.99930555555</v>
       </c>
       <c r="G259" t="inlineStr">
         <is>
@@ -11648,7 +11648,7 @@
         <v>45923</v>
       </c>
       <c r="F260" s="2" t="n">
-        <v>45933</v>
+        <v>45933.99930555555</v>
       </c>
       <c r="G260" t="inlineStr">
         <is>
@@ -11688,7 +11688,7 @@
         <v>45923</v>
       </c>
       <c r="F261" s="2" t="n">
-        <v>45926</v>
+        <v>45926.99930555555</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
@@ -11728,7 +11728,7 @@
         <v>45926</v>
       </c>
       <c r="F262" s="2" t="n">
-        <v>45928</v>
+        <v>45928.99930555555</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:47:39
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J262"/>
+  <dimension ref="A1:J263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11747,6 +11747,42 @@
       </c>
       <c r="J262" t="inlineStr"/>
     </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>333</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E263" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F263" s="2" t="n">
+        <v>45953.99930555555</v>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr"/>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
+        </is>
+      </c>
+      <c r="J263" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:49:35
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J263"/>
+  <dimension ref="A1:J264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11775,13 +11775,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H263" t="inlineStr"/>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I263" t="inlineStr">
         <is>
           <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>333</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E264" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="F264" s="2" t="n">
+        <v>45995.99930555555</v>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr"/>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J264" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:50:16
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J264"/>
+  <dimension ref="A1:J265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11815,13 +11815,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H264" t="inlineStr"/>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I264" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>333</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E265" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="F265" s="2" t="n">
+        <v>46010.99930555555</v>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr"/>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J265" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:50:39
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J265"/>
+  <dimension ref="A1:J266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11855,13 +11855,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H265" t="inlineStr"/>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I265" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
       <c r="J265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>333</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E266" s="2" t="n">
+        <v>46082</v>
+      </c>
+      <c r="F266" s="2" t="n">
+        <v>46091.99930555555</v>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr"/>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J266" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-26 19:51:17
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -11822,7 +11822,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J264" t="inlineStr"/>
@@ -11862,7 +11862,7 @@
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J265" t="inlineStr"/>
@@ -11895,10 +11895,14 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H266" t="inlineStr"/>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J266" t="inlineStr"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:52:43
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J266"/>
+  <dimension ref="A1:J267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11907,6 +11907,42 @@
       </c>
       <c r="J266" t="inlineStr"/>
     </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>333</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E267" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="F267" s="2" t="n">
+        <v>45956.99930555555</v>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr"/>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>['Benjamin Covington', 'Anita Antoninka', 'Matthew Bowker']</t>
+        </is>
+      </c>
+      <c r="J267" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:53:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J267"/>
+  <dimension ref="A1:J268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11935,13 +11935,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H267" t="inlineStr"/>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I267" t="inlineStr">
         <is>
           <t>['Benjamin Covington', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>333</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E268" s="2" t="n">
+        <v>45960</v>
+      </c>
+      <c r="F268" s="2" t="n">
+        <v>45967.99930555555</v>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr"/>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>['Keven Griffen', 'Anita Antoninka', 'Matthew Bowker']</t>
+        </is>
+      </c>
+      <c r="J268" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:55:13
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J268"/>
+  <dimension ref="A1:J269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11975,13 +11975,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H268" t="inlineStr"/>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I268" t="inlineStr">
         <is>
           <t>['Keven Griffen', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>333</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E269" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F269" s="2" t="n">
+        <v>46032.99930555555</v>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr"/>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
+        </is>
+      </c>
+      <c r="J269" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:56:43
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J269"/>
+  <dimension ref="A1:J270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12015,13 +12015,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H269" t="inlineStr"/>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I269" t="inlineStr">
         <is>
           <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>333</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E270" s="2" t="n">
+        <v>46038</v>
+      </c>
+      <c r="F270" s="2" t="n">
+        <v>46040.99930555555</v>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr"/>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>['Anita Antoninka']</t>
+        </is>
+      </c>
+      <c r="J270" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:57:21
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J270"/>
+  <dimension ref="A1:J271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12055,13 +12055,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H270" t="inlineStr"/>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I270" t="inlineStr">
         <is>
           <t>['Anita Antoninka']</t>
         </is>
       </c>
       <c r="J270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>333</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E271" s="2" t="n">
+        <v>46045</v>
+      </c>
+      <c r="F271" s="2" t="n">
+        <v>46047.99930555555</v>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr"/>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>['Anita Antoninka']</t>
+        </is>
+      </c>
+      <c r="J271" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:57:53
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J271"/>
+  <dimension ref="A1:J272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12095,13 +12095,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H271" t="inlineStr"/>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I271" t="inlineStr">
         <is>
           <t>['Anita Antoninka']</t>
         </is>
       </c>
       <c r="J271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>333</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E272" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="F272" s="2" t="n">
+        <v>46076.99930555555</v>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr"/>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>['Anita Antoninka']</t>
+        </is>
+      </c>
+      <c r="J272" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-26 19:58:33
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J272"/>
+  <dimension ref="A1:J273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12135,13 +12135,53 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H272" t="inlineStr"/>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I272" t="inlineStr">
         <is>
           <t>['Anita Antoninka']</t>
         </is>
       </c>
       <c r="J272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>333</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E273" s="2" t="n">
+        <v>46107</v>
+      </c>
+      <c r="F273" s="2" t="n">
+        <v>46109.99930555555</v>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr"/>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
+        </is>
+      </c>
+      <c r="J273" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-09-26 20:03:38
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -12175,7 +12175,11 @@
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="H273" t="inlineStr"/>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I273" t="inlineStr">
         <is>
           <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-09-30 14:55:55
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J273"/>
+  <dimension ref="A1:J274"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12187,6 +12187,46 @@
       </c>
       <c r="J273" t="inlineStr"/>
     </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>321</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Nathan Saurer</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E274" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="F274" s="2" t="n">
+        <v>45936.99930555555</v>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>Motor Pool supplemental vehicle.</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>['Nathan Saurer']</t>
+        </is>
+      </c>
+      <c r="J274" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk added 11 entries (grouped weekdays) via Streamlit app at 2025-10-01 18:25:59
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J274"/>
+  <dimension ref="A1:J285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12227,6 +12227,446 @@
       </c>
       <c r="J274" t="inlineStr"/>
     </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="n">
+        <v>325</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E275" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="F275" s="2" t="n">
+        <v>45933.99930555555</v>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="n">
+        <v>325</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E276" s="2" t="n">
+        <v>45939</v>
+      </c>
+      <c r="F276" s="2" t="n">
+        <v>45940.99930555555</v>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="n">
+        <v>325</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E277" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F277" s="2" t="n">
+        <v>45947.99930555555</v>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="n">
+        <v>325</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E278" s="2" t="n">
+        <v>45953</v>
+      </c>
+      <c r="F278" s="2" t="n">
+        <v>45954.99930555555</v>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="n">
+        <v>325</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E279" s="2" t="n">
+        <v>45960</v>
+      </c>
+      <c r="F279" s="2" t="n">
+        <v>45961.99930555555</v>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="n">
+        <v>325</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E280" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="F280" s="2" t="n">
+        <v>45968.99930555555</v>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="n">
+        <v>325</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E281" s="2" t="n">
+        <v>45974</v>
+      </c>
+      <c r="F281" s="2" t="n">
+        <v>45975.99930555555</v>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="n">
+        <v>325</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E282" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="F282" s="2" t="n">
+        <v>45982.99930555555</v>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="n">
+        <v>325</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E283" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="F283" s="2" t="n">
+        <v>45989.99930555555</v>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="n">
+        <v>325</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E284" s="2" t="n">
+        <v>45995</v>
+      </c>
+      <c r="F284" s="2" t="n">
+        <v>45996.99930555555</v>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="n">
+        <v>325</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E285" s="2" t="n">
+        <v>46002</v>
+      </c>
+      <c r="F285" s="2" t="n">
+        <v>46003.99930555555</v>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>Research</t>
+        </is>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J285" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk added 4 entries (multiple date ranges) via Streamlit app at 2025-10-01 18:28:19
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J285"/>
+  <dimension ref="A1:J289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12667,6 +12667,166 @@
       </c>
       <c r="J285" t="inlineStr"/>
     </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="n">
+        <v>325</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E286" s="2" t="n">
+        <v>45936</v>
+      </c>
+      <c r="F286" s="2" t="n">
+        <v>45936.99930555555</v>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>FOR 382/382H/582</t>
+        </is>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="n">
+        <v>325</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E287" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F287" s="2" t="n">
+        <v>45946.99930555555</v>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>FOR 382/382H/582</t>
+        </is>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="n">
+        <v>325</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E288" s="2" t="n">
+        <v>45953</v>
+      </c>
+      <c r="F288" s="2" t="n">
+        <v>45953.99930555555</v>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>FOR 382/382H/582</t>
+        </is>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="n">
+        <v>325</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E289" s="2" t="n">
+        <v>45985</v>
+      </c>
+      <c r="F289" s="2" t="n">
+        <v>45985.99930555555</v>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>FOR 382/382H/582</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>Peter Fule</t>
+        </is>
+      </c>
+      <c r="J289" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-01 19:38:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J289"/>
+  <dimension ref="A1:J290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12827,6 +12827,46 @@
       </c>
       <c r="J289" t="inlineStr"/>
     </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="n">
+        <v>331</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Anita Joy Antoninka</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E290" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="F290" s="2" t="n">
+        <v>45943.99930555555</v>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>trip to and from phoenix</t>
+        </is>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>['Anita Antoninka', 'Gayle Tyree']</t>
+        </is>
+      </c>
+      <c r="J290" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-01 19:57:23
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J290"/>
+  <dimension ref="A1:J291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12867,6 +12867,46 @@
       </c>
       <c r="J290" t="inlineStr"/>
     </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="n">
+        <v>268</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Matthew Bowker</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E291" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F291" s="2" t="n">
+        <v>45953.99930555555</v>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>We will be traveling from NAU to Mountainair, New Mexico with up to 4 crew members for field work. We expect to be in the field October 16-23. We will be camping on site, so we need to transport gear and supplies as well. Any of the 4 wheel drive vehicles will work for us. We need the camper shell on the back of the truck bed.</t>
+        </is>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+        </is>
+      </c>
+      <c r="J291" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-01 19:58:51
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J291"/>
+  <dimension ref="A1:J292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12907,6 +12907,46 @@
       </c>
       <c r="J291" t="inlineStr"/>
     </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="n">
+        <v>268</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Matthew Bowker</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E292" s="2" t="n">
+        <v>45963</v>
+      </c>
+      <c r="F292" s="2" t="n">
+        <v>45971.99930555555</v>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>We will travel from NAU to Temecula, CA for field work at Santa Margarita Ecological Reserve. We plan to be in the field Nov 2-Nov 10. We will be camping on site, so we need to be able to transport up to 5 people with gear. Any of the vehicles should work if they can transport 5 people with a covered truck bed.</t>
+        </is>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+        </is>
+      </c>
+      <c r="J292" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-01 20:00:00
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J292"/>
+  <dimension ref="A1:J293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12947,6 +12947,46 @@
       </c>
       <c r="J292" t="inlineStr"/>
     </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="n">
+        <v>268</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Matthew Bowker</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E293" s="2" t="n">
+        <v>45990</v>
+      </c>
+      <c r="F293" s="2" t="n">
+        <v>45995.99930555555</v>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>We will travel from NAU to Organ Pipe National Monument for fieldwork for CrustNet. We will have up to 5 field workers and will camp on site. So, we prefer a truck with a camper shell on the top.</t>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+        </is>
+      </c>
+      <c r="J293" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-01 20:01:18
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J293"/>
+  <dimension ref="A1:J294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12987,6 +12987,46 @@
       </c>
       <c r="J293" t="inlineStr"/>
     </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="n">
+        <v>268</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Matthew Bowker</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E294" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="F294" s="2" t="n">
+        <v>46010.99930555555</v>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>We will travel from NAU to Gold Butte National Monument for field work with up to 6 workers. We will camp on site. We need a 4-wheel drive vehicle and an enclosed camper shell.</t>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>['Sierra Jech', 'Matthew Bowker', 'Seth Charley']</t>
+        </is>
+      </c>
+      <c r="J294" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-10-02 21:43:06
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -12285,7 +12285,7 @@
         </is>
       </c>
       <c r="E276" s="2" t="n">
-        <v>45939</v>
+        <v>45940</v>
       </c>
       <c r="F276" s="2" t="n">
         <v>45940.99930555555</v>
@@ -12445,7 +12445,7 @@
         </is>
       </c>
       <c r="E280" s="2" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="F280" s="2" t="n">
         <v>45968.99930555555</v>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-10-02 21:45:20
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -12285,7 +12285,7 @@
         </is>
       </c>
       <c r="E276" s="2" t="n">
-        <v>45940</v>
+        <v>45939</v>
       </c>
       <c r="F276" s="2" t="n">
         <v>45940.99930555555</v>
@@ -12325,7 +12325,7 @@
         </is>
       </c>
       <c r="E277" s="2" t="n">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="F277" s="2" t="n">
         <v>45947.99930555555</v>
@@ -12365,7 +12365,7 @@
         </is>
       </c>
       <c r="E278" s="2" t="n">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="F278" s="2" t="n">
         <v>45954.99930555555</v>
@@ -12445,7 +12445,7 @@
         </is>
       </c>
       <c r="E280" s="2" t="n">
-        <v>45968</v>
+        <v>45967</v>
       </c>
       <c r="F280" s="2" t="n">
         <v>45968.99930555555</v>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-06 17:53:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13027,6 +13027,46 @@
       </c>
       <c r="J294" t="inlineStr"/>
     </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="n">
+        <v>310</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E295" s="2" t="n">
+        <v>45936</v>
+      </c>
+      <c r="F295" s="2" t="n">
+        <v>45938.99930555555</v>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>FOR 313</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>['Elsa Kauffman', 'Bear Murillo']</t>
+        </is>
+      </c>
+      <c r="J295" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-07 17:21:29
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J295"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13067,6 +13067,46 @@
       </c>
       <c r="J295" t="inlineStr"/>
     </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="n">
+        <v>310</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E296" s="2" t="n">
+        <v>45939</v>
+      </c>
+      <c r="F296" s="2" t="n">
+        <v>45939.99930555555</v>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Field site visit (day trip), Payson AZ, 2 occupants Sorry for the late ask, but I have the opportunity to go down to our field site on Thursday with a student to help them download data and do some quick tasks. </t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>['Kelsey Bryant', 'Ariela DellaSala']</t>
+        </is>
+      </c>
+      <c r="J296" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-10-07 17:27:07
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J296"/>
+  <dimension ref="A1:J295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11436,7 +11436,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -11445,10 +11445,10 @@
         </is>
       </c>
       <c r="E255" s="2" t="n">
-        <v>45957</v>
+        <v>45918</v>
       </c>
       <c r="F255" s="2" t="n">
-        <v>45958.99930555555</v>
+        <v>45919.99930555555</v>
       </c>
       <c r="G255" t="inlineStr">
         <is>
@@ -11457,12 +11457,12 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Students will drive to sites on Ellison and Bonita Creeks on the Tonto NF outside of Payson, AZ to collect water for stable isotope and nutrient analysis as part of the Dude Fire project funded by SRP Dude. This will be a 1-day trip with 3 NAU student/tech occupants.</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>['Adair Patterson']</t>
+          <t>['Paige Whitton', 'Logan Ozmet']</t>
         </is>
       </c>
       <c r="J255" t="inlineStr"/>
@@ -11472,11 +11472,11 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>321</v>
+        <v>268</v>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>OUT OF COMMISION</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -11485,24 +11485,24 @@
         </is>
       </c>
       <c r="E256" s="2" t="n">
-        <v>45918</v>
+        <v>45917</v>
       </c>
       <c r="F256" s="2" t="n">
-        <v>45919.99930555555</v>
+        <v>45923.99930555555</v>
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Students will drive to sites on Ellison and Bonita Creeks on the Tonto NF outside of Payson, AZ to collect water for stable isotope and nutrient analysis as part of the Dude Fire project funded by SRP Dude. This will be a 1-day trip with 3 NAU student/tech occupants.</t>
+          <t>Bad Tire</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>['Paige Whitton', 'Logan Ozmet']</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="J256" t="inlineStr"/>
@@ -11512,11 +11512,11 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>OUT OF COMMISION</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -11525,24 +11525,24 @@
         </is>
       </c>
       <c r="E257" s="2" t="n">
-        <v>45917</v>
+        <v>45923</v>
       </c>
       <c r="F257" s="2" t="n">
-        <v>45923.99930555555</v>
+        <v>45931.99930555555</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Bad Tire</t>
+          <t>will be driving to Workman Creek in the Sierra Ancha Experimental Forest near Globe, AZ to do field work pertaining to my PhD dissertation which focuses on vadose zone processes, critical zone hydrology, and the effects of fire on the hydrologic cycle in headwater catchments.</t>
         </is>
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>['Emory Ellis']</t>
         </is>
       </c>
       <c r="J257" t="inlineStr"/>
@@ -11552,11 +11552,11 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -11565,24 +11565,24 @@
         </is>
       </c>
       <c r="E258" s="2" t="n">
-        <v>45923</v>
+        <v>45926</v>
       </c>
       <c r="F258" s="2" t="n">
-        <v>45931.99930555555</v>
+        <v>45928.99930555555</v>
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>will be driving to Workman Creek in the Sierra Ancha Experimental Forest near Globe, AZ to do field work pertaining to my PhD dissertation which focuses on vadose zone processes, critical zone hydrology, and the effects of fire on the hydrologic cycle in headwater catchments.</t>
+          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>['Emory Ellis']</t>
+          <t>['Jackson Bledsoe', 'Kristen Waring']</t>
         </is>
       </c>
       <c r="J258" t="inlineStr"/>
@@ -11592,11 +11592,11 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>329</v>
+        <v>467</v>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>OUT OF COMMISION</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -11605,24 +11605,24 @@
         </is>
       </c>
       <c r="E259" s="2" t="n">
-        <v>45926</v>
+        <v>45923</v>
       </c>
       <c r="F259" s="2" t="n">
-        <v>45928.99930555555</v>
+        <v>45926.99930555555</v>
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
+          <t>Plow bracket removal</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>['Jackson Bledsoe', 'Kristen Waring']</t>
+          <t>['Jacob Shelly']</t>
         </is>
       </c>
       <c r="J259" t="inlineStr"/>
@@ -11632,11 +11632,11 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>467</v>
+        <v>331</v>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>OUT OF COMMISION</t>
+          <t>Nathan Saurer</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -11652,17 +11652,17 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Plow bracket removal</t>
+          <t>Motor Pool Supplemental vehicle.</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>['Jacob Shelly']</t>
+          <t>['Nathan Saurer']</t>
         </is>
       </c>
       <c r="J260" t="inlineStr"/>
@@ -11672,11 +11672,11 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>331</v>
+        <v>268</v>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Nathan Saurer</t>
+          <t>Kristen Waring</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -11685,24 +11685,24 @@
         </is>
       </c>
       <c r="E261" s="2" t="n">
-        <v>45923</v>
+        <v>45926</v>
       </c>
       <c r="F261" s="2" t="n">
-        <v>45926.99930555555</v>
+        <v>45928.99930555555</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Motor Pool Supplemental vehicle.</t>
+          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
         </is>
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>['Nathan Saurer']</t>
+          <t>['Kristen Waring', 'Jackson Bledsoe']</t>
         </is>
       </c>
       <c r="J261" t="inlineStr"/>
@@ -11712,11 +11712,11 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>268</v>
+        <v>333</v>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Kristen Waring</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -11725,24 +11725,24 @@
         </is>
       </c>
       <c r="E262" s="2" t="n">
-        <v>45926</v>
+        <v>45946</v>
       </c>
       <c r="F262" s="2" t="n">
-        <v>45928.99930555555</v>
+        <v>45953.99930555555</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>Looking for 2 vehicles, to go to the White Mountains. 7 occupants plus camping gear.</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>['Kristen Waring', 'Jackson Bledsoe']</t>
+          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J262" t="inlineStr"/>
@@ -11765,10 +11765,10 @@
         </is>
       </c>
       <c r="E263" s="2" t="n">
-        <v>45946</v>
+        <v>45982</v>
       </c>
       <c r="F263" s="2" t="n">
-        <v>45953.99930555555</v>
+        <v>45995.99930555555</v>
       </c>
       <c r="G263" t="inlineStr">
         <is>
@@ -11805,10 +11805,10 @@
         </is>
       </c>
       <c r="E264" s="2" t="n">
-        <v>45982</v>
+        <v>46003</v>
       </c>
       <c r="F264" s="2" t="n">
-        <v>45995.99930555555</v>
+        <v>46010.99930555555</v>
       </c>
       <c r="G264" t="inlineStr">
         <is>
@@ -11845,10 +11845,10 @@
         </is>
       </c>
       <c r="E265" s="2" t="n">
-        <v>46003</v>
+        <v>46082</v>
       </c>
       <c r="F265" s="2" t="n">
-        <v>46010.99930555555</v>
+        <v>46091.99930555555</v>
       </c>
       <c r="G265" t="inlineStr">
         <is>
@@ -11885,10 +11885,10 @@
         </is>
       </c>
       <c r="E266" s="2" t="n">
-        <v>46082</v>
+        <v>45954</v>
       </c>
       <c r="F266" s="2" t="n">
-        <v>46091.99930555555</v>
+        <v>45956.99930555555</v>
       </c>
       <c r="G266" t="inlineStr">
         <is>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>['Matthew Bowker', 'Anita Antoninka', 'Sierra Jech', 'Gayle Tyree']</t>
+          <t>['Benjamin Covington', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J266" t="inlineStr"/>
@@ -11925,10 +11925,10 @@
         </is>
       </c>
       <c r="E267" s="2" t="n">
-        <v>45954</v>
+        <v>45960</v>
       </c>
       <c r="F267" s="2" t="n">
-        <v>45956.99930555555</v>
+        <v>45967.99930555555</v>
       </c>
       <c r="G267" t="inlineStr">
         <is>
@@ -11942,7 +11942,7 @@
       </c>
       <c r="I267" t="inlineStr">
         <is>
-          <t>['Benjamin Covington', 'Anita Antoninka', 'Matthew Bowker']</t>
+          <t>['Keven Griffen', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J267" t="inlineStr"/>
@@ -11965,10 +11965,10 @@
         </is>
       </c>
       <c r="E268" s="2" t="n">
-        <v>45960</v>
+        <v>46025</v>
       </c>
       <c r="F268" s="2" t="n">
-        <v>45967.99930555555</v>
+        <v>46032.99930555555</v>
       </c>
       <c r="G268" t="inlineStr">
         <is>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="I268" t="inlineStr">
         <is>
-          <t>['Keven Griffen', 'Anita Antoninka', 'Matthew Bowker']</t>
+          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J268" t="inlineStr"/>
@@ -12005,10 +12005,10 @@
         </is>
       </c>
       <c r="E269" s="2" t="n">
-        <v>46025</v>
+        <v>46038</v>
       </c>
       <c r="F269" s="2" t="n">
-        <v>46032.99930555555</v>
+        <v>46040.99930555555</v>
       </c>
       <c r="G269" t="inlineStr">
         <is>
@@ -12022,7 +12022,7 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
+          <t>['Anita Antoninka']</t>
         </is>
       </c>
       <c r="J269" t="inlineStr"/>
@@ -12045,10 +12045,10 @@
         </is>
       </c>
       <c r="E270" s="2" t="n">
-        <v>46038</v>
+        <v>46045</v>
       </c>
       <c r="F270" s="2" t="n">
-        <v>46040.99930555555</v>
+        <v>46047.99930555555</v>
       </c>
       <c r="G270" t="inlineStr">
         <is>
@@ -12085,10 +12085,10 @@
         </is>
       </c>
       <c r="E271" s="2" t="n">
-        <v>46045</v>
+        <v>46065</v>
       </c>
       <c r="F271" s="2" t="n">
-        <v>46047.99930555555</v>
+        <v>46076.99930555555</v>
       </c>
       <c r="G271" t="inlineStr">
         <is>
@@ -12125,10 +12125,10 @@
         </is>
       </c>
       <c r="E272" s="2" t="n">
-        <v>46065</v>
+        <v>46107</v>
       </c>
       <c r="F272" s="2" t="n">
-        <v>46076.99930555555</v>
+        <v>46109.99930555555</v>
       </c>
       <c r="G272" t="inlineStr">
         <is>
@@ -12142,7 +12142,7 @@
       </c>
       <c r="I272" t="inlineStr">
         <is>
-          <t>['Anita Antoninka']</t>
+          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
         </is>
       </c>
       <c r="J272" t="inlineStr"/>
@@ -12152,11 +12152,11 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Nathan Saurer</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -12165,24 +12165,24 @@
         </is>
       </c>
       <c r="E273" s="2" t="n">
-        <v>46107</v>
+        <v>45932</v>
       </c>
       <c r="F273" s="2" t="n">
-        <v>46109.99930555555</v>
+        <v>45936.99930555555</v>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Motor Pool supplemental vehicle.</t>
         </is>
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>['Kara Gibson', 'Anita Antoninka', 'Matthew Bowker']</t>
+          <t>['Nathan Saurer']</t>
         </is>
       </c>
       <c r="J273" t="inlineStr"/>
@@ -12192,11 +12192,11 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Nathan Saurer</t>
+          <t>Pete Fule</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -12208,21 +12208,21 @@
         <v>45932</v>
       </c>
       <c r="F274" s="2" t="n">
-        <v>45936.99930555555</v>
+        <v>45933.99930555555</v>
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>Motor Pool supplemental vehicle.</t>
+          <t>Research</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>['Nathan Saurer']</t>
+          <t>Peter Fule</t>
         </is>
       </c>
       <c r="J274" t="inlineStr"/>
@@ -12245,10 +12245,10 @@
         </is>
       </c>
       <c r="E275" s="2" t="n">
-        <v>45932</v>
+        <v>45939</v>
       </c>
       <c r="F275" s="2" t="n">
-        <v>45933.99930555555</v>
+        <v>45940.99930555555</v>
       </c>
       <c r="G275" t="inlineStr">
         <is>
@@ -12285,10 +12285,10 @@
         </is>
       </c>
       <c r="E276" s="2" t="n">
-        <v>45939</v>
+        <v>45947</v>
       </c>
       <c r="F276" s="2" t="n">
-        <v>45940.99930555555</v>
+        <v>45947.99930555555</v>
       </c>
       <c r="G276" t="inlineStr">
         <is>
@@ -12325,10 +12325,10 @@
         </is>
       </c>
       <c r="E277" s="2" t="n">
-        <v>45947</v>
+        <v>45954</v>
       </c>
       <c r="F277" s="2" t="n">
-        <v>45947.99930555555</v>
+        <v>45954.99930555555</v>
       </c>
       <c r="G277" t="inlineStr">
         <is>
@@ -12365,10 +12365,10 @@
         </is>
       </c>
       <c r="E278" s="2" t="n">
-        <v>45954</v>
+        <v>45960</v>
       </c>
       <c r="F278" s="2" t="n">
-        <v>45954.99930555555</v>
+        <v>45961.99930555555</v>
       </c>
       <c r="G278" t="inlineStr">
         <is>
@@ -12405,10 +12405,10 @@
         </is>
       </c>
       <c r="E279" s="2" t="n">
-        <v>45960</v>
+        <v>45967</v>
       </c>
       <c r="F279" s="2" t="n">
-        <v>45961.99930555555</v>
+        <v>45968.99930555555</v>
       </c>
       <c r="G279" t="inlineStr">
         <is>
@@ -12445,10 +12445,10 @@
         </is>
       </c>
       <c r="E280" s="2" t="n">
-        <v>45967</v>
+        <v>45974</v>
       </c>
       <c r="F280" s="2" t="n">
-        <v>45968.99930555555</v>
+        <v>45975.99930555555</v>
       </c>
       <c r="G280" t="inlineStr">
         <is>
@@ -12485,10 +12485,10 @@
         </is>
       </c>
       <c r="E281" s="2" t="n">
-        <v>45974</v>
+        <v>45981</v>
       </c>
       <c r="F281" s="2" t="n">
-        <v>45975.99930555555</v>
+        <v>45982.99930555555</v>
       </c>
       <c r="G281" t="inlineStr">
         <is>
@@ -12525,10 +12525,10 @@
         </is>
       </c>
       <c r="E282" s="2" t="n">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="F282" s="2" t="n">
-        <v>45982.99930555555</v>
+        <v>45989.99930555555</v>
       </c>
       <c r="G282" t="inlineStr">
         <is>
@@ -12565,10 +12565,10 @@
         </is>
       </c>
       <c r="E283" s="2" t="n">
-        <v>45988</v>
+        <v>45995</v>
       </c>
       <c r="F283" s="2" t="n">
-        <v>45989.99930555555</v>
+        <v>45996.99930555555</v>
       </c>
       <c r="G283" t="inlineStr">
         <is>
@@ -12605,10 +12605,10 @@
         </is>
       </c>
       <c r="E284" s="2" t="n">
-        <v>45995</v>
+        <v>46002</v>
       </c>
       <c r="F284" s="2" t="n">
-        <v>45996.99930555555</v>
+        <v>46003.99930555555</v>
       </c>
       <c r="G284" t="inlineStr">
         <is>
@@ -12645,10 +12645,10 @@
         </is>
       </c>
       <c r="E285" s="2" t="n">
-        <v>46002</v>
+        <v>45936</v>
       </c>
       <c r="F285" s="2" t="n">
-        <v>46003.99930555555</v>
+        <v>45936.99930555555</v>
       </c>
       <c r="G285" t="inlineStr">
         <is>
@@ -12657,7 +12657,7 @@
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>Research</t>
+          <t>FOR 382/382H/582</t>
         </is>
       </c>
       <c r="I285" t="inlineStr">
@@ -12685,10 +12685,10 @@
         </is>
       </c>
       <c r="E286" s="2" t="n">
-        <v>45936</v>
+        <v>45946</v>
       </c>
       <c r="F286" s="2" t="n">
-        <v>45936.99930555555</v>
+        <v>45946.99930555555</v>
       </c>
       <c r="G286" t="inlineStr">
         <is>
@@ -12725,10 +12725,10 @@
         </is>
       </c>
       <c r="E287" s="2" t="n">
-        <v>45946</v>
+        <v>45953</v>
       </c>
       <c r="F287" s="2" t="n">
-        <v>45946.99930555555</v>
+        <v>45953.99930555555</v>
       </c>
       <c r="G287" t="inlineStr">
         <is>
@@ -12765,10 +12765,10 @@
         </is>
       </c>
       <c r="E288" s="2" t="n">
-        <v>45953</v>
+        <v>45985</v>
       </c>
       <c r="F288" s="2" t="n">
-        <v>45953.99930555555</v>
+        <v>45985.99930555555</v>
       </c>
       <c r="G288" t="inlineStr">
         <is>
@@ -12792,11 +12792,11 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>Pete Fule</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
@@ -12805,24 +12805,24 @@
         </is>
       </c>
       <c r="E289" s="2" t="n">
-        <v>45985</v>
+        <v>45938</v>
       </c>
       <c r="F289" s="2" t="n">
-        <v>45985.99930555555</v>
+        <v>45943.99930555555</v>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>325 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
         <is>
-          <t>FOR 382/382H/582</t>
+          <t>trip to and from phoenix</t>
         </is>
       </c>
       <c r="I289" t="inlineStr">
         <is>
-          <t>Peter Fule</t>
+          <t>['Anita Antoninka', 'Gayle Tyree']</t>
         </is>
       </c>
       <c r="J289" t="inlineStr"/>
@@ -12832,11 +12832,11 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>331</v>
+        <v>268</v>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Matthew Bowker</t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
@@ -12845,24 +12845,24 @@
         </is>
       </c>
       <c r="E290" s="2" t="n">
-        <v>45938</v>
+        <v>45946</v>
       </c>
       <c r="F290" s="2" t="n">
-        <v>45943.99930555555</v>
+        <v>45953.99930555555</v>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>trip to and from phoenix</t>
+          <t>We will be traveling from NAU to Mountainair, New Mexico with up to 4 crew members for field work. We expect to be in the field October 16-23. We will be camping on site, so we need to transport gear and supplies as well. Any of the 4 wheel drive vehicles will work for us. We need the camper shell on the back of the truck bed.</t>
         </is>
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>['Anita Antoninka', 'Gayle Tyree']</t>
+          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J290" t="inlineStr"/>
@@ -12885,10 +12885,10 @@
         </is>
       </c>
       <c r="E291" s="2" t="n">
-        <v>45946</v>
+        <v>45963</v>
       </c>
       <c r="F291" s="2" t="n">
-        <v>45953.99930555555</v>
+        <v>45971.99930555555</v>
       </c>
       <c r="G291" t="inlineStr">
         <is>
@@ -12897,7 +12897,7 @@
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>We will be traveling from NAU to Mountainair, New Mexico with up to 4 crew members for field work. We expect to be in the field October 16-23. We will be camping on site, so we need to transport gear and supplies as well. Any of the 4 wheel drive vehicles will work for us. We need the camper shell on the back of the truck bed.</t>
+          <t>We will travel from NAU to Temecula, CA for field work at Santa Margarita Ecological Reserve. We plan to be in the field Nov 2-Nov 10. We will be camping on site, so we need to be able to transport up to 5 people with gear. Any of the vehicles should work if they can transport 5 people with a covered truck bed.</t>
         </is>
       </c>
       <c r="I291" t="inlineStr">
@@ -12925,10 +12925,10 @@
         </is>
       </c>
       <c r="E292" s="2" t="n">
-        <v>45963</v>
+        <v>45990</v>
       </c>
       <c r="F292" s="2" t="n">
-        <v>45971.99930555555</v>
+        <v>45995.99930555555</v>
       </c>
       <c r="G292" t="inlineStr">
         <is>
@@ -12937,7 +12937,7 @@
       </c>
       <c r="H292" t="inlineStr">
         <is>
-          <t>We will travel from NAU to Temecula, CA for field work at Santa Margarita Ecological Reserve. We plan to be in the field Nov 2-Nov 10. We will be camping on site, so we need to be able to transport up to 5 people with gear. Any of the vehicles should work if they can transport 5 people with a covered truck bed.</t>
+          <t>We will travel from NAU to Organ Pipe National Monument for fieldwork for CrustNet. We will have up to 5 field workers and will camp on site. So, we prefer a truck with a camper shell on the top.</t>
         </is>
       </c>
       <c r="I292" t="inlineStr">
@@ -12965,10 +12965,10 @@
         </is>
       </c>
       <c r="E293" s="2" t="n">
-        <v>45990</v>
+        <v>46003</v>
       </c>
       <c r="F293" s="2" t="n">
-        <v>45995.99930555555</v>
+        <v>46010.99930555555</v>
       </c>
       <c r="G293" t="inlineStr">
         <is>
@@ -12977,12 +12977,12 @@
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>We will travel from NAU to Organ Pipe National Monument for fieldwork for CrustNet. We will have up to 5 field workers and will camp on site. So, we prefer a truck with a camper shell on the top.</t>
+          <t>We will travel from NAU to Gold Butte National Monument for field work with up to 6 workers. We will camp on site. We need a 4-wheel drive vehicle and an enclosed camper shell.</t>
         </is>
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+          <t>['Sierra Jech', 'Matthew Bowker', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J293" t="inlineStr"/>
@@ -12992,11 +12992,11 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>Matthew Bowker</t>
+          <t>Kelsey Bryant</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
@@ -13005,24 +13005,24 @@
         </is>
       </c>
       <c r="E294" s="2" t="n">
-        <v>46003</v>
+        <v>45936</v>
       </c>
       <c r="F294" s="2" t="n">
-        <v>46010.99930555555</v>
+        <v>45938.99930555555</v>
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
         <is>
-          <t>We will travel from NAU to Gold Butte National Monument for field work with up to 6 workers. We will camp on site. We need a 4-wheel drive vehicle and an enclosed camper shell.</t>
+          <t>FOR 313</t>
         </is>
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>['Sierra Jech', 'Matthew Bowker', 'Seth Charley']</t>
+          <t>['Elsa Kauffman', 'Bear Murillo']</t>
         </is>
       </c>
       <c r="J294" t="inlineStr"/>
@@ -13045,10 +13045,10 @@
         </is>
       </c>
       <c r="E295" s="2" t="n">
-        <v>45936</v>
+        <v>45939</v>
       </c>
       <c r="F295" s="2" t="n">
-        <v>45938.99930555555</v>
+        <v>45939.99930555555</v>
       </c>
       <c r="G295" t="inlineStr">
         <is>
@@ -13057,55 +13057,15 @@
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>FOR 313</t>
+          <t xml:space="preserve">Field site visit (day trip), Payson AZ, 2 occupants Sorry for the late ask, but I have the opportunity to go down to our field site on Thursday with a student to help them download data and do some quick tasks. </t>
         </is>
       </c>
       <c r="I295" t="inlineStr">
         <is>
-          <t>['Elsa Kauffman', 'Bear Murillo']</t>
+          <t>['Kelsey Bryant', 'Ariela DellaSala']</t>
         </is>
       </c>
       <c r="J295" t="inlineStr"/>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
-        <v>294</v>
-      </c>
-      <c r="B296" t="n">
-        <v>310</v>
-      </c>
-      <c r="C296" t="inlineStr">
-        <is>
-          <t>Kelsey Bryant</t>
-        </is>
-      </c>
-      <c r="D296" t="inlineStr">
-        <is>
-          <t>Confirmed</t>
-        </is>
-      </c>
-      <c r="E296" s="2" t="n">
-        <v>45939</v>
-      </c>
-      <c r="F296" s="2" t="n">
-        <v>45939.99930555555</v>
-      </c>
-      <c r="G296" t="inlineStr">
-        <is>
-          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
-        </is>
-      </c>
-      <c r="H296" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Field site visit (day trip), Payson AZ, 2 occupants Sorry for the late ask, but I have the opportunity to go down to our field site on Thursday with a student to help them download data and do some quick tasks. </t>
-        </is>
-      </c>
-      <c r="I296" t="inlineStr">
-        <is>
-          <t>['Kelsey Bryant', 'Ariela DellaSala']</t>
-        </is>
-      </c>
-      <c r="J296" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-08 22:38:05
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J295"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13067,6 +13067,46 @@
       </c>
       <c r="J295" t="inlineStr"/>
     </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="n">
+        <v>321</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E296" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F296" s="2" t="n">
+        <v>45946.99930555555</v>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>321 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>2 trucks needed to transport advisory council and faculty to Camp Navajo. Total occupants ~8 across both.</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>['Kristen Waring', 'Jill Beckmann']</t>
+        </is>
+      </c>
+      <c r="J296" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-08 22:39:01
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J296"/>
+  <dimension ref="A1:J297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13107,6 +13107,46 @@
       </c>
       <c r="J296" t="inlineStr"/>
     </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="n">
+        <v>310</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Kristen Waring</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E297" s="2" t="n">
+        <v>45946</v>
+      </c>
+      <c r="F297" s="2" t="n">
+        <v>45946.99930555555</v>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>2 trucks needed to transport advisory council and faculty to Camp Navajo. Total occupants ~8 across both.</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>['Kristen Waring', 'Jill Beckmann', 'Dave Auty']</t>
+        </is>
+      </c>
+      <c r="J297" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-08 22:44:03
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J297"/>
+  <dimension ref="A1:J298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13147,6 +13147,46 @@
       </c>
       <c r="J297" t="inlineStr"/>
     </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="n">
+        <v>330</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Pete Fule</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E298" s="2" t="n">
+        <v>45940</v>
+      </c>
+      <c r="F298" s="2" t="n">
+        <v>45943.99930555555</v>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>330 - 2024 Toyota Camry Hybrid, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>Two people travel to Phoenix for research reporting meeting.</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J298" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-10-10 15:32:34
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -10552,7 +10552,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
@@ -10572,7 +10572,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>329 - 2024 Chevy Trail Boss, White (5 seats)</t>
+          <t>332 - 2009 Dodge Dakota, White (5 Seats)</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-13 15:46:12
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J298"/>
+  <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13187,6 +13187,46 @@
       </c>
       <c r="J298" t="inlineStr"/>
     </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="n">
+        <v>331</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Nathan Saurer</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E299" s="2" t="n">
+        <v>45947</v>
+      </c>
+      <c r="F299" s="2" t="n">
+        <v>45954.99930555555</v>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>Supplemental vehicle for motor pool.</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J299" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk added 2 entries (grouped weekdays) via Streamlit app at 2025-10-13 16:22:42
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J299"/>
+  <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13227,6 +13227,86 @@
       </c>
       <c r="J299" t="inlineStr"/>
     </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="n">
+        <v>310</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E300" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F300" s="2" t="n">
+        <v>45943.99930555555</v>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="n">
+        <v>310</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E301" s="2" t="n">
+        <v>45945</v>
+      </c>
+      <c r="F301" s="2" t="n">
+        <v>45945.99930555555</v>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J301" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk added 9 entries (multiple date ranges) via Streamlit app at 2025-10-13 16:25:34
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J301"/>
+  <dimension ref="A1:J310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13307,6 +13307,366 @@
       </c>
       <c r="J301" t="inlineStr"/>
     </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="n">
+        <v>310</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E302" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F302" s="2" t="n">
+        <v>45943.99930555555</v>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="n">
+        <v>310</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E303" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="F303" s="2" t="n">
+        <v>45944.99930555555</v>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="n">
+        <v>310</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E304" s="2" t="n">
+        <v>45945</v>
+      </c>
+      <c r="F304" s="2" t="n">
+        <v>45945.99930555555</v>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="n">
+        <v>310</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E305" s="2" t="n">
+        <v>45957</v>
+      </c>
+      <c r="F305" s="2" t="n">
+        <v>45957.99930555555</v>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="n">
+        <v>310</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E306" s="2" t="n">
+        <v>45958</v>
+      </c>
+      <c r="F306" s="2" t="n">
+        <v>45958.99930555555</v>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="n">
+        <v>310</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E307" s="2" t="n">
+        <v>45959</v>
+      </c>
+      <c r="F307" s="2" t="n">
+        <v>45959.99930555555</v>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="n">
+        <v>310</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E308" s="2" t="n">
+        <v>45971</v>
+      </c>
+      <c r="F308" s="2" t="n">
+        <v>45971.99930555555</v>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="n">
+        <v>310</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E309" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="F309" s="2" t="n">
+        <v>45972.99930555555</v>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="n">
+        <v>310</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E310" s="2" t="n">
+        <v>45973</v>
+      </c>
+      <c r="F310" s="2" t="n">
+        <v>45973.99930555555</v>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>310 - 2024 Chevy Trail Boss, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>Lab for FOR 313 - around town; 2 occupans</t>
+        </is>
+      </c>
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>Kelsey Bryant, Christina Trimingham</t>
+        </is>
+      </c>
+      <c r="J310" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-13 16:29:43
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J310"/>
+  <dimension ref="A1:J311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13667,6 +13667,46 @@
       </c>
       <c r="J310" t="inlineStr"/>
     </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="n">
+        <v>330</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Nathan Saurer</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E311" s="2" t="n">
+        <v>45950</v>
+      </c>
+      <c r="F311" s="2" t="n">
+        <v>45957.99930555555</v>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>330 - 2024 Toyota Camry Hybrid, White (5 seats)</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>Motor Pool supplemental sedan for heavy travel week.</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J311" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-13 16:35:24
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J311"/>
+  <dimension ref="A1:J312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13707,6 +13707,46 @@
       </c>
       <c r="J311" t="inlineStr"/>
     </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="n">
+        <v>331</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Matthew Bowker</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E312" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F312" s="2" t="n">
+        <v>45943.99930555555</v>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>331 - 2024 Toyota Sienna Hybrid, White (8 seats)</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>Meeting. SRP, Tempe. 2 occupants.</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>['Matthew Bowker', 'Keven Griffen']</t>
+        </is>
+      </c>
+      <c r="J312" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new entry via Streamlit app at 2025-10-13 17:15:42
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J312"/>
+  <dimension ref="A1:J313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13747,6 +13747,46 @@
       </c>
       <c r="J312" t="inlineStr"/>
     </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="n">
+        <v>467</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E313" s="2" t="n">
+        <v>45943</v>
+      </c>
+      <c r="F313" s="2" t="n">
+        <v>45950.99930555555</v>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>['Richard Hofstetter', 'Julia Totty']</t>
+        </is>
+      </c>
+      <c r="J313" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk added 7 entries (grouped weekdays) via Streamlit app at 2025-10-13 17:16:58
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J313"/>
+  <dimension ref="A1:J320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13787,6 +13787,286 @@
       </c>
       <c r="J313" t="inlineStr"/>
     </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="n">
+        <v>467</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E314" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="F314" s="2" t="n">
+        <v>45956.99930555555</v>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="n">
+        <v>467</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E315" s="2" t="n">
+        <v>45961</v>
+      </c>
+      <c r="F315" s="2" t="n">
+        <v>45963.99930555555</v>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="n">
+        <v>467</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E316" s="2" t="n">
+        <v>45968</v>
+      </c>
+      <c r="F316" s="2" t="n">
+        <v>45970.99930555555</v>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="n">
+        <v>467</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E317" s="2" t="n">
+        <v>45975</v>
+      </c>
+      <c r="F317" s="2" t="n">
+        <v>45977.99930555555</v>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="n">
+        <v>467</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E318" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="F318" s="2" t="n">
+        <v>45984.99930555555</v>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="n">
+        <v>467</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E319" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="F319" s="2" t="n">
+        <v>45991.99930555555</v>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="n">
+        <v>467</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="E320" s="2" t="n">
+        <v>45996</v>
+      </c>
+      <c r="F320" s="2" t="n">
+        <v>45998.99930555555</v>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>Forest service roads to S. Kaibab, Coco, and Mogollon rim. 2-3 occupants. Parking at aspen exclosures.</t>
+        </is>
+      </c>
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>Richard Hofstetter, Julia Totty</t>
+        </is>
+      </c>
+      <c r="J320" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update from Streamlit app by user at 2025-10-13 20:29:17
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -12862,7 +12862,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+          <t>['Matthew Bowker', 'Sierra Gugel', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J290" t="inlineStr"/>
@@ -12902,7 +12902,7 @@
       </c>
       <c r="I291" t="inlineStr">
         <is>
-          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+          <t>['Matthew Bowker', 'Sierra Gugel', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J291" t="inlineStr"/>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="I292" t="inlineStr">
         <is>
-          <t>['Matthew Bowker', 'Sierra Jech', 'Seth Charley']</t>
+          <t>['Matthew Bowker', 'Sierra Gugel', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J292" t="inlineStr"/>
@@ -12982,7 +12982,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>['Sierra Jech', 'Matthew Bowker', 'Seth Charley']</t>
+          <t>['Sierra Gugel', 'Matthew Bowker', 'Seth Charley']</t>
         </is>
       </c>
       <c r="J293" t="inlineStr"/>

</xml_diff>